<commit_message>
Issue #4 Image Browser should show directory
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1070" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="2140" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>#</t>
   </si>
@@ -106,6 +106,9 @@
   </si>
   <si>
     <t>Remove REST v1/images</t>
+  </si>
+  <si>
+    <t>DONE</t>
   </si>
 </sst>
 </file>
@@ -579,7 +582,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -654,6 +657,9 @@
       <c r="A5" s="3">
         <v>4</v>
       </c>
+      <c r="B5" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="E5" s="3" t="s">
         <v>21</v>
       </c>
@@ -661,9 +667,12 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>26</v>

</xml_diff>

<commit_message>
Issue #6 Tidy image browser buttons
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>#</t>
   </si>
@@ -109,6 +109,12 @@
   </si>
   <si>
     <t>DONE</t>
+  </si>
+  <si>
+    <t>Make buttons on image browser not full width … like the ones on the home page</t>
+  </si>
+  <si>
+    <t>Tidy image browser buttons</t>
   </si>
 </sst>
 </file>
@@ -579,16 +585,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="8.7265625" style="3"/>
-    <col min="4" max="4" width="14" style="3" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" style="3" customWidth="1"/>
     <col min="5" max="5" width="15.6328125" style="3" customWidth="1"/>
     <col min="6" max="6" width="50.6328125" style="3" customWidth="1"/>
     <col min="7" max="16384" width="8.7265625" style="3"/>
@@ -681,6 +687,23 @@
         <v>26</v>
       </c>
     </row>
+    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="3">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Issue #7 Make browse playlist mode visible
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
   <si>
     <t>#</t>
   </si>
@@ -115,6 +115,9 @@
   </si>
   <si>
     <t>Tidy image browser buttons</t>
+  </si>
+  <si>
+    <t>Make browse playlist mode visibel</t>
   </si>
 </sst>
 </file>
@@ -585,10 +588,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -704,6 +707,20 @@
         <v>28</v>
       </c>
     </row>
+    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="3">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Issue #9 Cant save newly created playlist
Tidied up some other issues in here
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>#</t>
   </si>
@@ -117,7 +117,25 @@
     <t>Tidy image browser buttons</t>
   </si>
   <si>
-    <t>Make browse playlist mode visibel</t>
+    <t>Make browse playlist mode visible</t>
+  </si>
+  <si>
+    <t>Add playlist</t>
+  </si>
+  <si>
+    <t>make heading h4 and buttons same as on home</t>
+  </si>
+  <si>
+    <t>BUG</t>
+  </si>
+  <si>
+    <t>UI</t>
+  </si>
+  <si>
+    <t>Arch</t>
+  </si>
+  <si>
+    <t>Cant save newly created playlist</t>
   </si>
 </sst>
 </file>
@@ -588,10 +606,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -669,6 +687,9 @@
       <c r="B5" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="C5" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="E5" s="3" t="s">
         <v>21</v>
       </c>
@@ -676,12 +697,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>27</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>26</v>
@@ -697,6 +721,9 @@
       <c r="B7" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="C7" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="D7" s="3" t="s">
         <v>29</v>
       </c>
@@ -714,11 +741,45 @@
       <c r="B8" s="3" t="s">
         <v>27</v>
       </c>
+      <c r="C8" s="3" t="s">
+        <v>34</v>
+      </c>
       <c r="D8" s="3" t="s">
         <v>30</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="3">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #10 Play Playlist tidy
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
   <si>
     <t>#</t>
   </si>
@@ -136,6 +136,12 @@
   </si>
   <si>
     <t>Cant save newly created playlist</t>
+  </si>
+  <si>
+    <t>H4 and button layout on play playlist screen</t>
+  </si>
+  <si>
+    <t>Play Playlist tidy</t>
   </si>
 </sst>
 </file>
@@ -606,10 +612,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -775,11 +781,34 @@
       <c r="A10" s="3">
         <v>9</v>
       </c>
+      <c r="B10" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="C10" s="3" t="s">
         <v>33</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="3">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #11 Exception on directory images
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
   <si>
     <t>#</t>
   </si>
@@ -142,6 +142,18 @@
   </si>
   <si>
     <t>Play Playlist tidy</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Exception on playing images in directories</t>
+  </si>
+  <si>
+    <t>Exception on directory images</t>
+  </si>
+  <si>
+    <t>Better navigation from edit to play</t>
   </si>
 </sst>
 </file>
@@ -612,10 +624,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -811,6 +823,37 @@
         <v>37</v>
       </c>
     </row>
+    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="3">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="3">
+        <v>12</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Issue #12 Better navigation from edit to play
Also fixed the play/edit label on Playlist
Thanks to jagcolombat commented on Dec 7, 2017 in https://github.com/angular/angular/issues/13831
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
   <si>
     <t>#</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Track Disable</t>
   </si>
   <si>
-    <t>Need to have a play speed on the playlist so that I can vary the movement rate.</t>
-  </si>
-  <si>
     <t>Playlist Settings</t>
   </si>
   <si>
@@ -81,9 +78,6 @@
     <t>There will be general settings such as the number of LEDs on the device</t>
   </si>
   <si>
-    <t>Would be good to have an overall brightness</t>
-  </si>
-  <si>
     <t>NO READY</t>
   </si>
   <si>
@@ -154,6 +148,33 @@
   </si>
   <si>
     <t>Better navigation from edit to play</t>
+  </si>
+  <si>
+    <t>Need to have a play speed on the playlist so that I can vary the movement rate. Hamburger Menu</t>
+  </si>
+  <si>
+    <t>Would be good to have an overall brightness Hamburger Menu</t>
+  </si>
+  <si>
+    <t>Enabple playlist folders</t>
+  </si>
+  <si>
+    <t>Better Top Navigation … title and hamburger</t>
+  </si>
+  <si>
+    <t>Remove dirname from browse images path in app.module.ts</t>
+  </si>
+  <si>
+    <t>tech</t>
+  </si>
+  <si>
+    <t>remove dirname from path</t>
+  </si>
+  <si>
+    <t>In play mode want to be able to disable tracks</t>
+  </si>
+  <si>
+    <t>diasble tracks in play mode</t>
   </si>
 </sst>
 </file>
@@ -540,7 +561,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -586,34 +607,34 @@
     </row>
     <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -624,10 +645,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="E23" sqref="E22:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -675,27 +696,27 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -703,16 +724,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -720,16 +741,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -737,19 +758,19 @@
         <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -757,16 +778,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.35">
@@ -774,19 +795,19 @@
         <v>8</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.35">
@@ -794,13 +815,13 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.35">
@@ -808,19 +829,19 @@
         <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
@@ -828,30 +849,77 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="F12" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="C13" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="3">
+        <v>13</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="3">
+        <v>14</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #15 remove dirname from path
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
   <si>
     <t>#</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>diasble tracks in play mode</t>
+  </si>
+  <si>
+    <t>add return option to nav</t>
   </si>
 </sst>
 </file>
@@ -645,10 +648,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E22:E23"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -901,6 +904,9 @@
       <c r="A16" s="3">
         <v>15</v>
       </c>
+      <c r="B16" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="C16" s="3" t="s">
         <v>46</v>
       </c>
@@ -920,6 +926,14 @@
       </c>
       <c r="F17" s="3" t="s">
         <v>48</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="3">
+        <v>17</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #18 add  header component
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
   <si>
     <t>#</t>
   </si>
@@ -178,6 +178,21 @@
   </si>
   <si>
     <t>add return option to nav</t>
+  </si>
+  <si>
+    <t>Requires</t>
+  </si>
+  <si>
+    <t>need header component</t>
+  </si>
+  <si>
+    <t>Break header into own component so can drive behaviour</t>
+  </si>
+  <si>
+    <t>select/unselect all</t>
+  </si>
+  <si>
+    <t>on browse for images need to put the select all and un select all as buttons on the directory bar to save two buttons on the list at the bottom.</t>
   </si>
 </sst>
 </file>
@@ -648,22 +663,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="3" width="8.7265625" style="3"/>
     <col min="4" max="4" width="22.81640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="15.6328125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="50.6328125" style="3" customWidth="1"/>
-    <col min="7" max="16384" width="8.7265625" style="3"/>
+    <col min="5" max="5" width="10" style="3" customWidth="1"/>
+    <col min="6" max="6" width="15.6328125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="50.6328125" style="3" customWidth="1"/>
+    <col min="8" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -677,52 +693,55 @@
         <v>1</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="F3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -732,14 +751,14 @@
       <c r="C5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -752,11 +771,11 @@
       <c r="D6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -769,14 +788,14 @@
       <c r="D7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -789,11 +808,11 @@
       <c r="D8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -806,14 +825,14 @@
       <c r="D9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -823,11 +842,11 @@
       <c r="C10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -840,14 +859,14 @@
       <c r="D11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -860,11 +879,11 @@
       <c r="D12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -877,30 +896,30 @@
       <c r="D13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="F15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -913,27 +932,55 @@
       <c r="D16" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>50</v>
+      </c>
+      <c r="E18" s="3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19" s="3">
+        <v>18</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="G19" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A20" s="3">
+        <v>19</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #18 Navigate from playlist to playlists
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,12 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2140" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="3210" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$H$20</definedName>
+  </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
   <si>
     <t>#</t>
   </si>
@@ -171,9 +174,6 @@
     <t>remove dirname from path</t>
   </si>
   <si>
-    <t>In play mode want to be able to disable tracks</t>
-  </si>
-  <si>
     <t>diasble tracks in play mode</t>
   </si>
   <si>
@@ -193,6 +193,12 @@
   </si>
   <si>
     <t>on browse for images need to put the select all and un select all as buttons on the directory bar to save two buttons on the list at the bottom.</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>In play mode want to be able to disable tracks Duplicate of 1</t>
   </si>
 </sst>
 </file>
@@ -663,327 +669,366 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G20"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="3" width="8.7265625" style="3"/>
-    <col min="4" max="4" width="22.81640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10" style="3" customWidth="1"/>
-    <col min="6" max="6" width="15.6328125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="50.6328125" style="3" customWidth="1"/>
-    <col min="8" max="16384" width="8.7265625" style="3"/>
+    <col min="1" max="4" width="8.7265625" style="3"/>
+    <col min="5" max="5" width="22.81640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="10" style="3" customWidth="1"/>
+    <col min="7" max="7" width="15.6328125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="50.6328125" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="F1" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="3">
+        <v>2</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="B3" s="3">
+        <v>2</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="C5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="G5" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="C6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="H6" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="C7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="E7" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="C8" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="E8" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="C9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="C10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="C11" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="E11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="C12" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="G12" s="3" t="s">
+      <c r="H12" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="C13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="B14" s="3">
+        <v>2</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>14</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="B15" s="3">
+        <v>3</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>25</v>
-      </c>
       <c r="C16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D16" s="3" t="s">
+      <c r="E16" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="G16" s="3" t="s">
+      <c r="H16" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="D17" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="3" t="s">
+      <c r="B17" s="3">
+        <v>2</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E17" s="3" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H17" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="D18" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E18" s="3">
+      <c r="B18" s="3">
+        <v>1</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F18" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="3" t="s">
+      <c r="C19" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G19" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="20" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="D20" s="3" t="s">
+      <c r="B20" s="3">
+        <v>1</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H20" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="G20" s="3" t="s">
-        <v>55</v>
-      </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:H20">
+    <filterColumn colId="2">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Issue #19 select/unselect all in directory bar
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3210" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="4280" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
   <si>
     <t>#</t>
   </si>
@@ -189,9 +189,6 @@
     <t>Break header into own component so can drive behaviour</t>
   </si>
   <si>
-    <t>select/unselect all</t>
-  </si>
-  <si>
     <t>on browse for images need to put the select all and un select all as buttons on the directory bar to save two buttons on the list at the bottom.</t>
   </si>
   <si>
@@ -199,6 +196,15 @@
   </si>
   <si>
     <t>In play mode want to be able to disable tracks Duplicate of 1</t>
+  </si>
+  <si>
+    <t>add return from images to playlist on navbar</t>
+  </si>
+  <si>
+    <t>images to playlist return nav</t>
+  </si>
+  <si>
+    <t>select/unselect all in directory bar</t>
   </si>
 </sst>
 </file>
@@ -670,10 +676,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H20"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -691,7 +697,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>7</v>
@@ -975,7 +981,7 @@
         <v>48</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1016,11 +1022,28 @@
       <c r="B20" s="3">
         <v>1</v>
       </c>
+      <c r="C20" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H20" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H20" s="3" t="s">
-        <v>54</v>
+    </row>
+    <row r="21" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="3">
+        <v>20</v>
+      </c>
+      <c r="B21" s="3">
+        <v>1</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #20 images to playlist return nav
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="62">
   <si>
     <t>#</t>
   </si>
@@ -205,6 +205,15 @@
   </si>
   <si>
     <t>select/unselect all in directory bar</t>
+  </si>
+  <si>
+    <t>When adding all images it also adds the directory</t>
+  </si>
+  <si>
+    <t>don’t add directory to playlist</t>
+  </si>
+  <si>
+    <t>Playlist save not working</t>
   </si>
 </sst>
 </file>
@@ -676,10 +685,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:H23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1046,6 +1055,37 @@
         <v>56</v>
       </c>
     </row>
+    <row r="22" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="3">
+        <v>21</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23" s="3">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3">
+        <v>1</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H20">
     <filterColumn colId="2">

</xml_diff>

<commit_message>
Issue #21 don’t add directory to playlist
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="62">
   <si>
     <t>#</t>
   </si>
@@ -213,7 +213,7 @@
     <t>don’t add directory to playlist</t>
   </si>
   <si>
-    <t>Playlist save not working</t>
+    <t>Playlist save not working.  This was caused by Bitdefender Safe Files</t>
   </si>
 </sst>
 </file>
@@ -688,7 +688,7 @@
   <dimension ref="A1:H23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1048,6 +1048,9 @@
       <c r="B21" s="3">
         <v>1</v>
       </c>
+      <c r="C21" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E21" s="3" t="s">
         <v>57</v>
       </c>
@@ -1062,6 +1065,9 @@
       <c r="B22" s="3">
         <v>1</v>
       </c>
+      <c r="C22" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D22" s="3" t="s">
         <v>31</v>
       </c>
@@ -1072,12 +1078,15 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
       <c r="B23" s="3">
         <v>1</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Issue #24 Add Hamburger Menu
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$H$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$H$25</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="66">
   <si>
     <t>#</t>
   </si>
@@ -214,6 +214,18 @@
   </si>
   <si>
     <t>Playlist save not working.  This was caused by Bitdefender Safe Files</t>
+  </si>
+  <si>
+    <t>Hamburger Menu</t>
+  </si>
+  <si>
+    <t>Add Hamburger menu to top</t>
+  </si>
+  <si>
+    <t>Add slide transitions</t>
+  </si>
+  <si>
+    <t>slide transistion</t>
   </si>
 </sst>
 </file>
@@ -685,10 +697,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -751,6 +764,9 @@
       <c r="E3" s="3" t="s">
         <v>22</v>
       </c>
+      <c r="F3" s="3">
+        <v>24</v>
+      </c>
       <c r="G3" s="3" t="s">
         <v>15</v>
       </c>
@@ -941,6 +957,9 @@
       <c r="B14" s="3">
         <v>2</v>
       </c>
+      <c r="F14" s="3">
+        <v>24</v>
+      </c>
       <c r="H14" s="3" t="s">
         <v>44</v>
       </c>
@@ -993,7 +1012,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1024,7 +1043,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1041,7 +1060,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1058,7 +1077,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1078,7 +1097,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1095,8 +1114,45 @@
         <v>61</v>
       </c>
     </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24" s="3">
+        <v>24</v>
+      </c>
+      <c r="B24" s="3">
+        <v>1</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25" s="3">
+        <v>25</v>
+      </c>
+      <c r="B25" s="3">
+        <v>1</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H20">
+  <autoFilter ref="A1:H25">
     <filterColumn colId="2">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Issue #31 Repackage pages and pageComponents should be separate
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4280" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="5350" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="76">
   <si>
     <t>#</t>
   </si>
@@ -226,6 +226,36 @@
   </si>
   <si>
     <t>slide transistion</t>
+  </si>
+  <si>
+    <t>error</t>
+  </si>
+  <si>
+    <t>Better error handling when REST server not available</t>
+  </si>
+  <si>
+    <t>Hearbeat</t>
+  </si>
+  <si>
+    <t>Settings option to allow for connectivity to REST server to be established</t>
+  </si>
+  <si>
+    <t>icons same size</t>
+  </si>
+  <si>
+    <t>Should make the tick/cross icons the same size so they do not move the screen when they are changeg</t>
+  </si>
+  <si>
+    <t>Should add return from browse playlist to main menu</t>
+  </si>
+  <si>
+    <t>Should have an return nav bar on add playlist</t>
+  </si>
+  <si>
+    <t>arch</t>
+  </si>
+  <si>
+    <t>Repackage pages and pageComponents should be separate</t>
   </si>
 </sst>
 </file>
@@ -697,11 +727,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
+      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1139,7 +1169,7 @@
         <v>25</v>
       </c>
       <c r="B25" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>32</v>
@@ -1149,6 +1179,90 @@
       </c>
       <c r="H25" s="3" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A26" s="3">
+        <v>26</v>
+      </c>
+      <c r="B26" s="3">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A27" s="3">
+        <v>27</v>
+      </c>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F27" s="3">
+        <v>24</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A28" s="3">
+        <v>28</v>
+      </c>
+      <c r="B28" s="3">
+        <v>2</v>
+      </c>
+      <c r="E28" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A29" s="3">
+        <v>29</v>
+      </c>
+      <c r="B29" s="3">
+        <v>2</v>
+      </c>
+      <c r="E29" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A30" s="3">
+        <v>30</v>
+      </c>
+      <c r="B30" s="3">
+        <v>2</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A31" s="3">
+        <v>31</v>
+      </c>
+      <c r="B31" s="3">
+        <v>1</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #30 Should have an return nav bar on add playlist
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$H$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$H$31</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="79">
   <si>
     <t>#</t>
   </si>
@@ -256,6 +256,15 @@
   </si>
   <si>
     <t>Repackage pages and pageComponents should be separate</t>
+  </si>
+  <si>
+    <t>styles to css</t>
+  </si>
+  <si>
+    <t>message/alert component</t>
+  </si>
+  <si>
+    <t>based on timed messages and success/failure</t>
   </si>
 </sst>
 </file>
@@ -727,11 +736,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E31" sqref="E31"/>
+      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1144,7 +1153,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>24</v>
       </c>
@@ -1244,11 +1253,14 @@
       <c r="B30" s="3">
         <v>2</v>
       </c>
+      <c r="C30" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E30" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>31</v>
       </c>
@@ -1265,8 +1277,33 @@
         <v>75</v>
       </c>
     </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
+      <c r="B32" s="3">
+        <v>2</v>
+      </c>
+      <c r="E32" s="3" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A33" s="3">
+        <v>32</v>
+      </c>
+      <c r="B33" s="3">
+        <v>2</v>
+      </c>
+      <c r="E33" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H25">
+  <autoFilter ref="A1:H31">
     <filterColumn colId="2">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Issue #28 icons same size
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="81">
   <si>
     <t>#</t>
   </si>
@@ -265,6 +265,12 @@
   </si>
   <si>
     <t>based on timed messages and success/failure</t>
+  </si>
+  <si>
+    <t>icon config</t>
+  </si>
+  <si>
+    <t>move the config styles for icons into config and icon width</t>
   </si>
 </sst>
 </file>
@@ -736,11 +742,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H33"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B33" sqref="B33"/>
+      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1228,6 +1234,9 @@
       <c r="B28" s="3">
         <v>2</v>
       </c>
+      <c r="C28" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E28" s="3" t="s">
         <v>70</v>
       </c>
@@ -1242,6 +1251,9 @@
       <c r="B29" s="3">
         <v>2</v>
       </c>
+      <c r="C29" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E29" s="3" t="s">
         <v>72</v>
       </c>
@@ -1300,6 +1312,20 @@
       </c>
       <c r="H33" s="3" t="s">
         <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A34" s="3">
+        <v>33</v>
+      </c>
+      <c r="B34" s="3">
+        <v>2</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #35 Blank settings page
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$H$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$H$34</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="83">
   <si>
     <t>#</t>
   </si>
@@ -162,9 +162,6 @@
     <t>Enabple playlist folders</t>
   </si>
   <si>
-    <t>Better Top Navigation … title and hamburger</t>
-  </si>
-  <si>
     <t>Remove dirname from browse images path in app.module.ts</t>
   </si>
   <si>
@@ -271,6 +268,16 @@
   </si>
   <si>
     <t>move the config styles for icons into config and icon width</t>
+  </si>
+  <si>
+    <t>Better Top Navigation … title and hamburger.
+No code change … fixed as consequnce of other changes</t>
+  </si>
+  <si>
+    <t>Settings page placehold for other stuff</t>
+  </si>
+  <si>
+    <t>Blank settings page</t>
   </si>
 </sst>
 </file>
@@ -742,11 +749,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H34"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E28" sqref="E28"/>
+      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -764,7 +771,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>7</v>
@@ -776,7 +783,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>3</v>
@@ -804,13 +811,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>22</v>
       </c>
       <c r="F3" s="3">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>15</v>
@@ -824,10 +831,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>21</v>
+      </c>
+      <c r="F4" s="3">
+        <v>35</v>
       </c>
       <c r="G4" s="3" t="s">
         <v>15</v>
@@ -995,18 +1005,21 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
       <c r="B14" s="3">
         <v>2</v>
       </c>
+      <c r="C14" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="F14" s="3">
         <v>24</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>44</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1031,13 +1044,13 @@
         <v>25</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>47</v>
-      </c>
       <c r="H16" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1051,10 +1064,10 @@
         <v>25</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -1068,7 +1081,7 @@
         <v>25</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F18" s="3">
         <v>18</v>
@@ -1082,10 +1095,10 @@
         <v>25</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>51</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
@@ -1099,10 +1112,10 @@
         <v>25</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1116,10 +1129,10 @@
         <v>25</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1136,10 +1149,10 @@
         <v>31</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1156,7 +1169,7 @@
         <v>31</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -1173,10 +1186,10 @@
         <v>32</v>
       </c>
       <c r="E24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -1190,10 +1203,10 @@
         <v>32</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -1204,10 +1217,10 @@
         <v>1</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -1218,16 +1231,16 @@
         <v>1</v>
       </c>
       <c r="E27" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F27" s="3">
+        <v>35</v>
+      </c>
+      <c r="H27" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F27" s="3">
-        <v>24</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>28</v>
       </c>
@@ -1238,13 +1251,13 @@
         <v>25</v>
       </c>
       <c r="E28" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H28" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="H28" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:8" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>29</v>
       </c>
@@ -1255,10 +1268,10 @@
         <v>25</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>30</v>
       </c>
@@ -1269,7 +1282,7 @@
         <v>25</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
@@ -1283,10 +1296,10 @@
         <v>25</v>
       </c>
       <c r="D31" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E31" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -1297,7 +1310,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -1308,28 +1321,48 @@
         <v>2</v>
       </c>
       <c r="E33" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="H33" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H33" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>33</v>
       </c>
       <c r="B34" s="3">
         <v>2</v>
       </c>
+      <c r="C34" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E34" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H34" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="H34" s="3" t="s">
-        <v>80</v>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A35" s="3">
+        <v>35</v>
+      </c>
+      <c r="B35" s="3">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H35" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H31">
+  <autoFilter ref="A1:H34">
     <filterColumn colId="2">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Issue #38 plus on add image is cross
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="89">
   <si>
     <t>#</t>
   </si>
@@ -278,6 +278,24 @@
   </si>
   <si>
     <t>Blank settings page</t>
+  </si>
+  <si>
+    <t>REST server check</t>
+  </si>
+  <si>
+    <t>Check connectivity to Server on settings page</t>
+  </si>
+  <si>
+    <t>REST ping service</t>
+  </si>
+  <si>
+    <t>Add a rest ping service</t>
+  </si>
+  <si>
+    <t>Bug</t>
+  </si>
+  <si>
+    <t>plus on add image is cross</t>
   </si>
 </sst>
 </file>
@@ -749,11 +767,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:H38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
+      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1361,6 +1379,51 @@
         <v>81</v>
       </c>
     </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A36" s="3">
+        <v>36</v>
+      </c>
+      <c r="B36" s="3">
+        <v>1</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A37" s="3">
+        <v>37</v>
+      </c>
+      <c r="B37" s="3">
+        <v>1</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F37" s="3">
+        <v>37</v>
+      </c>
+      <c r="H37" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A38" s="3">
+        <v>38</v>
+      </c>
+      <c r="B38" s="3">
+        <v>1</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:H34">
     <filterColumn colId="2">

</xml_diff>

<commit_message>
Issue #36 REST server check
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="92">
   <si>
     <t>#</t>
   </si>
@@ -296,6 +296,15 @@
   </si>
   <si>
     <t>plus on add image is cross</t>
+  </si>
+  <si>
+    <t>need a way to kill and restart server from browser</t>
+  </si>
+  <si>
+    <t>pressing hambuger on settings takes you to main</t>
+  </si>
+  <si>
+    <t>bug</t>
   </si>
 </sst>
 </file>
@@ -767,11 +776,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H38"/>
+  <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
+      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1386,6 +1395,9 @@
       <c r="B36" s="3">
         <v>1</v>
       </c>
+      <c r="C36" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E36" s="3" t="s">
         <v>83</v>
       </c>
@@ -1400,6 +1412,9 @@
       <c r="B37" s="3">
         <v>1</v>
       </c>
+      <c r="C37" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E37" s="3" t="s">
         <v>85</v>
       </c>
@@ -1417,11 +1432,39 @@
       <c r="B38" s="3">
         <v>1</v>
       </c>
+      <c r="C38" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="D38" s="3" t="s">
         <v>87</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A39" s="3">
+        <v>39</v>
+      </c>
+      <c r="B39" s="3">
+        <v>2</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H39" s="3" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A40" s="3">
+        <v>40</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #42 upgrade Playlist to use Message Component
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5350" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="6420" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$H$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$H$40</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="96">
   <si>
     <t>#</t>
   </si>
@@ -69,9 +69,6 @@
     <t>Want to be able to have a temporary omit on a track that stops it from playing.  This would mean that I would not have to delete if from the track and re-add (from a nested directory) it to turn it off and on.</t>
   </si>
   <si>
-    <t>Track Disable</t>
-  </si>
-  <si>
     <t>Playlist Settings</t>
   </si>
   <si>
@@ -232,9 +229,6 @@
   </si>
   <si>
     <t>Hearbeat</t>
-  </si>
-  <si>
-    <t>Settings option to allow for connectivity to REST server to be established</t>
   </si>
   <si>
     <t>icons same size</t>
@@ -305,6 +299,24 @@
   </si>
   <si>
     <t>bug</t>
+  </si>
+  <si>
+    <t>Track Disable Client</t>
+  </si>
+  <si>
+    <t>Add track disable to server</t>
+  </si>
+  <si>
+    <t>Settings option to allow for connectivity to REST server to be established - non needed as there is now the poll for change</t>
+  </si>
+  <si>
+    <t>There is a better approach but this is not done everyhwere yet.  This still needs to be done for the repo fetches of data</t>
+  </si>
+  <si>
+    <t>Make the playlist save and play errors use the Message component</t>
+  </si>
+  <si>
+    <t>upgrade Playlist to use Message Component</t>
   </si>
 </sst>
 </file>
@@ -737,34 +749,34 @@
     </row>
     <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>17</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -776,11 +788,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E36" sqref="E36"/>
+      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -798,7 +810,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>7</v>
@@ -810,7 +822,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>3</v>
@@ -826,8 +838,11 @@
       <c r="B2" s="3">
         <v>2</v>
       </c>
+      <c r="C2" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E2" s="3" t="s">
-        <v>13</v>
+        <v>90</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>12</v>
@@ -841,16 +856,16 @@
         <v>1</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F3" s="3">
         <v>35</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -861,16 +876,16 @@
         <v>1</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F4" s="3">
         <v>35</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -878,16 +893,16 @@
         <v>4</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -895,16 +910,16 @@
         <v>5</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -912,19 +927,19 @@
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -932,16 +947,16 @@
         <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -949,19 +964,19 @@
         <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -969,13 +984,13 @@
         <v>9</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -983,19 +998,19 @@
         <v>10</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1003,16 +1018,16 @@
         <v>11</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1020,16 +1035,16 @@
         <v>12</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1040,13 +1055,13 @@
         <v>2</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14" s="3">
         <v>24</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1060,7 +1075,7 @@
         <v>6</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1068,16 +1083,16 @@
         <v>15</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>46</v>
-      </c>
       <c r="H16" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1088,13 +1103,13 @@
         <v>2</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -1105,10 +1120,10 @@
         <v>1</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F18" s="3">
         <v>18</v>
@@ -1119,13 +1134,13 @@
         <v>18</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
@@ -1136,13 +1151,13 @@
         <v>1</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1153,13 +1168,13 @@
         <v>1</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1170,16 +1185,16 @@
         <v>1</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1190,13 +1205,13 @@
         <v>1</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -1207,16 +1222,16 @@
         <v>1</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -1227,13 +1242,13 @@
         <v>2</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -1244,13 +1259,16 @@
         <v>1</v>
       </c>
       <c r="D26" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="H26" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>27</v>
       </c>
@@ -1258,13 +1276,13 @@
         <v>1</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F27" s="3">
         <v>35</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>68</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1275,13 +1293,13 @@
         <v>2</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
@@ -1292,10 +1310,10 @@
         <v>2</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1306,10 +1324,10 @@
         <v>2</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
@@ -1320,13 +1338,13 @@
         <v>1</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -1337,7 +1355,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -1348,10 +1366,10 @@
         <v>2</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -1362,16 +1380,16 @@
         <v>2</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>35</v>
       </c>
@@ -1379,16 +1397,16 @@
         <v>1</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>36</v>
       </c>
@@ -1396,16 +1414,16 @@
         <v>1</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>37</v>
       </c>
@@ -1413,19 +1431,19 @@
         <v>1</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F37" s="3">
         <v>37</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>38</v>
       </c>
@@ -1433,13 +1451,13 @@
         <v>1</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
@@ -1450,25 +1468,53 @@
         <v>2</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>40</v>
       </c>
+      <c r="B40" s="3">
+        <v>3</v>
+      </c>
       <c r="D40" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A41" s="3">
+        <v>41</v>
+      </c>
+      <c r="B41" s="3">
+        <v>2</v>
+      </c>
+      <c r="E41" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H40" s="3" t="s">
-        <v>90</v>
+    </row>
+    <row r="42" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A42" s="3">
+        <v>42</v>
+      </c>
+      <c r="B42" s="3">
+        <v>1</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>94</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H34">
+  <autoFilter ref="A1:H40">
     <filterColumn colId="2">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Issue #41 Add track disable to server
Fixed a couple of UI things and put enable/disable icons into config
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="96">
   <si>
     <t>#</t>
   </si>
@@ -792,7 +792,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E42" sqref="E42"/>
+      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1495,6 +1495,9 @@
       <c r="B41" s="3">
         <v>2</v>
       </c>
+      <c r="C41" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E41" s="3" t="s">
         <v>91</v>
       </c>
@@ -1505,6 +1508,9 @@
       </c>
       <c r="B42" s="3">
         <v>1</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>95</v>

</xml_diff>

<commit_message>
Issue #48 ng bulid failure
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$H$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$H$44</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="106">
   <si>
     <t>#</t>
   </si>
@@ -156,9 +156,6 @@
     <t>Would be good to have an overall brightness Hamburger Menu</t>
   </si>
   <si>
-    <t>Enabple playlist folders</t>
-  </si>
-  <si>
     <t>Remove dirname from browse images path in app.module.ts</t>
   </si>
   <si>
@@ -222,9 +219,6 @@
     <t>slide transistion</t>
   </si>
   <si>
-    <t>error</t>
-  </si>
-  <si>
     <t>Better error handling when REST server not available</t>
   </si>
   <si>
@@ -253,9 +247,6 @@
   </si>
   <si>
     <t>message/alert component</t>
-  </si>
-  <si>
-    <t>based on timed messages and success/failure</t>
   </si>
   <si>
     <t>icon config</t>
@@ -310,13 +301,54 @@
     <t>Settings option to allow for connectivity to REST server to be established - non needed as there is now the poll for change</t>
   </si>
   <si>
-    <t>There is a better approach but this is not done everyhwere yet.  This still needs to be done for the repo fetches of data</t>
-  </si>
-  <si>
     <t>Make the playlist save and play errors use the Message component</t>
   </si>
   <si>
     <t>upgrade Playlist to use Message Component</t>
+  </si>
+  <si>
+    <t>Prevent playing unsaved data</t>
+  </si>
+  <si>
+    <t>encapsulate playlist into a model and protect the data</t>
+  </si>
+  <si>
+    <t>There is a better approach but this is not done everyhwere yet.  This still needs to be done for the repo fetches of data
+It is kind of obvious as there is no data … and there is the settings option to test connectivity</t>
+  </si>
+  <si>
+    <t>Server side handling for config</t>
+  </si>
+  <si>
+    <t>Server side handling for config.</t>
+  </si>
+  <si>
+    <t>CLOSED</t>
+  </si>
+  <si>
+    <t>Enable playlist folders</t>
+  </si>
+  <si>
+    <t>based on timed messages and success/failure
+this has been done</t>
+  </si>
+  <si>
+    <t>issue</t>
+  </si>
+  <si>
+    <t>need to debounce button</t>
+  </si>
+  <si>
+    <t>Error Handling</t>
+  </si>
+  <si>
+    <t>move /app to /</t>
+  </si>
+  <si>
+    <t>handle 404</t>
+  </si>
+  <si>
+    <t>ng bulid failure</t>
   </si>
 </sst>
 </file>
@@ -788,11 +820,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H42"/>
+  <dimension ref="A1:H48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C41" sqref="C41"/>
+      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -810,7 +842,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>7</v>
@@ -822,7 +854,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>3</v>
@@ -831,7 +863,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -842,7 +874,7 @@
         <v>24</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>12</v>
@@ -1061,21 +1093,24 @@
         <v>24</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
+        <v>44</v>
+      </c>
+      <c r="B15" s="3">
+        <v>1</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="3">
-        <v>3</v>
-      </c>
-      <c r="G15" s="3" t="s">
-        <v>6</v>
-      </c>
       <c r="H15" s="3" t="s">
-        <v>42</v>
+        <v>96</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1086,13 +1121,13 @@
         <v>24</v>
       </c>
       <c r="D16" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>45</v>
-      </c>
       <c r="H16" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1106,10 +1141,10 @@
         <v>24</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -1123,7 +1158,7 @@
         <v>24</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F18" s="3">
         <v>18</v>
@@ -1137,10 +1172,10 @@
         <v>24</v>
       </c>
       <c r="E19" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H19" s="3" t="s">
         <v>49</v>
-      </c>
-      <c r="H19" s="3" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
@@ -1154,10 +1189,10 @@
         <v>24</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1171,10 +1206,10 @@
         <v>24</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1191,10 +1226,10 @@
         <v>30</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1211,7 +1246,7 @@
         <v>30</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -1228,61 +1263,58 @@
         <v>31</v>
       </c>
       <c r="E24" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H24" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H24" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    </row>
+    <row r="25" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B25" s="3">
-        <v>2</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>63</v>
       </c>
+      <c r="G25" s="3" t="s">
+        <v>102</v>
+      </c>
       <c r="H25" s="3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="B26" s="3">
-        <v>1</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>64</v>
+        <v>3</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="H26" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>27</v>
       </c>
       <c r="B27" s="3">
         <v>1</v>
       </c>
+      <c r="C27" s="3" t="s">
+        <v>97</v>
+      </c>
       <c r="E27" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F27" s="3">
         <v>35</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1296,10 +1328,10 @@
         <v>24</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
@@ -1313,7 +1345,7 @@
         <v>24</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1327,7 +1359,7 @@
         <v>24</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
@@ -1341,35 +1373,41 @@
         <v>24</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E31" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="A32" s="3">
+        <v>32</v>
+      </c>
+      <c r="B32" s="3">
+        <v>3</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="3">
-        <v>31</v>
-      </c>
-      <c r="B32" s="3">
-        <v>2</v>
-      </c>
-      <c r="E32" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+      <c r="H32" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B33" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -1383,10 +1421,10 @@
         <v>24</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -1400,10 +1438,10 @@
         <v>24</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -1417,10 +1455,10 @@
         <v>24</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -1434,13 +1472,13 @@
         <v>24</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F37" s="3">
         <v>37</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
@@ -1454,41 +1492,41 @@
         <v>24</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="B39" s="3">
         <v>2</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="B40" s="3">
-        <v>3</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>89</v>
+        <v>5</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>41</v>
       </c>
@@ -1499,10 +1537,10 @@
         <v>24</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>42</v>
       </c>
@@ -1513,17 +1551,110 @@
         <v>24</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>94</v>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A43" s="3">
+        <v>25</v>
+      </c>
+      <c r="B43" s="3">
+        <v>5</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A44" s="3">
+        <v>40</v>
+      </c>
+      <c r="B44" s="3">
+        <v>5</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A45" s="3">
+        <v>45</v>
+      </c>
+      <c r="B45" s="3">
+        <v>1</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A46" s="3">
+        <v>46</v>
+      </c>
+      <c r="B46" s="3">
+        <v>1</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A47" s="3">
+        <v>47</v>
+      </c>
+      <c r="B47" s="3">
+        <v>3</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A48" s="3">
+        <v>48</v>
+      </c>
+      <c r="B48" s="3">
+        <v>1</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H40">
+  <autoFilter ref="A1:H44">
     <filterColumn colId="2">
       <filters blank="1"/>
     </filterColumn>
+    <sortState ref="A3:H44">
+      <sortCondition ref="B2:B44"/>
+    </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Issue #46 move /app to /
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="106">
   <si>
     <t>#</t>
   </si>
@@ -824,7 +824,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C48" sqref="C48"/>
+      <selection pane="bottomLeft" activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1609,6 +1609,9 @@
       <c r="B46" s="3">
         <v>1</v>
       </c>
+      <c r="C46" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="D46" s="3" t="s">
         <v>69</v>
       </c>

</xml_diff>

<commit_message>
Issue #45 need to debounce button
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="108">
   <si>
     <t>#</t>
   </si>
@@ -349,6 +349,12 @@
   </si>
   <si>
     <t>ng bulid failure</t>
+  </si>
+  <si>
+    <t>piW fav icon</t>
+  </si>
+  <si>
+    <t>run on port 80</t>
   </si>
 </sst>
 </file>
@@ -820,11 +826,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H48"/>
+  <dimension ref="A1:H50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E46" sqref="E46"/>
+      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1595,6 +1601,9 @@
       <c r="B45" s="3">
         <v>1</v>
       </c>
+      <c r="C45" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="D45" s="3" t="s">
         <v>100</v>
       </c>
@@ -1648,6 +1657,34 @@
       </c>
       <c r="E48" s="3" t="s">
         <v>105</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A49" s="3">
+        <v>49</v>
+      </c>
+      <c r="B49" s="3">
+        <v>3</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A50" s="3">
+        <v>50</v>
+      </c>
+      <c r="B50" s="3">
+        <v>3</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #52 REST getConfig
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="7490" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$H$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$H$52</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="111">
   <si>
     <t>#</t>
   </si>
@@ -355,6 +355,15 @@
   </si>
   <si>
     <t>run on port 80</t>
+  </si>
+  <si>
+    <t>Need to be able to config debounce timeout</t>
+  </si>
+  <si>
+    <t>REST service for get config</t>
+  </si>
+  <si>
+    <t>REST service for set config</t>
   </si>
 </sst>
 </file>
@@ -826,11 +835,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H50"/>
+  <dimension ref="A1:H53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C45" sqref="C45"/>
+      <selection pane="bottomLeft" activeCell="C56" sqref="C56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1385,7 +1394,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>32</v>
       </c>
@@ -1594,7 +1603,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>45</v>
       </c>
@@ -1611,7 +1620,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>46</v>
       </c>
@@ -1642,7 +1651,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>48</v>
       </c>
@@ -1659,7 +1668,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>49</v>
       </c>
@@ -1673,7 +1682,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>50</v>
       </c>
@@ -1687,8 +1696,56 @@
         <v>107</v>
       </c>
     </row>
+    <row r="51" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A51" s="3">
+        <v>51</v>
+      </c>
+      <c r="B51" s="3">
+        <v>3</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A52" s="3">
+        <v>52</v>
+      </c>
+      <c r="B52" s="3">
+        <v>2</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A53" s="3">
+        <v>51</v>
+      </c>
+      <c r="B53" s="3">
+        <v>2</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:H44">
+  <autoFilter ref="A1:H52">
     <filterColumn colId="2">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Issue #57 modal library inclusion
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$H$52</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$56</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="116">
   <si>
     <t>#</t>
   </si>
@@ -320,9 +320,6 @@
     <t>Server side handling for config</t>
   </si>
   <si>
-    <t>Server side handling for config.</t>
-  </si>
-  <si>
     <t>CLOSED</t>
   </si>
   <si>
@@ -373,6 +370,15 @@
   </si>
   <si>
     <t>update internals based on post config</t>
+  </si>
+  <si>
+    <t>Seq</t>
+  </si>
+  <si>
+    <t>Server side handling for config.  Split into 53 and 56</t>
+  </si>
+  <si>
+    <t>modal library inclusion</t>
   </si>
 </sst>
 </file>
@@ -844,976 +850,999 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:H56"/>
+  <dimension ref="A1:I57"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E53" sqref="E53"/>
+      <selection pane="bottomLeft" activeCell="A58" sqref="A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="8.7265625" style="3"/>
-    <col min="5" max="5" width="22.81640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="10" style="3" customWidth="1"/>
-    <col min="7" max="7" width="15.6328125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="50.6328125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="8.7265625" style="3"/>
+    <col min="1" max="5" width="8.7265625" style="3"/>
+    <col min="6" max="6" width="22.81640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="10" style="3" customWidth="1"/>
+    <col min="8" max="8" width="15.6328125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="50.6328125" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>1</v>
-      </c>
       <c r="F1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="C2" s="3">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="D2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="s">
+      <c r="C3" s="3">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="3">
+      <c r="G3" s="3">
         <v>35</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="C4" s="3">
+        <v>1</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="3">
+      <c r="G4" s="3">
         <v>35</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
-      <c r="C5" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="D5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="G5" s="3" t="s">
+      <c r="H5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="D6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="D7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="D8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="D9" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="D10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="I10" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="D11" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="D12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="H12" s="3" t="s">
+      <c r="I12" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="D13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
+      <c r="C14" s="3">
         <v>2</v>
       </c>
-      <c r="C14" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="3">
-        <v>24</v>
-      </c>
-      <c r="H14" s="3" t="s">
+      <c r="D14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G14" s="3">
+        <v>24</v>
+      </c>
+      <c r="I14" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>44</v>
       </c>
-      <c r="B15" s="3">
-        <v>1</v>
-      </c>
-      <c r="E15" s="3" t="s">
+      <c r="C15" s="3">
+        <v>1</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H15" s="3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I15" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
-      <c r="C16" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="D16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="H16" s="3" t="s">
+      <c r="I16" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
-      <c r="B17" s="3">
+      <c r="C17" s="3">
         <v>2</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E17" s="3" t="s">
+      <c r="D17" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H17" s="3" t="s">
+      <c r="I17" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
-      <c r="B18" s="3">
-        <v>1</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E18" s="3" t="s">
+      <c r="C18" s="3">
+        <v>1</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F18" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F18" s="3">
+      <c r="G18" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="3" t="s">
+      <c r="D19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="I19" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
-      <c r="B20" s="3">
-        <v>1</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E20" s="3" t="s">
+      <c r="C20" s="3">
+        <v>1</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F20" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="I20" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
-      <c r="B21" s="3">
-        <v>1</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E21" s="3" t="s">
+      <c r="C21" s="3">
+        <v>1</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H21" s="3" t="s">
+      <c r="I21" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
-      <c r="B22" s="3">
-        <v>1</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>24</v>
+      <c r="C22" s="3">
+        <v>1</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H22" s="3" t="s">
+      <c r="I22" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
-      <c r="B23" s="3">
-        <v>1</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>24</v>
+      <c r="C23" s="3">
+        <v>1</v>
       </c>
       <c r="D23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H23" s="3" t="s">
+      <c r="I23" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>24</v>
       </c>
-      <c r="B24" s="3">
-        <v>1</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>24</v>
+      <c r="C24" s="3">
+        <v>1</v>
       </c>
       <c r="D24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H24" s="3" t="s">
+      <c r="I24" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>26</v>
       </c>
-      <c r="B25" s="3">
+      <c r="C25" s="3">
         <v>3</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G25" s="3" t="s">
-        <v>102</v>
-      </c>
       <c r="H25" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I25" s="3" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>31</v>
       </c>
-      <c r="B26" s="3">
+      <c r="C26" s="3">
         <v>3</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>27</v>
       </c>
-      <c r="B27" s="3">
-        <v>1</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E27" s="3" t="s">
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F27" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F27" s="3">
+      <c r="G27" s="3">
         <v>35</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="I27" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>28</v>
       </c>
-      <c r="B28" s="3">
+      <c r="C28" s="3">
         <v>2</v>
       </c>
-      <c r="C28" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E28" s="3" t="s">
+      <c r="D28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F28" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="I28" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>29</v>
       </c>
-      <c r="B29" s="3">
+      <c r="C29" s="3">
         <v>2</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E29" s="3" t="s">
+      <c r="D29" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>30</v>
       </c>
-      <c r="B30" s="3">
+      <c r="C30" s="3">
         <v>2</v>
       </c>
-      <c r="C30" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E30" s="3" t="s">
+      <c r="D30" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="3" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>31</v>
       </c>
-      <c r="B31" s="3">
-        <v>1</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>24</v>
+      <c r="C31" s="3">
+        <v>1</v>
       </c>
       <c r="D31" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E31" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>32</v>
       </c>
-      <c r="B32" s="3">
+      <c r="C32" s="3">
         <v>3</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="E32" s="3" t="s">
+      <c r="D32" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="F32" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H32" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="I32" s="3" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>39</v>
       </c>
-      <c r="B33" s="3">
+      <c r="C33" s="3">
         <v>3</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="F33" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="H33" s="3" t="s">
+      <c r="I33" s="3" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>33</v>
       </c>
-      <c r="B34" s="3">
+      <c r="C34" s="3">
         <v>2</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E34" s="3" t="s">
+      <c r="D34" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="H34" s="3" t="s">
+      <c r="I34" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>35</v>
       </c>
-      <c r="B35" s="3">
-        <v>1</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E35" s="3" t="s">
+      <c r="C35" s="3">
+        <v>1</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="H35" s="3" t="s">
+      <c r="I35" s="3" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>36</v>
       </c>
-      <c r="B36" s="3">
-        <v>1</v>
-      </c>
-      <c r="C36" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E36" s="3" t="s">
+      <c r="C36" s="3">
+        <v>1</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F36" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="I36" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>37</v>
       </c>
-      <c r="B37" s="3">
-        <v>1</v>
-      </c>
-      <c r="C37" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E37" s="3" t="s">
+      <c r="C37" s="3">
+        <v>1</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="F37" s="3">
+      <c r="G37" s="3">
         <v>37</v>
       </c>
-      <c r="H37" s="3" t="s">
+      <c r="I37" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>38</v>
       </c>
-      <c r="B38" s="3">
-        <v>1</v>
-      </c>
-      <c r="C38" s="3" t="s">
-        <v>24</v>
+      <c r="C38" s="3">
+        <v>1</v>
       </c>
       <c r="D38" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E38" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>43</v>
       </c>
-      <c r="B39" s="3">
+      <c r="C39" s="3">
         <v>2</v>
       </c>
-      <c r="E39" s="3" t="s">
+      <c r="F39" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="H39" s="3" t="s">
+      <c r="I39" s="3" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>14</v>
       </c>
-      <c r="B40" s="3">
+      <c r="C40" s="3">
         <v>5</v>
       </c>
-      <c r="G40" s="3" t="s">
+      <c r="H40" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H40" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="I40" s="3" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>41</v>
       </c>
-      <c r="B41" s="3">
+      <c r="C41" s="3">
         <v>2</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E41" s="3" t="s">
+      <c r="D41" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>42</v>
       </c>
-      <c r="B42" s="3">
-        <v>1</v>
-      </c>
-      <c r="C42" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E42" s="3" t="s">
+      <c r="C42" s="3">
+        <v>1</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="H42" s="3" t="s">
+      <c r="I42" s="3" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>25</v>
       </c>
-      <c r="B43" s="3">
+      <c r="C43" s="3">
         <v>5</v>
       </c>
-      <c r="D43" s="3" t="s">
+      <c r="E43" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="F43" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H43" s="3" t="s">
+      <c r="I43" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>40</v>
       </c>
-      <c r="B44" s="3">
+      <c r="C44" s="3">
         <v>5</v>
       </c>
-      <c r="D44" s="3" t="s">
+      <c r="E44" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="H44" s="3" t="s">
+      <c r="I44" s="3" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>45</v>
       </c>
-      <c r="B45" s="3">
-        <v>1</v>
-      </c>
-      <c r="C45" s="3" t="s">
-        <v>24</v>
+      <c r="C45" s="3">
+        <v>1</v>
       </c>
       <c r="D45" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="F45" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="E45" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>46</v>
       </c>
-      <c r="B46" s="3">
-        <v>1</v>
-      </c>
-      <c r="C46" s="3" t="s">
-        <v>24</v>
+      <c r="C46" s="3">
+        <v>1</v>
       </c>
       <c r="D46" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E46" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F46" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>47</v>
       </c>
-      <c r="B47" s="3">
+      <c r="C47" s="3">
         <v>3</v>
       </c>
-      <c r="D47" s="3" t="s">
+      <c r="E47" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F47" s="3" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>48</v>
       </c>
-      <c r="B48" s="3">
-        <v>1</v>
-      </c>
-      <c r="C48" s="3" t="s">
-        <v>24</v>
+      <c r="C48" s="3">
+        <v>1</v>
       </c>
       <c r="D48" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E48" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E48" s="3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F48" s="3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>49</v>
       </c>
-      <c r="B49" s="3">
+      <c r="C49" s="3">
         <v>3</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="E49" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="F49" s="3" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>50</v>
       </c>
-      <c r="B50" s="3">
+      <c r="C50" s="3">
         <v>3</v>
       </c>
-      <c r="D50" s="3" t="s">
+      <c r="E50" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E50" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="51" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="F50" s="3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>51</v>
       </c>
       <c r="B51" s="3">
+        <v>2</v>
+      </c>
+      <c r="C51" s="3">
         <v>3</v>
       </c>
-      <c r="E51" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="G51" s="3" t="s">
+      <c r="F51" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="H51" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>52</v>
       </c>
-      <c r="B52" s="3">
+      <c r="C52" s="3">
         <v>2</v>
       </c>
-      <c r="C52" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="D52" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E52" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E52" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="G52" s="3" t="s">
+      <c r="F52" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="H52" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>53</v>
       </c>
-      <c r="B53" s="3">
+      <c r="C53" s="3">
         <v>2</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>24</v>
-      </c>
       <c r="D53" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E53" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E53" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="G53" s="3" t="s">
+      <c r="F53" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="H53" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>54</v>
       </c>
       <c r="B54" s="3">
+        <v>1</v>
+      </c>
+      <c r="C54" s="3">
         <v>2</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="E54" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E54" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="G54" s="3" t="s">
+      <c r="F54" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H54" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>55</v>
       </c>
-      <c r="B55" s="3">
+      <c r="C55" s="3">
         <v>2</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="E55" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E55" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="G55" s="3" t="s">
+      <c r="F55" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="H55" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>56</v>
       </c>
-      <c r="B56" s="3">
+      <c r="C56" s="3">
         <v>2</v>
       </c>
-      <c r="D56" s="3" t="s">
+      <c r="E56" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="E56" s="3" t="s">
-        <v>113</v>
+      <c r="F56" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A57" s="3">
+        <v>57</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H52">
-    <filterColumn colId="2">
+  <autoFilter ref="A1:I56">
+    <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
-    <sortState ref="A3:H44">
-      <sortCondition ref="B2:B44"/>
+    <sortState ref="A3:I44">
+      <sortCondition ref="C2:C44"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Issue #65 added version number to PlaylistDTO, and hence saved file
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="9630" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="10700" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="127">
   <si>
     <t>#</t>
   </si>
@@ -398,6 +398,21 @@
   </si>
   <si>
     <t>playlist model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arch </t>
+  </si>
+  <si>
+    <t>emulator to share same server as main</t>
+  </si>
+  <si>
+    <t>means that there are not two ports</t>
+  </si>
+  <si>
+    <t>angular logging</t>
+  </si>
+  <si>
+    <t>version numbers on saved playlist</t>
   </si>
 </sst>
 </file>
@@ -869,11 +884,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I62"/>
+  <dimension ref="A1:I65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G62" sqref="G62"/>
+      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E72" sqref="E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1903,11 +1918,47 @@
       <c r="A62" s="3">
         <v>62</v>
       </c>
+      <c r="D62" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E62" s="3" t="s">
         <v>69</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A63" s="3">
+        <v>63</v>
+      </c>
+      <c r="E63" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I63" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A64" s="3">
+        <v>64</v>
+      </c>
+      <c r="F64" s="3" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A65" s="3">
+        <v>65</v>
+      </c>
+      <c r="D65" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F65" s="3" t="s">
+        <v>126</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issues #2, #3, #51, #54, #55 Basic config set and send
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="128">
   <si>
     <t>#</t>
   </si>
@@ -413,6 +413,9 @@
   </si>
   <si>
     <t>version numbers on saved playlist</t>
+  </si>
+  <si>
+    <t>handle error in Repository services</t>
   </si>
 </sst>
 </file>
@@ -884,11 +887,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I65"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E72" sqref="E72"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -954,6 +957,9 @@
       <c r="C3" s="3">
         <v>1</v>
       </c>
+      <c r="D3" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="F3" s="3" t="s">
         <v>21</v>
       </c>
@@ -974,6 +980,9 @@
       <c r="C4" s="3">
         <v>1</v>
       </c>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="F4" s="3" t="s">
         <v>20</v>
       </c>
@@ -1761,6 +1770,9 @@
       <c r="C51" s="3">
         <v>3</v>
       </c>
+      <c r="D51" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="F51" s="3" t="s">
         <v>107</v>
       </c>
@@ -1818,6 +1830,9 @@
       <c r="C54" s="3">
         <v>2</v>
       </c>
+      <c r="D54" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E54" s="3" t="s">
         <v>69</v>
       </c>
@@ -1835,6 +1850,9 @@
       <c r="C55" s="3">
         <v>2</v>
       </c>
+      <c r="D55" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E55" s="3" t="s">
         <v>69</v>
       </c>
@@ -1863,6 +1881,9 @@
       <c r="A57" s="3">
         <v>57</v>
       </c>
+      <c r="D57" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E57" s="3" t="s">
         <v>31</v>
       </c>
@@ -1959,6 +1980,17 @@
       </c>
       <c r="F65" s="3" t="s">
         <v>126</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A66" s="3">
+        <v>66</v>
+      </c>
+      <c r="D66" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F66" s="3" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #56 server implementation of speed, brightness, NUM_LEDS config
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$56</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$66</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="130">
   <si>
     <t>#</t>
   </si>
@@ -416,6 +416,12 @@
   </si>
   <si>
     <t>handle error in Repository services</t>
+  </si>
+  <si>
+    <t>server implementaiton of debounce config from client</t>
+  </si>
+  <si>
+    <t>when updating config need to reload playlist</t>
   </si>
 </sst>
 </file>
@@ -887,11 +893,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I66"/>
+  <dimension ref="A1:I68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
+      <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -950,7 +956,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -973,7 +979,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1760,7 +1766,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>51</v>
       </c>
@@ -1820,7 +1826,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>54</v>
       </c>
@@ -1843,7 +1849,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>55</v>
       </c>
@@ -1870,6 +1876,9 @@
       <c r="C56" s="3">
         <v>2</v>
       </c>
+      <c r="D56" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E56" s="3" t="s">
         <v>69</v>
       </c>
@@ -1877,7 +1886,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>57</v>
       </c>
@@ -1935,7 +1944,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>62</v>
       </c>
@@ -1971,7 +1980,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>65</v>
       </c>
@@ -1982,7 +1991,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>66</v>
       </c>
@@ -1993,8 +2002,24 @@
         <v>127</v>
       </c>
     </row>
+    <row r="67" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A67" s="3">
+        <v>67</v>
+      </c>
+      <c r="F67" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+      <c r="A68" s="3">
+        <v>68</v>
+      </c>
+      <c r="F68" s="3" t="s">
+        <v>129</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I56">
+  <autoFilter ref="A1:I66">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Issue #68 when updating config need to reload playlist
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$66</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$68</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="130">
   <si>
     <t>#</t>
   </si>
@@ -892,11 +892,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I68"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
@@ -939,7 +938,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -956,7 +955,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -979,7 +978,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1002,7 +1001,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1019,7 +1018,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1036,7 +1035,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1056,7 +1055,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1073,7 +1072,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1093,7 +1092,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1107,7 +1106,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1127,7 +1126,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1144,7 +1143,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1161,7 +1160,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1178,7 +1177,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>44</v>
       </c>
@@ -1198,7 +1197,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1215,7 +1214,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1232,7 +1231,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1249,7 +1248,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1263,7 +1262,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1280,7 +1279,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1297,7 +1296,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1317,7 +1316,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1334,7 +1333,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>24</v>
       </c>
@@ -1382,7 +1381,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>27</v>
       </c>
@@ -1402,7 +1401,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>28</v>
       </c>
@@ -1419,7 +1418,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>29</v>
       </c>
@@ -1433,7 +1432,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>30</v>
       </c>
@@ -1447,7 +1446,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>31</v>
       </c>
@@ -1464,7 +1463,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>32</v>
       </c>
@@ -1495,7 +1494,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -1512,7 +1511,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>35</v>
       </c>
@@ -1529,7 +1528,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>36</v>
       </c>
@@ -1546,7 +1545,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>37</v>
       </c>
@@ -1566,7 +1565,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>38</v>
       </c>
@@ -1611,7 +1610,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>41</v>
       </c>
@@ -1625,7 +1624,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>42</v>
       </c>
@@ -1673,7 +1672,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>45</v>
       </c>
@@ -1690,7 +1689,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>46</v>
       </c>
@@ -1721,7 +1720,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>48</v>
       </c>
@@ -1766,7 +1765,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>51</v>
       </c>
@@ -1786,7 +1785,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>52</v>
       </c>
@@ -1806,7 +1805,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>53</v>
       </c>
@@ -1826,7 +1825,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>54</v>
       </c>
@@ -1849,7 +1848,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>55</v>
       </c>
@@ -1886,7 +1885,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>57</v>
       </c>
@@ -1944,7 +1943,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>62</v>
       </c>
@@ -1980,7 +1979,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>65</v>
       </c>
@@ -1991,7 +1990,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>66</v>
       </c>
@@ -2014,15 +2013,15 @@
       <c r="A68" s="3">
         <v>68</v>
       </c>
+      <c r="D68" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="F68" s="3" t="s">
         <v>129</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I66">
-    <filterColumn colId="3">
-      <filters blank="1"/>
-    </filterColumn>
+  <autoFilter ref="A1:I68">
     <sortState ref="A3:I44">
       <sortCondition ref="C2:C44"/>
     </sortState>

</xml_diff>

<commit_message>
Issue #63 emulator to share same server as main
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="138">
   <si>
     <t>#</t>
   </si>
@@ -217,9 +217,6 @@
   </si>
   <si>
     <t>slide transistion</t>
-  </si>
-  <si>
-    <t>Better error handling when REST server not available</t>
   </si>
   <si>
     <t>Hearbeat</t>
@@ -313,10 +310,6 @@
     <t>encapsulate playlist into a model and protect the data</t>
   </si>
   <si>
-    <t>There is a better approach but this is not done everyhwere yet.  This still needs to be done for the repo fetches of data
-It is kind of obvious as there is no data … and there is the settings option to test connectivity</t>
-  </si>
-  <si>
     <t>Server side handling for config</t>
   </si>
   <si>
@@ -422,6 +415,38 @@
   </si>
   <si>
     <t>when updating config need to reload playlist</t>
+  </si>
+  <si>
+    <t>need a way to kill and restart server from browser . this is covered by the move to the new model</t>
+  </si>
+  <si>
+    <t>Better error handling when REST server not availableThere is a better approach but this is not done everyhwere yet.  
+This still needs to be done for the repo fetches of data
+It is kind of obvious as there is no data … and there is the settings option to test connectivity</t>
+  </si>
+  <si>
+    <t>REST error handline</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Playlist Folders</t>
+  </si>
+  <si>
+    <t>Size/brightness per image</t>
+  </si>
+  <si>
+    <t>hamburger bug</t>
+  </si>
+  <si>
+    <t>uniform message handling</t>
+  </si>
+  <si>
+    <t>covered by playlist model</t>
+  </si>
+  <si>
+    <t>add image should only show one select all remove all button at a time</t>
   </si>
 </sst>
 </file>
@@ -892,11 +917,12 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I68"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:I70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A54" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D68" sqref="D68"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E78" sqref="E78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -905,7 +931,7 @@
     <col min="6" max="6" width="22.81640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="10" style="3" customWidth="1"/>
     <col min="8" max="8" width="15.6328125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="50.6328125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="101.90625" style="3" customWidth="1"/>
     <col min="10" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
@@ -914,7 +940,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>51</v>
@@ -926,7 +952,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>1</v>
+        <v>131</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>47</v>
@@ -938,7 +964,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -949,13 +975,13 @@
         <v>24</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -978,7 +1004,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1001,7 +1027,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1018,7 +1044,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1035,7 +1061,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1055,7 +1081,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1072,7 +1098,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1092,7 +1118,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1106,7 +1132,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1126,7 +1152,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1143,7 +1169,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1160,7 +1186,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1174,10 +1200,10 @@
         <v>24</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>44</v>
       </c>
@@ -1188,16 +1214,16 @@
         <v>24</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H15" s="3" t="s">
         <v>14</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1214,7 +1240,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1231,7 +1257,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1248,7 +1274,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1262,7 +1288,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1279,7 +1305,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1296,7 +1322,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1316,7 +1342,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1333,7 +1359,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>24</v>
       </c>
@@ -1353,7 +1379,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="72.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>26</v>
       </c>
@@ -1361,13 +1387,13 @@
         <v>3</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>63</v>
+        <v>130</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>94</v>
+        <v>129</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -1378,10 +1404,10 @@
         <v>3</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>27</v>
       </c>
@@ -1389,19 +1415,19 @@
         <v>1</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G27" s="3">
         <v>35</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>28</v>
       </c>
@@ -1412,13 +1438,13 @@
         <v>24</v>
       </c>
       <c r="F28" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I28" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I28" s="3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="29" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>29</v>
       </c>
@@ -1429,10 +1455,10 @@
         <v>24</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>30</v>
       </c>
@@ -1443,10 +1469,10 @@
         <v>24</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>31</v>
       </c>
@@ -1457,13 +1483,13 @@
         <v>24</v>
       </c>
       <c r="E31" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="32" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="32" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>32</v>
       </c>
@@ -1471,30 +1497,33 @@
         <v>3</v>
       </c>
       <c r="D32" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F32" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I32" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="33" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>39</v>
       </c>
       <c r="C33" s="3">
         <v>3</v>
       </c>
+      <c r="D33" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="F33" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -1505,13 +1534,13 @@
         <v>24</v>
       </c>
       <c r="F34" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="I34" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="I34" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>35</v>
       </c>
@@ -1522,13 +1551,13 @@
         <v>24</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>36</v>
       </c>
@@ -1539,13 +1568,13 @@
         <v>24</v>
       </c>
       <c r="F36" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="I36" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="I36" s="3" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    </row>
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>37</v>
       </c>
@@ -1556,16 +1585,16 @@
         <v>24</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G37" s="3">
         <v>37</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>38</v>
       </c>
@@ -1576,24 +1605,27 @@
         <v>24</v>
       </c>
       <c r="E38" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F38" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F38" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>43</v>
       </c>
       <c r="C39" s="3">
         <v>2</v>
       </c>
+      <c r="D39" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="F39" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="I39" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="I39" s="3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.35">
@@ -1603,14 +1635,17 @@
       <c r="C40" s="3">
         <v>5</v>
       </c>
+      <c r="F40" s="3" t="s">
+        <v>132</v>
+      </c>
       <c r="H40" s="3" t="s">
         <v>6</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>41</v>
       </c>
@@ -1621,10 +1656,10 @@
         <v>24</v>
       </c>
       <c r="F41" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="42" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>42</v>
       </c>
@@ -1635,10 +1670,10 @@
         <v>24</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.35">
@@ -1666,13 +1701,16 @@
         <v>5</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>45</v>
       </c>
@@ -1683,13 +1721,13 @@
         <v>24</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>46</v>
       </c>
@@ -1700,10 +1738,10 @@
         <v>24</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F46" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.35">
@@ -1714,13 +1752,13 @@
         <v>3</v>
       </c>
       <c r="E47" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>48</v>
       </c>
@@ -1731,10 +1769,10 @@
         <v>24</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="F48" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.35">
@@ -1748,7 +1786,7 @@
         <v>31</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
@@ -1759,13 +1797,13 @@
         <v>3</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>51</v>
       </c>
@@ -1779,13 +1817,13 @@
         <v>24</v>
       </c>
       <c r="F51" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H51" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>52</v>
       </c>
@@ -1796,16 +1834,16 @@
         <v>24</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H52" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>53</v>
       </c>
@@ -1816,16 +1854,16 @@
         <v>24</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F53" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H53" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>54</v>
       </c>
@@ -1839,16 +1877,16 @@
         <v>24</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H54" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>55</v>
       </c>
@@ -1859,16 +1897,16 @@
         <v>24</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F55" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H55" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>56</v>
       </c>
@@ -1879,13 +1917,13 @@
         <v>24</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>57</v>
       </c>
@@ -1896,10 +1934,10 @@
         <v>31</v>
       </c>
       <c r="F57" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>58</v>
       </c>
@@ -1907,32 +1945,44 @@
         <v>2</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>116</v>
+        <v>135</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>59</v>
       </c>
+      <c r="D59" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="F59" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>60</v>
       </c>
+      <c r="C60" s="3">
+        <v>5</v>
+      </c>
       <c r="E60" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -1940,10 +1990,10 @@
         <v>61</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>62</v>
       </c>
@@ -1951,35 +2001,44 @@
         <v>24</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>63</v>
       </c>
+      <c r="C63" s="3">
+        <v>1</v>
+      </c>
+      <c r="D63" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E63" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="F63" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="I63" s="3" t="s">
         <v>122</v>
-      </c>
-      <c r="F63" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="I63" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>64</v>
       </c>
+      <c r="C64" s="3">
+        <v>3</v>
+      </c>
       <c r="F64" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>65</v>
       </c>
@@ -1987,10 +2046,10 @@
         <v>24</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>66</v>
       </c>
@@ -1998,18 +2057,21 @@
         <v>24</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>67</v>
       </c>
+      <c r="C67" s="3">
+        <v>2</v>
+      </c>
       <c r="F67" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="29" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>68</v>
       </c>
@@ -2017,11 +2079,39 @@
         <v>24</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A69" s="3">
+        <v>69</v>
+      </c>
+      <c r="C69" s="3">
+        <v>5</v>
+      </c>
+      <c r="F69" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A70" s="3">
+        <v>70</v>
+      </c>
+      <c r="C70" s="3">
+        <v>3</v>
+      </c>
+      <c r="F70" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I70" s="3" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:I68">
+    <filterColumn colId="3">
+      <filters blank="1"/>
+    </filterColumn>
     <sortState ref="A3:I44">
       <sortCondition ref="C2:C44"/>
     </sortState>

</xml_diff>

<commit_message>
Issue #71 use new model
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$68</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$70</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="141">
   <si>
     <t>#</t>
   </si>
@@ -378,10 +378,6 @@
   </si>
   <si>
     <t>should add message when navigating away from playlist and playlist needs saving</t>
-  </si>
-  <si>
-    <t>import { Observable } from 'rxjs/Observable';
-import 'rxjs/add/observable/of';</t>
   </si>
   <si>
     <t>of</t>
@@ -425,9 +421,6 @@
 It is kind of obvious as there is no data … and there is the settings option to test connectivity</t>
   </si>
   <si>
-    <t>REST error handline</t>
-  </si>
-  <si>
     <t>Title</t>
   </si>
   <si>
@@ -447,6 +440,23 @@
   </si>
   <si>
     <t>add image should only show one select all remove all button at a time</t>
+  </si>
+  <si>
+    <t>import { Observable } from 'rxjs/Observable';
+import 'rxjs/add/observable/of';
+Couldn’t get this to work easily … closing it to cut down noise</t>
+  </si>
+  <si>
+    <t>REST error handling</t>
+  </si>
+  <si>
+    <t>moveup and move down of tracks should take advantage of the new model</t>
+  </si>
+  <si>
+    <t>use new model</t>
+  </si>
+  <si>
+    <t>Edit playlist starts dirty</t>
   </si>
 </sst>
 </file>
@@ -918,11 +928,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I70"/>
+  <dimension ref="A1:I72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E78" sqref="E78"/>
+      <selection pane="bottomLeft" activeCell="E79" sqref="E79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -952,7 +962,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>47</v>
@@ -964,7 +974,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -981,7 +991,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1004,7 +1014,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1027,7 +1037,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1288,7 +1298,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1342,7 +1352,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1387,13 +1397,13 @@
         <v>3</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="H25" s="3" t="s">
         <v>99</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
@@ -1407,7 +1417,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>27</v>
       </c>
@@ -1427,7 +1437,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>28</v>
       </c>
@@ -1520,7 +1530,7 @@
         <v>83</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -1636,7 +1646,7 @@
         <v>5</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H40" s="3" t="s">
         <v>6</v>
@@ -1704,7 +1714,7 @@
         <v>85</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="I44" s="3" t="s">
         <v>84</v>
@@ -1948,13 +1958,13 @@
         <v>68</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="I58" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>59</v>
       </c>
@@ -1965,24 +1975,27 @@
         <v>115</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>60</v>
       </c>
       <c r="C60" s="3">
         <v>5</v>
       </c>
+      <c r="D60" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="E60" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F60" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -1990,7 +2003,7 @@
         <v>61</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2004,10 +2017,10 @@
         <v>68</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="63" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>63</v>
       </c>
@@ -2018,13 +2031,13 @@
         <v>24</v>
       </c>
       <c r="E63" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="F63" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="F63" s="3" t="s">
+      <c r="I63" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="I63" s="3" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
@@ -2035,7 +2048,7 @@
         <v>3</v>
       </c>
       <c r="F64" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2046,7 +2059,7 @@
         <v>24</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2057,7 +2070,7 @@
         <v>24</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
@@ -2065,10 +2078,10 @@
         <v>67</v>
       </c>
       <c r="C67" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2079,7 +2092,7 @@
         <v>24</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.35">
@@ -2090,7 +2103,10 @@
         <v>5</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
@@ -2104,11 +2120,39 @@
         <v>31</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A71" s="3">
+        <v>71</v>
+      </c>
+      <c r="C71" s="3">
+        <v>1</v>
+      </c>
+      <c r="D71" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F71" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="I71" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A72" s="3">
+        <v>72</v>
+      </c>
+      <c r="C72" s="3">
+        <v>1</v>
+      </c>
+      <c r="F72" s="3" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I68">
+  <autoFilter ref="A1:I70">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Issue #58 uniform ui message handling
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$70</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$75</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="149">
   <si>
     <t>#</t>
   </si>
@@ -457,6 +457,30 @@
   </si>
   <si>
     <t>Edit playlist starts dirty</t>
+  </si>
+  <si>
+    <t>Playlist names should not have .json</t>
+  </si>
+  <si>
+    <t>PENDING</t>
+  </si>
+  <si>
+    <t>This is not the case</t>
+  </si>
+  <si>
+    <t>Should not be able to navigate from Edit Playlist and have Playlist dirty</t>
+  </si>
+  <si>
+    <t>Refetch playlist from server</t>
+  </si>
+  <si>
+    <t>AWAIT TEST</t>
+  </si>
+  <si>
+    <t>Add selected tracks does not mark playlist as dirty</t>
+  </si>
+  <si>
+    <t>BUT</t>
   </si>
 </sst>
 </file>
@@ -928,11 +952,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I72"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E79" sqref="E79"/>
+      <selection pane="bottomLeft" activeCell="D47" sqref="D47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1391,30 +1415,33 @@
     </row>
     <row r="25" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="C25" s="3">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>146</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
+        <v>70</v>
+      </c>
+      <c r="C26" s="3">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C26" s="3">
-        <v>3</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>70</v>
+      <c r="I26" s="3" t="s">
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1638,21 +1665,21 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
-        <v>14</v>
+        <v>72</v>
       </c>
       <c r="C40" s="3">
-        <v>5</v>
+        <v>1</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>94</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H40" s="3" t="s">
-        <v>6</v>
+        <v>140</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1686,38 +1713,26 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
-        <v>25</v>
+        <v>74</v>
       </c>
       <c r="C43" s="3">
-        <v>5</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>31</v>
+        <v>1</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="I43" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="C44" s="3">
-        <v>5</v>
-      </c>
-      <c r="E44" s="3" t="s">
-        <v>85</v>
+        <v>1</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="I44" s="3" t="s">
-        <v>84</v>
+        <v>145</v>
       </c>
     </row>
     <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -1754,18 +1769,24 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C47" s="3">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>101</v>
+        <v>133</v>
+      </c>
+      <c r="I47" s="3" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -1785,32 +1806,32 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
-        <v>49</v>
+        <v>26</v>
       </c>
       <c r="C49" s="3">
         <v>3</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="F49" s="3" t="s">
-        <v>103</v>
+        <v>137</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="I49" s="3" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="C50" s="3">
         <v>3</v>
       </c>
-      <c r="E50" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="F50" s="3" t="s">
-        <v>104</v>
+        <v>70</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1947,21 +1968,18 @@
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C58" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E58" s="3" t="s">
         <v>68</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="I58" s="3" t="s">
-        <v>114</v>
+        <v>101</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="58" hidden="1" x14ac:dyDescent="0.35">
@@ -1998,12 +2016,18 @@
         <v>136</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
-        <v>61</v>
+        <v>49</v>
+      </c>
+      <c r="C61" s="3">
+        <v>3</v>
+      </c>
+      <c r="E61" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
     </row>
     <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2042,13 +2066,16 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="C64" s="3">
         <v>3</v>
       </c>
+      <c r="E64" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="F64" s="3" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
     </row>
     <row r="65" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2073,15 +2100,15 @@
         <v>124</v>
       </c>
     </row>
-    <row r="67" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="C67" s="3">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F67" s="3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2095,35 +2122,35 @@
         <v>126</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C69" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="H69" s="3" t="s">
-        <v>6</v>
+        <v>141</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="C70" s="3">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="E70" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>31</v>
+        <v>132</v>
       </c>
       <c r="I70" s="3" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>71</v>
       </c>
@@ -2142,24 +2169,88 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
-        <v>72</v>
+        <v>14</v>
       </c>
       <c r="C72" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>140</v>
+        <v>130</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A73" s="3">
+        <v>25</v>
+      </c>
+      <c r="C73" s="3">
+        <v>5</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F73" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I73" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A74" s="3">
+        <v>69</v>
+      </c>
+      <c r="C74" s="3">
+        <v>5</v>
+      </c>
+      <c r="F74" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A75" s="3">
+        <v>61</v>
+      </c>
+      <c r="F75" s="3" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A76" s="3">
+        <v>76</v>
+      </c>
+      <c r="C76" s="3">
+        <v>1</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I70">
+  <autoFilter ref="A1:I75">
     <filterColumn colId="3">
-      <filters blank="1"/>
+      <filters blank="1">
+        <filter val="PENDING"/>
+      </filters>
     </filterColumn>
-    <sortState ref="A3:I44">
-      <sortCondition ref="C2:C44"/>
+    <sortState ref="A25:I73">
+      <sortCondition ref="C2:C73"/>
     </sortState>
   </autoFilter>
+  <sortState ref="A25:I75">
+    <sortCondition ref="C2:C75"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Issue #76 Adding track does not mark playlist as dirty
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="149">
   <si>
     <t>#</t>
   </si>
@@ -956,7 +956,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D47" sqref="D47"/>
+      <selection pane="bottomLeft" activeCell="F80" sqref="F80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2229,6 +2229,9 @@
       </c>
       <c r="C76" s="3">
         <v>1</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>148</v>

</xml_diff>

<commit_message>
Issue #67 debonce server config changes
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$76</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="150">
   <si>
     <t>#</t>
   </si>
@@ -474,13 +474,16 @@
     <t>Refetch playlist from server</t>
   </si>
   <si>
-    <t>AWAIT TEST</t>
-  </si>
-  <si>
     <t>Add selected tracks does not mark playlist as dirty</t>
   </si>
   <si>
     <t>BUT</t>
+  </si>
+  <si>
+    <t>duplicate track from edit playlist screen</t>
+  </si>
+  <si>
+    <t>Config issues stopping ng build</t>
   </si>
 </sst>
 </file>
@@ -952,11 +955,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I76"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F80" sqref="F80"/>
+      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1421,7 +1424,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>146</v>
+        <v>24</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>125</v>
@@ -1769,7 +1772,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>58</v>
       </c>
@@ -2223,7 +2226,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>76</v>
       </c>
@@ -2234,16 +2237,39 @@
         <v>24</v>
       </c>
       <c r="E76" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F76" s="3" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A77" s="3">
+        <v>77</v>
+      </c>
+      <c r="C77" s="3">
+        <v>5</v>
+      </c>
+      <c r="F77" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="F76" s="3" t="s">
-        <v>147</v>
+    </row>
+    <row r="78" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A78" s="3">
+        <v>78</v>
+      </c>
+      <c r="C78" s="3">
+        <v>1</v>
+      </c>
+      <c r="F78" s="3" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I75">
+  <autoFilter ref="A1:I76">
     <filterColumn colId="3">
       <filters blank="1">
+        <filter val="AWAIT TEST"/>
         <filter val="PENDING"/>
       </filters>
     </filterColumn>

</xml_diff>

<commit_message>
Issue #50 run on port 80
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$76</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$78</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="155">
   <si>
     <t>#</t>
   </si>
@@ -484,6 +484,21 @@
   </si>
   <si>
     <t>Config issues stopping ng build</t>
+  </si>
+  <si>
+    <t>display name should have * from model</t>
+  </si>
+  <si>
+    <t>client side logging</t>
+  </si>
+  <si>
+    <t>server side logging</t>
+  </si>
+  <si>
+    <t>use node debug</t>
+  </si>
+  <si>
+    <t>use ngx-logger</t>
   </si>
 </sst>
 </file>
@@ -955,11 +970,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I78"/>
+  <dimension ref="A1:I81"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomLeft" activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1416,7 +1431,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>67</v>
       </c>
@@ -2254,22 +2269,57 @@
         <v>148</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>78</v>
       </c>
       <c r="C78" s="3">
         <v>1</v>
       </c>
+      <c r="D78" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="F78" s="3" t="s">
         <v>149</v>
       </c>
     </row>
+    <row r="79" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A79" s="3">
+        <v>79</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F79" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A80" s="3">
+        <v>80</v>
+      </c>
+      <c r="F80" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="I80" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A81" s="3">
+        <v>81</v>
+      </c>
+      <c r="F81" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="I81" s="3" t="s">
+        <v>153</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I76">
+  <autoFilter ref="A1:I78">
     <filterColumn colId="3">
       <filters blank="1">
-        <filter val="AWAIT TEST"/>
         <filter val="PENDING"/>
       </filters>
     </filterColumn>

</xml_diff>

<commit_message>
Issue #83 upgrade to fontawesome 5
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10700" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="11770" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$78</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$81</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="166">
   <si>
     <t>#</t>
   </si>
@@ -389,6 +389,9 @@
     <t>playlist model</t>
   </si>
   <si>
+    <t>arc</t>
+  </si>
+  <si>
     <t xml:space="preserve">arch </t>
   </si>
   <si>
@@ -414,11 +417,6 @@
   </si>
   <si>
     <t>need a way to kill and restart server from browser . this is covered by the move to the new model</t>
-  </si>
-  <si>
-    <t>Better error handling when REST server not availableThere is a better approach but this is not done everyhwere yet.  
-This still needs to be done for the repo fetches of data
-It is kind of obvious as there is no data … and there is the settings option to test connectivity</t>
   </si>
   <si>
     <t>Title</t>
@@ -499,6 +497,44 @@
   </si>
   <si>
     <t>use ngx-logger</t>
+  </si>
+  <si>
+    <t>The browse list makes it clear that it is not saved</t>
+  </si>
+  <si>
+    <t>Duplicate of 80</t>
+  </si>
+  <si>
+    <t>not erally sure what this refers to anymore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">feature </t>
+  </si>
+  <si>
+    <t>Better error handling when REST server not availableThere is a better approach but this is not done everyhwere yet.  
+This still needs to be done for the repo fetches of data
+It is kind of obvious as there is no data … and there is the settings option to test connectivity
+Makes sens to add this when going over the code putting in logging</t>
+  </si>
+  <si>
+    <t>see https://expressjs.com/en/starter/faq.html on 404
+and https://expressjs.com/en/4x/api.html under static and fallthrough
+and https://stackoverflow.com/questions/9321027/how-to-send-files-with-node-js for sending file</t>
+  </si>
+  <si>
+    <t>make models and mappers angular services (DTOs should be fine) if that makes sense</t>
+  </si>
+  <si>
+    <t>angualize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fortawesome </t>
+  </si>
+  <si>
+    <t>upgrade font awesome to v5</t>
+  </si>
+  <si>
+    <t>see 83</t>
   </si>
 </sst>
 </file>
@@ -970,16 +1006,17 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I81"/>
+  <dimension ref="A1:I83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E86" sqref="E86"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G49" sqref="G49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="5" width="8.7265625" style="3"/>
+    <col min="1" max="4" width="8.7265625" style="3"/>
+    <col min="5" max="5" width="19.7265625" style="3" customWidth="1"/>
     <col min="6" max="6" width="22.81640625" style="3" customWidth="1"/>
     <col min="7" max="7" width="10" style="3" customWidth="1"/>
     <col min="8" max="8" width="15.6328125" style="3" customWidth="1"/>
@@ -1442,10 +1479,10 @@
         <v>24</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>70</v>
       </c>
@@ -1575,7 +1612,7 @@
         <v>83</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -1731,15 +1768,21 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>74</v>
       </c>
       <c r="C43" s="3">
         <v>1</v>
       </c>
+      <c r="D43" s="3" t="s">
+        <v>142</v>
+      </c>
       <c r="F43" s="3" t="s">
         <v>144</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -1824,32 +1867,38 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="C49" s="3">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H49" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="I49" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+        <v>148</v>
+      </c>
+      <c r="G49" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C50" s="3">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="F50" s="3" t="s">
-        <v>70</v>
+        <v>101</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1988,16 +2037,22 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
-        <v>47</v>
+        <v>80</v>
       </c>
       <c r="C58" s="3">
         <v>3</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>68</v>
+        <v>119</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>101</v>
+        <v>151</v>
+      </c>
+      <c r="G58" s="3">
+        <v>26</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="58" hidden="1" x14ac:dyDescent="0.35">
@@ -2034,12 +2089,15 @@
         <v>136</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>49</v>
       </c>
       <c r="C61" s="3">
         <v>3</v>
+      </c>
+      <c r="D61" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>31</v>
@@ -2073,21 +2131,24 @@
         <v>24</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>50</v>
       </c>
       <c r="C64" s="3">
         <v>3</v>
+      </c>
+      <c r="D64" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>68</v>
@@ -2104,7 +2165,7 @@
         <v>24</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
     </row>
     <row r="66" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2115,18 +2176,24 @@
         <v>24</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>64</v>
       </c>
       <c r="C67" s="3">
         <v>3</v>
       </c>
+      <c r="D67" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="F67" s="3" t="s">
-        <v>122</v>
+        <v>123</v>
+      </c>
+      <c r="I67" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2137,18 +2204,24 @@
         <v>24</v>
       </c>
       <c r="F68" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C69" s="3">
         <v>3</v>
       </c>
+      <c r="E69" s="3" t="s">
+        <v>119</v>
+      </c>
       <c r="F69" s="3" t="s">
-        <v>141</v>
+        <v>152</v>
+      </c>
+      <c r="I69" s="3" t="s">
+        <v>153</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.35">
@@ -2187,58 +2260,64 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C72" s="3">
         <v>5</v>
       </c>
+      <c r="E72" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="F72" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H72" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I72" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="C73" s="3">
         <v>5</v>
       </c>
-      <c r="E73" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="F73" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="I73" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+        <v>141</v>
+      </c>
+      <c r="H73" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="C74" s="3">
         <v>5</v>
       </c>
+      <c r="E74" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="F74" s="3" t="s">
-        <v>131</v>
+        <v>137</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="75" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="I74" s="3" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>61</v>
       </c>
+      <c r="D75" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="F75" s="3" t="s">
         <v>117</v>
+      </c>
+      <c r="I75" s="3" t="s">
+        <v>157</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2258,15 +2337,21 @@
         <v>146</v>
       </c>
     </row>
-    <row r="77" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="C77" s="3">
         <v>5</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>148</v>
+        <v>130</v>
+      </c>
+      <c r="H77" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I77" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2283,7 +2368,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>79</v>
       </c>
@@ -2296,39 +2381,71 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
-        <v>80</v>
+        <v>25</v>
+      </c>
+      <c r="C80" s="3">
+        <v>5</v>
+      </c>
+      <c r="E80" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>151</v>
+        <v>62</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>154</v>
+        <v>61</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
-        <v>81</v>
+        <v>69</v>
+      </c>
+      <c r="C81" s="3">
+        <v>5</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="I81" s="3" t="s">
-        <v>153</v>
+        <v>131</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A82" s="3">
+        <v>82</v>
+      </c>
+      <c r="C82" s="3">
+        <v>5</v>
+      </c>
+      <c r="F82" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="I82" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A83" s="3">
+        <v>83</v>
+      </c>
+      <c r="F83" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="I83" s="3" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I78">
+  <autoFilter ref="A1:I81">
     <filterColumn colId="3">
-      <filters blank="1">
-        <filter val="PENDING"/>
-      </filters>
+      <filters blank="1"/>
     </filterColumn>
-    <sortState ref="A25:I73">
-      <sortCondition ref="C2:C73"/>
+    <sortState ref="A44:I81">
+      <sortCondition ref="C2:C81"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A25:I75">
-    <sortCondition ref="C2:C75"/>
+  <sortState ref="A44:I81">
+    <sortCondition ref="C2:C81"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Issue #85 reload does not properly reload playlist
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$85</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="169">
   <si>
     <t>#</t>
   </si>
@@ -517,24 +517,33 @@
 Makes sens to add this when going over the code putting in logging</t>
   </si>
   <si>
+    <t>make models and mappers angular services (DTOs should be fine) if that makes sense</t>
+  </si>
+  <si>
+    <t>angualize</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fortawesome </t>
+  </si>
+  <si>
+    <t>upgrade font awesome to v5</t>
+  </si>
+  <si>
+    <t>see 83</t>
+  </si>
+  <si>
     <t>see https://expressjs.com/en/starter/faq.html on 404
-and https://expressjs.com/en/4x/api.html under static and fallthrough
+and   under static and fallthrough
 and https://stackoverflow.com/questions/9321027/how-to-send-files-with-node-js for sending file</t>
   </si>
   <si>
-    <t>make models and mappers angular services (DTOs should be fine) if that makes sense</t>
-  </si>
-  <si>
-    <t>angualize</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fortawesome </t>
-  </si>
-  <si>
-    <t>upgrade font awesome to v5</t>
-  </si>
-  <si>
-    <t>see 83</t>
+    <t>remove model demo from front screen</t>
+  </si>
+  <si>
+    <t>reload path does not work</t>
+  </si>
+  <si>
+    <t>it loads an empty playlist</t>
   </si>
 </sst>
 </file>
@@ -1006,11 +1015,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I83"/>
+  <dimension ref="A1:I85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G49" sqref="G49"/>
+      <selection pane="bottomLeft" activeCell="E86" sqref="E86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1790,7 +1799,7 @@
         <v>75</v>
       </c>
       <c r="C44" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>145</v>
@@ -1872,7 +1881,7 @@
         <v>77</v>
       </c>
       <c r="C49" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>158</v>
@@ -1881,16 +1890,19 @@
         <v>148</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>47</v>
       </c>
       <c r="C50" s="3">
         <v>1</v>
       </c>
+      <c r="D50" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E50" s="3" t="s">
         <v>68</v>
       </c>
@@ -1898,7 +1910,7 @@
         <v>101</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>160</v>
+        <v>165</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2418,25 +2430,56 @@
         <v>5</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>83</v>
       </c>
+      <c r="D83" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="F83" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="I83" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="I83" s="3" t="s">
-        <v>164</v>
+    </row>
+    <row r="84" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A84" s="3">
+        <v>84</v>
+      </c>
+      <c r="C84" s="3">
+        <v>1</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F84" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A85" s="3">
+        <v>85</v>
+      </c>
+      <c r="C85" s="3">
+        <v>1</v>
+      </c>
+      <c r="F85" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="I85" s="3" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I81">
+  <autoFilter ref="A1:I85">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Issue #86 resolve circular dependency
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="285" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="170">
   <si>
     <t>#</t>
   </si>
@@ -544,6 +544,9 @@
   </si>
   <si>
     <t>it loads an empty playlist</t>
+  </si>
+  <si>
+    <t>resolve cricular build dependency</t>
   </si>
 </sst>
 </file>
@@ -1015,11 +1018,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I85"/>
+  <dimension ref="A1:I86"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E86" sqref="E86"/>
+      <selection pane="bottomLeft" activeCell="D86" sqref="D86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2471,11 +2474,28 @@
       <c r="C85" s="3">
         <v>1</v>
       </c>
+      <c r="D85" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="F85" s="3" t="s">
         <v>167</v>
       </c>
       <c r="I85" s="3" t="s">
         <v>168</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A86" s="3">
+        <v>86</v>
+      </c>
+      <c r="C86" s="3">
+        <v>1</v>
+      </c>
+      <c r="D86" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F86" s="3" t="s">
+        <v>169</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #87  TypeError: Converting circular structure to JSON
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="171">
   <si>
     <t>#</t>
   </si>
@@ -547,6 +547,9 @@
   </si>
   <si>
     <t>resolve cricular build dependency</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> TypeError: Converting circular structure to JSON</t>
   </si>
 </sst>
 </file>
@@ -1018,11 +1021,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I86"/>
+  <dimension ref="A1:I87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D86" sqref="D86"/>
+      <selection pane="bottomLeft" activeCell="F87" sqref="F87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2498,6 +2501,23 @@
         <v>169</v>
       </c>
     </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A87" s="3">
+        <v>87</v>
+      </c>
+      <c r="C87" s="3">
+        <v>1</v>
+      </c>
+      <c r="D87" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F87" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I85">
     <filterColumn colId="3">

</xml_diff>

<commit_message>
Issue #88 demo page not working for serverEmulator
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="291" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="172">
   <si>
     <t>#</t>
   </si>
@@ -550,6 +550,9 @@
   </si>
   <si>
     <t xml:space="preserve"> TypeError: Converting circular structure to JSON</t>
+  </si>
+  <si>
+    <t>demo page not working in server emulator</t>
   </si>
 </sst>
 </file>
@@ -1021,11 +1024,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I87"/>
+  <dimension ref="A1:I88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F87" sqref="F87"/>
+      <selection pane="bottomLeft" activeCell="F98" sqref="F97:F98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2518,6 +2521,23 @@
         <v>170</v>
       </c>
     </row>
+    <row r="88" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A88" s="3">
+        <v>88</v>
+      </c>
+      <c r="C88" s="3">
+        <v>1</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E88" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="F88" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I85">
     <filterColumn colId="3">

</xml_diff>

<commit_message>
Issue #93 header not displaying properly on small screens
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="11770" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="12840" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$85</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$88</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="177">
   <si>
     <t>#</t>
   </si>
@@ -553,6 +553,21 @@
   </si>
   <si>
     <t>demo page not working in server emulator</t>
+  </si>
+  <si>
+    <t>use material design</t>
+  </si>
+  <si>
+    <t>visual acknowledgement of startup</t>
+  </si>
+  <si>
+    <t>auto startup</t>
+  </si>
+  <si>
+    <t>Test button in setting text too long</t>
+  </si>
+  <si>
+    <t>Nav bar not displaying proplerly on Samsung S7 edge</t>
   </si>
 </sst>
 </file>
@@ -1024,11 +1039,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I88"/>
+  <dimension ref="A1:I93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F98" sqref="F97:F98"/>
+      <selection pane="bottomLeft" activeCell="H103" sqref="H103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1805,13 +1820,13 @@
     </row>
     <row r="44" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="C44" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
     </row>
     <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -1885,21 +1900,15 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
-        <v>77</v>
+        <v>91</v>
       </c>
       <c r="C49" s="3">
-        <v>2</v>
-      </c>
-      <c r="E49" s="3" t="s">
-        <v>158</v>
+        <v>1</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="G49" s="3" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
@@ -2056,24 +2065,15 @@
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="C58" s="3">
-        <v>3</v>
-      </c>
-      <c r="E58" s="3" t="s">
-        <v>119</v>
+        <v>1</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="G58" s="3">
-        <v>26</v>
-      </c>
-      <c r="I58" s="3" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="58" hidden="1" x14ac:dyDescent="0.35">
@@ -2228,38 +2228,26 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="C69" s="3">
-        <v>3</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>119</v>
+        <v>1</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="I69" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
-        <v>40</v>
+        <v>75</v>
       </c>
       <c r="C70" s="3">
-        <v>4</v>
-      </c>
-      <c r="E70" s="3" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="I70" s="3" t="s">
-        <v>84</v>
+        <v>145</v>
       </c>
     </row>
     <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2279,52 +2267,58 @@
         <v>138</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
-        <v>31</v>
+        <v>77</v>
       </c>
       <c r="C72" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>68</v>
+        <v>158</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>148</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="C73" s="3">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="E73" s="3" t="s">
+        <v>119</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="H73" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+        <v>151</v>
+      </c>
+      <c r="G73" s="3">
+        <v>26</v>
+      </c>
+      <c r="I73" s="3" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
-        <v>26</v>
+        <v>81</v>
       </c>
       <c r="C74" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>68</v>
+        <v>119</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H74" s="3" t="s">
-        <v>99</v>
+        <v>152</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2360,19 +2354,19 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="C77" s="3">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="E77" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H77" s="3" t="s">
-        <v>6</v>
+        <v>132</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2402,47 +2396,50 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C80" s="3">
         <v>5</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="I80" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C81" s="3">
         <v>5</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
       <c r="H81" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
-        <v>82</v>
+        <v>26</v>
       </c>
       <c r="C82" s="3">
         <v>5</v>
       </c>
+      <c r="E82" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="F82" s="3" t="s">
-        <v>161</v>
+        <v>137</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2459,7 +2456,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>84</v>
       </c>
@@ -2473,7 +2470,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="3">
         <v>85</v>
       </c>
@@ -2490,7 +2487,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="3">
         <v>86</v>
       </c>
@@ -2504,7 +2501,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="3">
         <v>87</v>
       </c>
@@ -2521,7 +2518,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="3">
         <v>88</v>
       </c>
@@ -2538,8 +2535,84 @@
         <v>171</v>
       </c>
     </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A89" s="3">
+        <v>14</v>
+      </c>
+      <c r="C89" s="3">
+        <v>5</v>
+      </c>
+      <c r="F89" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I89" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A90" s="3">
+        <v>25</v>
+      </c>
+      <c r="C90" s="3">
+        <v>5</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F90" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A91" s="3">
+        <v>69</v>
+      </c>
+      <c r="C91" s="3">
+        <v>5</v>
+      </c>
+      <c r="F91" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="H91" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A92" s="3">
+        <v>82</v>
+      </c>
+      <c r="C92" s="3">
+        <v>5</v>
+      </c>
+      <c r="F92" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I92" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A93" s="3">
+        <v>89</v>
+      </c>
+      <c r="C93" s="3">
+        <v>5</v>
+      </c>
+      <c r="D93" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="F93" s="3" t="s">
+        <v>172</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I85">
+  <autoFilter ref="A1:I88">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
@@ -2547,8 +2620,8 @@
       <sortCondition ref="C2:C81"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A44:I81">
-    <sortCondition ref="C2:C81"/>
+  <sortState ref="A44:I93">
+    <sortCondition ref="C2:C93"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Issue #92 Test button in setting text too long
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="177">
   <si>
     <t>#</t>
   </si>
@@ -1043,7 +1043,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H103" sqref="H103"/>
+      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2072,6 +2072,9 @@
       <c r="C58" s="3">
         <v>1</v>
       </c>
+      <c r="D58" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="F58" s="3" t="s">
         <v>175</v>
       </c>
@@ -2234,6 +2237,9 @@
       </c>
       <c r="C69" s="3">
         <v>1</v>
+      </c>
+      <c r="D69" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="F69" s="3" t="s">
         <v>176</v>

</xml_diff>

<commit_message>
Issue #90 visual acknowledgement of startup
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="177">
   <si>
     <t>#</t>
   </si>
@@ -1043,7 +1043,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D58" sqref="D58"/>
+      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1825,6 +1825,9 @@
       <c r="C44" s="3">
         <v>1</v>
       </c>
+      <c r="D44" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="F44" s="3" t="s">
         <v>173</v>
       </c>

</xml_diff>

<commit_message>
Issue #94 track icons squashed on small screen
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="178">
   <si>
     <t>#</t>
   </si>
@@ -568,6 +568,9 @@
   </si>
   <si>
     <t>Nav bar not displaying proplerly on Samsung S7 edge</t>
+  </si>
+  <si>
+    <t>track icons squashed on small screen</t>
   </si>
 </sst>
 </file>
@@ -1039,11 +1042,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I93"/>
+  <dimension ref="A1:I94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F44" sqref="F44"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2620,6 +2623,20 @@
         <v>172</v>
       </c>
     </row>
+    <row r="94" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A94" s="3">
+        <v>94</v>
+      </c>
+      <c r="C94" s="3">
+        <v>1</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F94" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I88">
     <filterColumn colId="3">

</xml_diff>

<commit_message>
Issue #91 auto startup and restart
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="179">
   <si>
     <t>#</t>
   </si>
@@ -571,6 +571,9 @@
   </si>
   <si>
     <t>track icons squashed on small screen</t>
+  </si>
+  <si>
+    <t>autostartup in rc.local</t>
   </si>
 </sst>
 </file>
@@ -1042,11 +1045,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I94"/>
+  <dimension ref="A1:I95"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F94" sqref="F94"/>
+      <selection pane="bottomLeft" activeCell="E105" sqref="E105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1913,6 +1916,9 @@
       <c r="C49" s="3">
         <v>1</v>
       </c>
+      <c r="D49" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="F49" s="3" t="s">
         <v>174</v>
       </c>
@@ -2635,6 +2641,17 @@
       </c>
       <c r="F94" s="3" t="s">
         <v>177</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A95" s="3">
+        <v>95</v>
+      </c>
+      <c r="C95" s="3">
+        <v>2</v>
+      </c>
+      <c r="F95" s="3" t="s">
+        <v>178</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #81 server side looging using npm debug
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="12840" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView minimized="1" xWindow="14980" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$88</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$96</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="191">
   <si>
     <t>#</t>
   </si>
@@ -574,13 +574,49 @@
   </si>
   <si>
     <t>autostartup in rc.local</t>
+  </si>
+  <si>
+    <t>get Release text into client</t>
+  </si>
+  <si>
+    <t>Better place for IssuesLog</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/7783341/run-script-with-rc-local-script-works-but-not-at-boot</t>
+  </si>
+  <si>
+    <t>don’t have std in in daemon</t>
+  </si>
+  <si>
+    <t>faster boot time for r PI</t>
+  </si>
+  <si>
+    <t>On play playlist screen should only show the elements that are enabled</t>
+  </si>
+  <si>
+    <t>rotate and scale images</t>
+  </si>
+  <si>
+    <t>see 25</t>
+  </si>
+  <si>
+    <t>see 101</t>
+  </si>
+  <si>
+    <t>toch drag and drop</t>
+  </si>
+  <si>
+    <t>https://www.w3schools.com/howto/howto_js_rangeslider.asp</t>
+  </si>
+  <si>
+    <t>range sliders for config</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -592,6 +628,14 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -626,10 +670,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -643,8 +688,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1045,11 +1092,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I95"/>
+  <dimension ref="A1:I103"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E105" sqref="E105"/>
+      <selection pane="bottomLeft" activeCell="F104" sqref="F104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1824,7 +1871,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>90</v>
       </c>
@@ -1909,7 +1956,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>91</v>
       </c>
@@ -2077,7 +2124,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>92</v>
       </c>
@@ -2243,7 +2290,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>93</v>
       </c>
@@ -2597,6 +2644,9 @@
       <c r="F91" s="3" t="s">
         <v>131</v>
       </c>
+      <c r="G91" s="3" t="s">
+        <v>187</v>
+      </c>
       <c r="H91" s="3" t="s">
         <v>6</v>
       </c>
@@ -2615,7 +2665,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" s="3">
         <v>89</v>
       </c>
@@ -2629,7 +2679,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="3">
         <v>94</v>
       </c>
@@ -2654,8 +2704,102 @@
         <v>178</v>
       </c>
     </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A96" s="3">
+        <v>96</v>
+      </c>
+      <c r="C96" s="3">
+        <v>2</v>
+      </c>
+      <c r="F96" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A97" s="3">
+        <v>97</v>
+      </c>
+      <c r="C97" s="3">
+        <v>2</v>
+      </c>
+      <c r="F97" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A98" s="3">
+        <v>98</v>
+      </c>
+      <c r="C98" s="3">
+        <v>5</v>
+      </c>
+      <c r="F98" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="I98" s="5" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A99" s="3">
+        <v>99</v>
+      </c>
+      <c r="C99" s="3">
+        <v>1</v>
+      </c>
+      <c r="F99" s="3" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+      <c r="A100" s="3">
+        <v>100</v>
+      </c>
+      <c r="C100" s="3">
+        <v>1</v>
+      </c>
+      <c r="F100" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A101" s="3">
+        <v>101</v>
+      </c>
+      <c r="C101" s="3">
+        <v>2</v>
+      </c>
+      <c r="F101" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A102" s="3">
+        <v>102</v>
+      </c>
+      <c r="C102" s="3">
+        <v>3</v>
+      </c>
+      <c r="F102" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A103" s="3">
+        <v>103</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="I103" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I88">
+  <autoFilter ref="A1:I96">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
@@ -2666,7 +2810,10 @@
   <sortState ref="A44:I93">
     <sortCondition ref="C2:C93"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="I98" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Issue #100 Only display enabled elements on Track screen
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="14980" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="16050" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="193">
   <si>
     <t>#</t>
   </si>
@@ -494,9 +494,6 @@
   </si>
   <si>
     <t>use node debug</t>
-  </si>
-  <si>
-    <t>use ngx-logger</t>
   </si>
   <si>
     <t>The browse list makes it clear that it is not saved</t>
@@ -610,6 +607,15 @@
   </si>
   <si>
     <t>range sliders for config</t>
+  </si>
+  <si>
+    <t>remove repository.service.ts</t>
+  </si>
+  <si>
+    <t>refactor into another component</t>
+  </si>
+  <si>
+    <t>use single quote style in html</t>
   </si>
 </sst>
 </file>
@@ -1092,11 +1098,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I103"/>
+  <dimension ref="A1:I105"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F104" sqref="F104"/>
+      <selection pane="bottomLeft" activeCell="D100" sqref="D100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1868,7 +1874,7 @@
         <v>144</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1882,7 +1888,7 @@
         <v>24</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -1967,7 +1973,7 @@
         <v>24</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
@@ -1987,7 +1993,7 @@
         <v>101</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2135,7 +2141,7 @@
         <v>24</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="58" hidden="1" x14ac:dyDescent="0.35">
@@ -2276,7 +2282,7 @@
         <v>123</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2301,7 +2307,7 @@
         <v>24</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -2340,13 +2346,13 @@
         <v>2</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F72" s="3" t="s">
         <v>148</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.35">
@@ -2356,6 +2362,9 @@
       <c r="C73" s="3">
         <v>3</v>
       </c>
+      <c r="D73" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E73" s="3" t="s">
         <v>119</v>
       </c>
@@ -2366,7 +2375,7 @@
         <v>26</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.35">
@@ -2376,6 +2385,9 @@
       <c r="C74" s="3">
         <v>3</v>
       </c>
+      <c r="D74" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E74" s="3" t="s">
         <v>119</v>
       </c>
@@ -2397,7 +2409,7 @@
         <v>117</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2504,7 +2516,7 @@
         <v>99</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2515,10 +2527,10 @@
         <v>24</v>
       </c>
       <c r="F83" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I83" s="3" t="s">
         <v>162</v>
-      </c>
-      <c r="I83" s="3" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2532,7 +2544,7 @@
         <v>24</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2546,10 +2558,10 @@
         <v>24</v>
       </c>
       <c r="F85" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="I85" s="3" t="s">
         <v>167</v>
-      </c>
-      <c r="I85" s="3" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2563,7 +2575,7 @@
         <v>24</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2580,7 +2592,7 @@
         <v>85</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2597,7 +2609,7 @@
         <v>85</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
@@ -2645,7 +2657,7 @@
         <v>131</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="H91" s="3" t="s">
         <v>6</v>
@@ -2659,10 +2671,10 @@
         <v>5</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2676,7 +2688,7 @@
         <v>142</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2690,7 +2702,7 @@
         <v>24</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.35">
@@ -2701,7 +2713,7 @@
         <v>2</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
@@ -2712,7 +2724,7 @@
         <v>2</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.35">
@@ -2723,7 +2735,7 @@
         <v>2</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -2734,10 +2746,10 @@
         <v>5</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="I98" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
@@ -2748,7 +2760,7 @@
         <v>1</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="100" spans="1:9" ht="58" x14ac:dyDescent="0.35">
@@ -2758,8 +2770,11 @@
       <c r="C100" s="3">
         <v>1</v>
       </c>
+      <c r="D100" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="F100" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
@@ -2770,10 +2785,10 @@
         <v>2</v>
       </c>
       <c r="F101" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="G101" s="3" t="s">
         <v>185</v>
-      </c>
-      <c r="G101" s="3" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.35">
@@ -2784,18 +2799,46 @@
         <v>3</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" s="3">
         <v>103</v>
       </c>
+      <c r="C103" s="3">
+        <v>5</v>
+      </c>
       <c r="F103" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="I103" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A104" s="3">
+        <v>104</v>
+      </c>
+      <c r="C104" s="3">
+        <v>3</v>
+      </c>
+      <c r="F104" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="I103" s="3" t="s">
-        <v>189</v>
+      <c r="I104" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A105" s="3">
+        <v>105</v>
+      </c>
+      <c r="C105" s="3">
+        <v>3</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #95 document restart
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="193">
   <si>
     <t>#</t>
   </si>
@@ -1102,7 +1102,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D100" sqref="D100"/>
+      <selection pane="bottomLeft" activeCell="D92" sqref="D92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2670,6 +2670,9 @@
       <c r="C92" s="3">
         <v>5</v>
       </c>
+      <c r="D92" s="3" t="s">
+        <v>94</v>
+      </c>
       <c r="F92" s="3" t="s">
         <v>160</v>
       </c>
@@ -2711,6 +2714,9 @@
       </c>
       <c r="C95" s="3">
         <v>2</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="F95" s="3" t="s">
         <v>177</v>

</xml_diff>

<commit_message>
Issue #103 final Sliders for config
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$96</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$105</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="195">
   <si>
     <t>#</t>
   </si>
@@ -426,9 +426,6 @@
   </si>
   <si>
     <t>Size/brightness per image</t>
-  </si>
-  <si>
-    <t>hamburger bug</t>
   </si>
   <si>
     <t>uniform message handling</t>
@@ -600,9 +597,6 @@
     <t>see 101</t>
   </si>
   <si>
-    <t>toch drag and drop</t>
-  </si>
-  <si>
     <t>https://www.w3schools.com/howto/howto_js_rangeslider.asp</t>
   </si>
   <si>
@@ -616,6 +610,18 @@
   </si>
   <si>
     <t>use single quote style in html</t>
+  </si>
+  <si>
+    <t>hamburger feature</t>
+  </si>
+  <si>
+    <t>touch drag and drop</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>Config Service should return min, max, value for items</t>
   </si>
 </sst>
 </file>
@@ -680,7 +686,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -695,6 +701,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1098,11 +1107,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I105"/>
+  <dimension ref="A1:I107"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D92" sqref="D92"/>
+      <selection pane="bottomLeft" activeCell="D96" sqref="D96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1582,13 +1591,13 @@
         <v>1</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>31</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1823,10 +1832,10 @@
         <v>94</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1868,13 +1877,13 @@
         <v>1</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1888,7 +1897,7 @@
         <v>24</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -1939,7 +1948,7 @@
         <v>68</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="I47" s="3" t="s">
         <v>114</v>
@@ -1973,7 +1982,7 @@
         <v>24</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
@@ -1993,7 +2002,7 @@
         <v>101</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2141,7 +2150,7 @@
         <v>24</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="58" hidden="1" x14ac:dyDescent="0.35">
@@ -2155,7 +2164,7 @@
         <v>115</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
@@ -2175,7 +2184,7 @@
         <v>116</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2282,7 +2291,7 @@
         <v>123</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2307,18 +2316,24 @@
         <v>24</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C70" s="3">
         <v>2</v>
       </c>
+      <c r="E70" s="3" t="s">
+        <v>156</v>
+      </c>
       <c r="F70" s="3" t="s">
-        <v>145</v>
+        <v>147</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>162</v>
       </c>
     </row>
     <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2332,30 +2347,27 @@
         <v>24</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C72" s="3">
         <v>2</v>
       </c>
-      <c r="E72" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="F72" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="G72" s="3" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+        <v>140</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>80</v>
       </c>
@@ -2369,16 +2381,16 @@
         <v>119</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G73" s="3">
         <v>26</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>81</v>
       </c>
@@ -2392,10 +2404,10 @@
         <v>119</v>
       </c>
       <c r="F74" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="I74" s="3" t="s">
         <v>152</v>
-      </c>
-      <c r="I74" s="3" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2409,7 +2421,7 @@
         <v>117</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2423,27 +2435,27 @@
         <v>24</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
-        <v>40</v>
+        <v>14</v>
       </c>
       <c r="C77" s="3">
-        <v>4</v>
-      </c>
-      <c r="E77" s="3" t="s">
-        <v>85</v>
+        <v>2</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
+      </c>
+      <c r="H77" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>84</v>
+        <v>95</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2457,7 +2469,7 @@
         <v>24</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2468,55 +2480,49 @@
         <v>24</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="C80" s="3">
-        <v>5</v>
-      </c>
-      <c r="E80" s="3" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>131</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="H80" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
-        <v>73</v>
+        <v>101</v>
       </c>
       <c r="C81" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="H81" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+        <v>183</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
-        <v>26</v>
+        <v>75</v>
       </c>
       <c r="C82" s="3">
-        <v>5</v>
-      </c>
-      <c r="E82" s="3" t="s">
-        <v>68</v>
+        <v>3</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="H82" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="I82" s="3" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
     </row>
     <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2527,10 +2533,10 @@
         <v>24</v>
       </c>
       <c r="F83" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="I83" s="3" t="s">
         <v>161</v>
-      </c>
-      <c r="I83" s="3" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2544,7 +2550,7 @@
         <v>24</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2558,10 +2564,10 @@
         <v>24</v>
       </c>
       <c r="F85" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="I85" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="I85" s="3" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2575,7 +2581,7 @@
         <v>24</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2592,7 +2598,7 @@
         <v>85</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2609,61 +2615,55 @@
         <v>85</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" s="3">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="C89" s="3">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="E89" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="F89" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H89" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I89" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A90" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C90" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>62</v>
+        <v>136</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>61</v>
+        <v>157</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" s="3">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="C91" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="G91" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="H91" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="3">
         <v>82</v>
       </c>
@@ -2674,10 +2674,10 @@
         <v>94</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2688,10 +2688,10 @@
         <v>5</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2705,10 +2705,10 @@
         <v>24</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" s="3">
         <v>95</v>
       </c>
@@ -2719,57 +2719,69 @@
         <v>24</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A96" s="3">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="C96" s="3">
         <v>2</v>
       </c>
+      <c r="D96" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="F96" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+      <c r="I96" s="6" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A97" s="3">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="C97" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>179</v>
+        <v>188</v>
+      </c>
+      <c r="I97" s="3" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A98" s="3">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C98" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>181</v>
-      </c>
-      <c r="I98" s="5" t="s">
-        <v>180</v>
+        <v>190</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A99" s="3">
-        <v>99</v>
+        <v>40</v>
       </c>
       <c r="C99" s="3">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+        <v>191</v>
+      </c>
+      <c r="I99" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" s="3">
         <v>100</v>
       </c>
@@ -2780,89 +2792,112 @@
         <v>24</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A101" s="3">
-        <v>101</v>
+        <v>25</v>
       </c>
       <c r="C101" s="3">
-        <v>2</v>
+        <v>4</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="F101" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="G101" s="3" t="s">
-        <v>185</v>
+        <v>62</v>
+      </c>
+      <c r="I101" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" s="3">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C102" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" s="3">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C103" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="I103" s="3" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A104" s="3">
-        <v>104</v>
+        <v>98</v>
       </c>
       <c r="C104" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="I104" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>180</v>
+      </c>
+      <c r="I104" s="5" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A105" s="3">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C105" s="3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>192</v>
+        <v>181</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A106" s="3">
+        <v>106</v>
+      </c>
+      <c r="C106" s="3">
+        <v>5</v>
+      </c>
+      <c r="F106" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A107" s="3">
+        <v>107</v>
+      </c>
+      <c r="C107" s="3">
+        <v>5</v>
+      </c>
+      <c r="F107" s="3" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I96">
+  <autoFilter ref="A1:I105">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
-    <sortState ref="A44:I81">
-      <sortCondition ref="C2:C81"/>
+    <sortState ref="A70:I105">
+      <sortCondition ref="C1:C105"/>
     </sortState>
   </autoFilter>
   <sortState ref="A44:I93">
     <sortCondition ref="C2:C93"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="I98" r:id="rId1"/>
+    <hyperlink ref="I104" r:id="rId1"/>
+    <hyperlink ref="I96" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Issue #111 hr not showing on advanced track screen
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$105</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$107</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="201">
   <si>
     <t>#</t>
   </si>
@@ -622,6 +622,24 @@
   </si>
   <si>
     <t>Config Service should return min, max, value for items</t>
+  </si>
+  <si>
+    <t>Advanced config space on edit page</t>
+  </si>
+  <si>
+    <t>Slider pipe for values</t>
+  </si>
+  <si>
+    <t>client side</t>
+  </si>
+  <si>
+    <t>see 101, 69</t>
+  </si>
+  <si>
+    <t>might need to move the advanced tab from track to playlist so that it is outside the ul</t>
+  </si>
+  <si>
+    <t>hr issue on advanced track detasil</t>
   </si>
 </sst>
 </file>
@@ -1107,11 +1125,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I107"/>
+  <dimension ref="A1:I111"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D96" sqref="D96"/>
+      <selection pane="bottomLeft" activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2324,7 +2342,7 @@
         <v>77</v>
       </c>
       <c r="C70" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>156</v>
@@ -2353,18 +2371,27 @@
         <v>137</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C72" s="3">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="D72" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>140</v>
+        <v>131</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>185</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>6</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2443,19 +2470,16 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
-        <v>14</v>
+        <v>101</v>
       </c>
       <c r="C77" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F77" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H77" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I77" s="3" t="s">
-        <v>95</v>
+        <v>183</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>184</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2483,18 +2507,15 @@
         <v>149</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="C80" s="3">
         <v>2</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="G80" s="3" t="s">
-        <v>185</v>
+        <v>140</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>6</v>
@@ -2502,16 +2523,19 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
-        <v>101</v>
+        <v>14</v>
       </c>
       <c r="C81" s="3">
         <v>2</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>183</v>
-      </c>
-      <c r="G81" s="3" t="s">
-        <v>184</v>
+        <v>130</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I81" s="3" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="82" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -2519,7 +2543,7 @@
         <v>75</v>
       </c>
       <c r="C82" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F82" s="3" t="s">
         <v>144</v>
@@ -2722,7 +2746,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" s="3">
         <v>103</v>
       </c>
@@ -2814,24 +2838,24 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A102" s="3">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="C102" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A103" s="3">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C103" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -2881,13 +2905,75 @@
         <v>194</v>
       </c>
     </row>
+    <row r="108" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A108" s="3">
+        <v>108</v>
+      </c>
+      <c r="C108" s="3">
+        <v>1</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F108" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A109" s="3">
+        <v>109</v>
+      </c>
+      <c r="C109" s="3">
+        <v>1</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A110" s="3">
+        <v>110</v>
+      </c>
+      <c r="C110" s="3">
+        <v>1</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="H110" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A111" s="3">
+        <v>111</v>
+      </c>
+      <c r="C111" s="3">
+        <v>1</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="I111" s="3" t="s">
+        <v>199</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I105">
+  <autoFilter ref="A1:I107">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
-    <sortState ref="A70:I105">
-      <sortCondition ref="C1:C105"/>
+    <sortState ref="A70:I107">
+      <sortCondition ref="C1:C107"/>
     </sortState>
   </autoFilter>
   <sortState ref="A44:I93">

</xml_diff>

<commit_message>
Issue #110 speed/brightness per image server side
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="203">
   <si>
     <t>#</t>
   </si>
@@ -423,9 +423,6 @@
   </si>
   <si>
     <t>Playlist Folders</t>
-  </si>
-  <si>
-    <t>Size/brightness per image</t>
   </si>
   <si>
     <t>uniform message handling</t>
@@ -640,6 +637,15 @@
   </si>
   <si>
     <t>hr issue on advanced track detasil</t>
+  </si>
+  <si>
+    <t>Speed/brightness per image</t>
+  </si>
+  <si>
+    <t>speed/brightness per image</t>
+  </si>
+  <si>
+    <t>server side</t>
   </si>
 </sst>
 </file>
@@ -1129,7 +1135,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C115" sqref="C115"/>
+      <selection pane="bottomLeft" activeCell="I119" sqref="I119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1609,13 +1615,13 @@
         <v>1</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>31</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1850,10 +1856,10 @@
         <v>94</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="41" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1895,13 +1901,13 @@
         <v>1</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="44" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -1915,7 +1921,7 @@
         <v>24</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -1966,7 +1972,7 @@
         <v>68</v>
       </c>
       <c r="F47" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="I47" s="3" t="s">
         <v>114</v>
@@ -2000,7 +2006,7 @@
         <v>24</v>
       </c>
       <c r="F49" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
@@ -2020,7 +2026,7 @@
         <v>101</v>
       </c>
       <c r="I50" s="3" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2168,7 +2174,7 @@
         <v>24</v>
       </c>
       <c r="F58" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="58" hidden="1" x14ac:dyDescent="0.35">
@@ -2182,7 +2188,7 @@
         <v>115</v>
       </c>
       <c r="I59" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
@@ -2202,7 +2208,7 @@
         <v>116</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2309,7 +2315,7 @@
         <v>123</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="68" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2334,7 +2340,7 @@
         <v>24</v>
       </c>
       <c r="F69" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="70" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -2345,13 +2351,13 @@
         <v>1</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2365,13 +2371,13 @@
         <v>24</v>
       </c>
       <c r="F71" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="I71" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>69</v>
       </c>
@@ -2382,16 +2388,16 @@
         <v>24</v>
       </c>
       <c r="F72" s="3" t="s">
-        <v>131</v>
+        <v>201</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H72" s="3" t="s">
         <v>6</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2408,13 +2414,13 @@
         <v>119</v>
       </c>
       <c r="F73" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G73" s="3">
         <v>26</v>
       </c>
       <c r="I73" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2431,10 +2437,10 @@
         <v>119</v>
       </c>
       <c r="F74" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="I74" s="3" t="s">
         <v>151</v>
-      </c>
-      <c r="I74" s="3" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="75" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2448,7 +2454,7 @@
         <v>117</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="76" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2462,10 +2468,10 @@
         <v>24</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F76" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.35">
@@ -2476,10 +2482,10 @@
         <v>1</v>
       </c>
       <c r="F77" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="G77" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="G77" s="3" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="78" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2493,7 +2499,7 @@
         <v>24</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="79" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2504,7 +2510,7 @@
         <v>24</v>
       </c>
       <c r="F79" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="80" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -2515,7 +2521,7 @@
         <v>2</v>
       </c>
       <c r="F80" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="H80" s="3" t="s">
         <v>6</v>
@@ -2546,7 +2552,7 @@
         <v>2</v>
       </c>
       <c r="F82" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2557,10 +2563,10 @@
         <v>24</v>
       </c>
       <c r="F83" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="I83" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="I83" s="3" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="84" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2574,7 +2580,7 @@
         <v>24</v>
       </c>
       <c r="F84" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="85" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2588,10 +2594,10 @@
         <v>24</v>
       </c>
       <c r="F85" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="I85" s="3" t="s">
         <v>165</v>
-      </c>
-      <c r="I85" s="3" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="86" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2605,7 +2611,7 @@
         <v>24</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2622,7 +2628,7 @@
         <v>85</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="88" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2639,7 +2645,7 @@
         <v>85</v>
       </c>
       <c r="F88" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.35">
@@ -2667,13 +2673,13 @@
         <v>68</v>
       </c>
       <c r="F90" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H90" s="3" t="s">
         <v>99</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.35">
@@ -2684,7 +2690,7 @@
         <v>3</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2698,10 +2704,10 @@
         <v>94</v>
       </c>
       <c r="F92" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2712,10 +2718,10 @@
         <v>5</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F93" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="94" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2729,7 +2735,7 @@
         <v>24</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2743,7 +2749,7 @@
         <v>24</v>
       </c>
       <c r="F95" s="3" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
@@ -2757,10 +2763,10 @@
         <v>24</v>
       </c>
       <c r="F96" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="I96" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="97" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -2771,10 +2777,10 @@
         <v>3</v>
       </c>
       <c r="F97" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I97" s="3" t="s">
         <v>188</v>
-      </c>
-      <c r="I97" s="3" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="98" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -2785,7 +2791,7 @@
         <v>3</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.35">
@@ -2799,7 +2805,7 @@
         <v>85</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="I99" s="3" t="s">
         <v>84</v>
@@ -2816,7 +2822,7 @@
         <v>24</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.35">
@@ -2844,7 +2850,7 @@
         <v>4</v>
       </c>
       <c r="F102" s="3" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.35">
@@ -2855,7 +2861,7 @@
         <v>5</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="104" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -2866,10 +2872,10 @@
         <v>5</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="I104" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.35">
@@ -2880,7 +2886,7 @@
         <v>5</v>
       </c>
       <c r="F105" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.35">
@@ -2891,7 +2897,7 @@
         <v>5</v>
       </c>
       <c r="F106" s="3" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="107" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
@@ -2902,7 +2908,7 @@
         <v>5</v>
       </c>
       <c r="F107" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="108" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -2916,7 +2922,7 @@
         <v>24</v>
       </c>
       <c r="F108" s="3" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.35">
@@ -2927,27 +2933,30 @@
         <v>1</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A110" s="3">
         <v>110</v>
       </c>
       <c r="C110" s="3">
         <v>1</v>
       </c>
+      <c r="D110" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="F110" s="3" t="s">
-        <v>131</v>
+        <v>200</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H110" s="3" t="s">
         <v>6</v>
       </c>
       <c r="I110" s="3" t="s">
-        <v>112</v>
+        <v>202</v>
       </c>
     </row>
     <row r="111" spans="1:9" ht="29" x14ac:dyDescent="0.35">
@@ -2961,10 +2970,10 @@
         <v>24</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="I111" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #77 duplicate track from playlist screen
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$107</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$112</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="206">
   <si>
     <t>#</t>
   </si>
@@ -646,6 +646,16 @@
   </si>
   <si>
     <t>server side</t>
+  </si>
+  <si>
+    <t>Missing lines effect</t>
+  </si>
+  <si>
+    <t>Horizontal flip/Vertical flip image</t>
+  </si>
+  <si>
+    <t>fas fa-arrows-alt-v, fas fa-arrows-alt-h from fontawesome
+https://www.w3schools.com/howto/howto_css_flip_image.asp</t>
   </si>
 </sst>
 </file>
@@ -1131,11 +1141,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I111"/>
+  <dimension ref="A1:I113"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I119" sqref="I119"/>
+      <selection pane="bottomLeft" activeCell="I113" sqref="I113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2377,7 +2387,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>69</v>
       </c>
@@ -2911,7 +2921,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="108" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" s="3">
         <v>108</v>
       </c>
@@ -2930,13 +2940,13 @@
         <v>109</v>
       </c>
       <c r="C109" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F109" s="3" t="s">
         <v>195</v>
       </c>
     </row>
-    <row r="110" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" s="3">
         <v>110</v>
       </c>
@@ -2959,7 +2969,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="3">
         <v>111</v>
       </c>
@@ -2976,8 +2986,33 @@
         <v>198</v>
       </c>
     </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A112" s="3">
+        <v>112</v>
+      </c>
+      <c r="C112" s="3">
+        <v>2</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A113" s="3">
+        <v>113</v>
+      </c>
+      <c r="C113" s="3">
+        <v>1</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="I113" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I107">
+  <autoFilter ref="A1:I112">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Issue #118 Play/save/add track button visible when showing details of track
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$I$112</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$J$118</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="214">
   <si>
     <t>#</t>
   </si>
@@ -655,7 +655,32 @@
   </si>
   <si>
     <t>fas fa-arrows-alt-v, fas fa-arrows-alt-h from fontawesome
-https://www.w3schools.com/howto/howto_css_flip_image.asp</t>
+https://www.w3schools.com/howto/howto_css_flip_image.asp
+JIMP image.flip( horz, vert );         // flip the image horizontally or vertically</t>
+  </si>
+  <si>
+    <t>On UI just have a one of 4 arrows showing</t>
+  </si>
+  <si>
+    <t>Fix header at top</t>
+  </si>
+  <si>
+    <t>Groups in playlist</t>
+  </si>
+  <si>
+    <t>Where you can resize, reverse, flipY the group as a whole</t>
+  </si>
+  <si>
+    <t>Use typescript on server</t>
+  </si>
+  <si>
+    <t>Status Date</t>
+  </si>
+  <si>
+    <t>remove unneeded calls in Track.component.ts and have better naming</t>
+  </si>
+  <si>
+    <t>Play/save/add track button visible when showing details of track</t>
   </si>
 </sst>
 </file>
@@ -720,7 +745,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -736,6 +761,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1141,25 +1169,26 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I113"/>
+  <dimension ref="A1:J118"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I113" sqref="I113"/>
+      <selection pane="bottomLeft" activeCell="E118" sqref="E118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="4" width="8.7265625" style="3"/>
-    <col min="5" max="5" width="19.7265625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="22.81640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="10" style="3" customWidth="1"/>
-    <col min="8" max="8" width="15.6328125" style="3" customWidth="1"/>
-    <col min="9" max="9" width="101.90625" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="3"/>
+    <col min="5" max="5" width="10.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7265625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="22.81640625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10" style="3" customWidth="1"/>
+    <col min="9" max="9" width="15.6328125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="101.90625" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1173,22 +1202,25 @@
         <v>7</v>
       </c>
       <c r="E1" s="4" t="s">
+        <v>211</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1198,14 +1230,14 @@
       <c r="D2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1215,20 +1247,20 @@
       <c r="D3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G3" s="3">
+      <c r="H3" s="3">
         <v>35</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="J3" s="3" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1238,179 +1270,179 @@
       <c r="D4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="3">
+      <c r="H4" s="3">
         <v>35</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H5" s="3" t="s">
+      <c r="I5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="J5" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="G6" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="F7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="F9" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="J11" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
       <c r="D12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="3" t="s">
+      <c r="F12" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="J12" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
       <c r="D13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="J13" s="3" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1420,14 +1452,14 @@
       <c r="D14" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="G14" s="3">
-        <v>24</v>
-      </c>
-      <c r="I14" s="3" t="s">
+      <c r="H14" s="3">
+        <v>24</v>
+      </c>
+      <c r="J14" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>44</v>
       </c>
@@ -1437,34 +1469,34 @@
       <c r="D15" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="I15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="J15" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="3" t="s">
+      <c r="F16" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="G16" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="I16" s="3" t="s">
+      <c r="J16" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1474,14 +1506,14 @@
       <c r="D17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="G17" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="I17" s="3" t="s">
+      <c r="J17" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1491,28 +1523,28 @@
       <c r="D18" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F18" s="3" t="s">
+      <c r="G18" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G18" s="3">
+      <c r="H18" s="3">
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="G19" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="J19" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1522,14 +1554,14 @@
       <c r="D20" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="G20" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="J20" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1539,14 +1571,14 @@
       <c r="D21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="G21" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="J21" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1556,17 +1588,17 @@
       <c r="D22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E22" s="3" t="s">
+      <c r="F22" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="G22" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="J22" s="3" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1576,14 +1608,14 @@
       <c r="D23" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E23" s="3" t="s">
+      <c r="F23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="J23" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>24</v>
       </c>
@@ -1593,17 +1625,17 @@
       <c r="D24" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="F24" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="G24" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="J24" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>67</v>
       </c>
@@ -1613,11 +1645,11 @@
       <c r="D25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="G25" s="3" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>70</v>
       </c>
@@ -1627,14 +1659,14 @@
       <c r="D26" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="G26" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="J26" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>27</v>
       </c>
@@ -1644,17 +1676,17 @@
       <c r="D27" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="G27" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="G27" s="3">
+      <c r="H27" s="3">
         <v>35</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="J27" s="3" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>28</v>
       </c>
@@ -1664,14 +1696,14 @@
       <c r="D28" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="G28" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="J28" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>29</v>
       </c>
@@ -1681,11 +1713,11 @@
       <c r="D29" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="G29" s="3" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>30</v>
       </c>
@@ -1695,11 +1727,11 @@
       <c r="D30" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="G30" s="3" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>31</v>
       </c>
@@ -1709,14 +1741,14 @@
       <c r="D31" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>32</v>
       </c>
@@ -1726,14 +1758,14 @@
       <c r="D32" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="G32" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="I32" s="3" t="s">
+      <c r="J32" s="3" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>39</v>
       </c>
@@ -1743,14 +1775,14 @@
       <c r="D33" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="G33" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="J33" s="3" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -1760,14 +1792,14 @@
       <c r="D34" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="G34" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="I34" s="3" t="s">
+      <c r="J34" s="3" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>35</v>
       </c>
@@ -1777,14 +1809,14 @@
       <c r="D35" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="G35" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="I35" s="3" t="s">
+      <c r="J35" s="3" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>36</v>
       </c>
@@ -1794,14 +1826,14 @@
       <c r="D36" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="G36" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="I36" s="3" t="s">
+      <c r="J36" s="3" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>37</v>
       </c>
@@ -1811,17 +1843,17 @@
       <c r="D37" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="G37" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="G37" s="3">
+      <c r="H37" s="3">
         <v>37</v>
       </c>
-      <c r="I37" s="3" t="s">
+      <c r="J37" s="3" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>38</v>
       </c>
@@ -1831,14 +1863,14 @@
       <c r="D38" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E38" s="3" t="s">
+      <c r="F38" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="G38" s="3" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>43</v>
       </c>
@@ -1848,14 +1880,14 @@
       <c r="D39" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="G39" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="I39" s="3" t="s">
+      <c r="J39" s="3" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>72</v>
       </c>
@@ -1865,14 +1897,14 @@
       <c r="D40" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F40" s="3" t="s">
+      <c r="G40" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="I40" s="3" t="s">
+      <c r="J40" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>41</v>
       </c>
@@ -1882,11 +1914,11 @@
       <c r="D41" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="G41" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>42</v>
       </c>
@@ -1896,14 +1928,14 @@
       <c r="D42" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F42" s="3" t="s">
+      <c r="G42" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="I42" s="3" t="s">
+      <c r="J42" s="3" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>74</v>
       </c>
@@ -1913,14 +1945,14 @@
       <c r="D43" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F43" s="3" t="s">
+      <c r="G43" s="3" t="s">
         <v>142</v>
       </c>
-      <c r="I43" s="3" t="s">
+      <c r="J43" s="3" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>90</v>
       </c>
@@ -1930,11 +1962,11 @@
       <c r="D44" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F44" s="3" t="s">
+      <c r="G44" s="3" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>45</v>
       </c>
@@ -1944,14 +1976,14 @@
       <c r="D45" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E45" s="3" t="s">
+      <c r="F45" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F45" s="3" t="s">
+      <c r="G45" s="3" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>46</v>
       </c>
@@ -1961,14 +1993,14 @@
       <c r="D46" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E46" s="3" t="s">
+      <c r="F46" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F46" s="3" t="s">
+      <c r="G46" s="3" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>58</v>
       </c>
@@ -1978,17 +2010,17 @@
       <c r="D47" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E47" s="3" t="s">
+      <c r="F47" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F47" s="3" t="s">
+      <c r="G47" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="I47" s="3" t="s">
+      <c r="J47" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>48</v>
       </c>
@@ -1998,14 +2030,14 @@
       <c r="D48" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E48" s="3" t="s">
+      <c r="F48" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F48" s="3" t="s">
+      <c r="G48" s="3" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>91</v>
       </c>
@@ -2015,11 +2047,11 @@
       <c r="D49" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F49" s="3" t="s">
+      <c r="G49" s="3" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>47</v>
       </c>
@@ -2029,17 +2061,17 @@
       <c r="D50" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E50" s="3" t="s">
+      <c r="F50" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F50" s="3" t="s">
+      <c r="G50" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="I50" s="3" t="s">
+      <c r="J50" s="3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>51</v>
       </c>
@@ -2052,14 +2084,14 @@
       <c r="D51" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F51" s="3" t="s">
+      <c r="G51" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="H51" s="3" t="s">
+      <c r="I51" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>52</v>
       </c>
@@ -2069,17 +2101,17 @@
       <c r="D52" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="F52" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F52" s="3" t="s">
+      <c r="G52" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="H52" s="3" t="s">
+      <c r="I52" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>53</v>
       </c>
@@ -2089,17 +2121,17 @@
       <c r="D53" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="F53" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F53" s="3" t="s">
+      <c r="G53" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="H53" s="3" t="s">
+      <c r="I53" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>54</v>
       </c>
@@ -2112,17 +2144,17 @@
       <c r="D54" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E54" s="3" t="s">
+      <c r="F54" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F54" s="3" t="s">
+      <c r="G54" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="H54" s="3" t="s">
+      <c r="I54" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>55</v>
       </c>
@@ -2132,17 +2164,17 @@
       <c r="D55" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E55" s="3" t="s">
+      <c r="F55" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F55" s="3" t="s">
+      <c r="G55" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="H55" s="3" t="s">
+      <c r="I55" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>56</v>
       </c>
@@ -2152,28 +2184,28 @@
       <c r="D56" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E56" s="3" t="s">
+      <c r="F56" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F56" s="3" t="s">
+      <c r="G56" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>57</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E57" s="3" t="s">
+      <c r="F57" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F57" s="3" t="s">
+      <c r="G57" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>92</v>
       </c>
@@ -2183,25 +2215,25 @@
       <c r="D58" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F58" s="3" t="s">
+      <c r="G58" s="3" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>59</v>
       </c>
       <c r="D59" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F59" s="3" t="s">
+      <c r="G59" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="I59" s="3" t="s">
+      <c r="J59" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>60</v>
       </c>
@@ -2211,17 +2243,17 @@
       <c r="D60" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="E60" s="3" t="s">
+      <c r="F60" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F60" s="3" t="s">
+      <c r="G60" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="I60" s="3" t="s">
+      <c r="J60" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>49</v>
       </c>
@@ -2231,28 +2263,28 @@
       <c r="D61" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E61" s="3" t="s">
+      <c r="F61" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F61" s="3" t="s">
+      <c r="G61" s="3" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>62</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E62" s="3" t="s">
+      <c r="F62" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F62" s="3" t="s">
+      <c r="G62" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>63</v>
       </c>
@@ -2262,17 +2294,17 @@
       <c r="D63" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E63" s="3" t="s">
+      <c r="F63" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="F63" s="3" t="s">
+      <c r="G63" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="I63" s="3" t="s">
+      <c r="J63" s="3" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>50</v>
       </c>
@@ -2282,36 +2314,36 @@
       <c r="D64" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E64" s="3" t="s">
+      <c r="F64" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F64" s="3" t="s">
+      <c r="G64" s="3" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="65" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>65</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F65" s="3" t="s">
+      <c r="G65" s="3" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="66" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>66</v>
       </c>
       <c r="D66" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F66" s="3" t="s">
+      <c r="G66" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>64</v>
       </c>
@@ -2321,25 +2353,25 @@
       <c r="D67" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F67" s="3" t="s">
+      <c r="G67" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="I67" s="3" t="s">
+      <c r="J67" s="3" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="68" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>68</v>
       </c>
       <c r="D68" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F68" s="3" t="s">
+      <c r="G68" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="1:9" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>93</v>
       </c>
@@ -2349,28 +2381,31 @@
       <c r="D69" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F69" s="3" t="s">
+      <c r="G69" s="3" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>77</v>
       </c>
       <c r="C70" s="3">
         <v>1</v>
       </c>
-      <c r="E70" s="3" t="s">
+      <c r="D70" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F70" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="F70" s="3" t="s">
+      <c r="G70" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="G70" s="3" t="s">
+      <c r="H70" s="3" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>71</v>
       </c>
@@ -2380,14 +2415,14 @@
       <c r="D71" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F71" s="3" t="s">
+      <c r="G71" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="I71" s="3" t="s">
+      <c r="J71" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="72" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>69</v>
       </c>
@@ -2397,20 +2432,20 @@
       <c r="D72" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F72" s="3" t="s">
+      <c r="G72" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="G72" s="3" t="s">
+      <c r="H72" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="H72" s="3" t="s">
+      <c r="I72" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I72" s="3" t="s">
+      <c r="J72" s="3" t="s">
         <v>196</v>
       </c>
     </row>
-    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>80</v>
       </c>
@@ -2420,20 +2455,20 @@
       <c r="D73" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E73" s="3" t="s">
+      <c r="F73" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="F73" s="3" t="s">
+      <c r="G73" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="G73" s="3">
+      <c r="H73" s="3">
         <v>26</v>
       </c>
-      <c r="I73" s="3" t="s">
+      <c r="J73" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>81</v>
       </c>
@@ -2443,31 +2478,31 @@
       <c r="D74" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E74" s="3" t="s">
+      <c r="F74" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="F74" s="3" t="s">
+      <c r="G74" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="I74" s="3" t="s">
+      <c r="J74" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="75" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>61</v>
       </c>
       <c r="D75" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F75" s="3" t="s">
+      <c r="G75" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="I75" s="3" t="s">
+      <c r="J75" s="3" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="76" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>76</v>
       </c>
@@ -2477,28 +2512,31 @@
       <c r="D76" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E76" s="3" t="s">
+      <c r="F76" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="F76" s="3" t="s">
+      <c r="G76" s="3" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>101</v>
       </c>
       <c r="C77" s="3">
         <v>1</v>
       </c>
-      <c r="F77" s="3" t="s">
+      <c r="G77" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="G77" s="3" t="s">
+      <c r="H77" s="3" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="78" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="J77" s="3" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>78</v>
       </c>
@@ -2508,78 +2546,87 @@
       <c r="D78" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F78" s="3" t="s">
+      <c r="G78" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="79" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>79</v>
       </c>
       <c r="D79" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F79" s="3" t="s">
+      <c r="G79" s="3" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="80" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
+        <v>113</v>
+      </c>
+      <c r="C80" s="3">
+        <v>1</v>
+      </c>
+      <c r="D80" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E80" s="7">
+        <v>43214</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="J80" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A81" s="3">
         <v>73</v>
-      </c>
-      <c r="C80" s="3">
-        <v>2</v>
-      </c>
-      <c r="F80" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="H80" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A81" s="3">
-        <v>14</v>
       </c>
       <c r="C81" s="3">
         <v>2</v>
       </c>
-      <c r="F81" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="H81" s="3" t="s">
+      <c r="G81" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="I81" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I81" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="82" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
-        <v>75</v>
+        <v>14</v>
       </c>
       <c r="C82" s="3">
         <v>2</v>
       </c>
-      <c r="F82" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G82" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I82" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="J82" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>83</v>
       </c>
       <c r="D83" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F83" s="3" t="s">
+      <c r="G83" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="I83" s="3" t="s">
+      <c r="J83" s="3" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>84</v>
       </c>
@@ -2589,11 +2636,11 @@
       <c r="D84" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F84" s="3" t="s">
+      <c r="G84" s="3" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="85" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="3">
         <v>85</v>
       </c>
@@ -2603,14 +2650,14 @@
       <c r="D85" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F85" s="3" t="s">
+      <c r="G85" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="I85" s="3" t="s">
+      <c r="J85" s="3" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="86" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="3">
         <v>86</v>
       </c>
@@ -2620,11 +2667,11 @@
       <c r="D86" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F86" s="3" t="s">
+      <c r="G86" s="3" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="3">
         <v>87</v>
       </c>
@@ -2634,14 +2681,14 @@
       <c r="D87" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E87" s="3" t="s">
+      <c r="F87" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F87" s="3" t="s">
+      <c r="G87" s="3" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="88" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="3">
         <v>88</v>
       </c>
@@ -2651,59 +2698,47 @@
       <c r="D88" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E88" s="3" t="s">
+      <c r="F88" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F88" s="3" t="s">
+      <c r="G88" s="3" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A89" s="3">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="C89" s="3">
-        <v>3</v>
-      </c>
-      <c r="E89" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F89" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="90" spans="1:9" ht="58" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="3">
-        <v>26</v>
+        <v>109</v>
       </c>
       <c r="C90" s="3">
-        <v>3</v>
-      </c>
-      <c r="E90" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F90" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="H90" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="I90" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="3">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="C91" s="3">
-        <v>3</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="3">
         <v>82</v>
       </c>
@@ -2713,14 +2748,14 @@
       <c r="D92" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="F92" s="3" t="s">
+      <c r="G92" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="I92" s="3" t="s">
+      <c r="J92" s="3" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" s="3">
         <v>89</v>
       </c>
@@ -2730,11 +2765,11 @@
       <c r="D93" s="3" t="s">
         <v>140</v>
       </c>
-      <c r="F93" s="3" t="s">
+      <c r="G93" s="3" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="94" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="3">
         <v>94</v>
       </c>
@@ -2744,11 +2779,11 @@
       <c r="D94" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F94" s="3" t="s">
+      <c r="G94" s="3" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" s="3">
         <v>95</v>
       </c>
@@ -2758,11 +2793,11 @@
       <c r="D95" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F95" s="3" t="s">
+      <c r="G95" s="3" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" s="3">
         <v>103</v>
       </c>
@@ -2772,56 +2807,59 @@
       <c r="D96" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F96" s="3" t="s">
+      <c r="G96" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="I96" s="6" t="s">
+      <c r="J96" s="6" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="97" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A97" s="3">
-        <v>104</v>
+        <v>31</v>
       </c>
       <c r="C97" s="3">
         <v>3</v>
       </c>
       <c r="F97" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="I97" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="98" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A98" s="3">
-        <v>105</v>
+        <v>26</v>
       </c>
       <c r="C98" s="3">
         <v>3</v>
       </c>
       <c r="F98" s="3" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+        <v>68</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="I98" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J98" s="3" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="3">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="C99" s="3">
-        <v>4</v>
-      </c>
-      <c r="E99" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="F99" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="I99" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="100" spans="1:9" ht="58" hidden="1" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="100" spans="1:10" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" s="3">
         <v>100</v>
       </c>
@@ -2831,97 +2869,106 @@
       <c r="D100" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F100" s="3" t="s">
+      <c r="G100" s="3" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A101" s="3">
+        <v>104</v>
+      </c>
+      <c r="C101" s="3">
+        <v>3</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J101" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A102" s="3">
+        <v>105</v>
+      </c>
+      <c r="C102" s="3">
+        <v>3</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A103" s="3">
+        <v>40</v>
+      </c>
+      <c r="C103" s="3">
+        <v>4</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="J103" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A104" s="3">
         <v>25</v>
       </c>
-      <c r="C101" s="3">
+      <c r="C104" s="3">
         <v>4</v>
       </c>
-      <c r="E101" s="3" t="s">
+      <c r="F104" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F101" s="3" t="s">
+      <c r="G104" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="I101" s="3" t="s">
+      <c r="J104" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A102" s="3">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A105" s="3">
         <v>102</v>
       </c>
-      <c r="C102" s="3">
+      <c r="C105" s="3">
         <v>4</v>
       </c>
-      <c r="F102" s="3" t="s">
+      <c r="G105" s="3" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A103" s="3">
+    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A106" s="3">
         <v>97</v>
-      </c>
-      <c r="C103" s="3">
-        <v>5</v>
-      </c>
-      <c r="F103" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="104" spans="1:9" ht="29" x14ac:dyDescent="0.35">
-      <c r="A104" s="3">
-        <v>98</v>
-      </c>
-      <c r="C104" s="3">
-        <v>5</v>
-      </c>
-      <c r="F104" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="I104" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A105" s="3">
-        <v>99</v>
-      </c>
-      <c r="C105" s="3">
-        <v>5</v>
-      </c>
-      <c r="F105" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A106" s="3">
-        <v>106</v>
       </c>
       <c r="C106" s="3">
         <v>5</v>
       </c>
-      <c r="F106" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="107" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="G106" s="3" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A107" s="3">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C107" s="3">
         <v>5</v>
       </c>
-      <c r="F107" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+      <c r="G107" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="J107" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="108" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" s="3">
         <v>108</v>
       </c>
@@ -2931,22 +2978,22 @@
       <c r="D108" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F108" s="3" t="s">
+      <c r="G108" s="3" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" s="3">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="C109" s="3">
-        <v>2</v>
-      </c>
-      <c r="F109" s="3" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="110" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="110" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" s="3">
         <v>110</v>
       </c>
@@ -2956,20 +3003,20 @@
       <c r="D110" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F110" s="3" t="s">
+      <c r="G110" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="G110" s="3" t="s">
+      <c r="H110" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="H110" s="3" t="s">
+      <c r="I110" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I110" s="3" t="s">
+      <c r="J110" s="3" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="111" spans="1:9" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="3">
         <v>111</v>
       </c>
@@ -2979,53 +3026,120 @@
       <c r="D111" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F111" s="3" t="s">
+      <c r="G111" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="I111" s="3" t="s">
+      <c r="J111" s="3" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" s="3">
-        <v>112</v>
+        <v>106</v>
       </c>
       <c r="C112" s="3">
-        <v>2</v>
-      </c>
-      <c r="F112" s="3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="113" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+      <c r="G112" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A113" s="3">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C113" s="3">
-        <v>1</v>
-      </c>
-      <c r="F113" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="I113" s="3" t="s">
-        <v>205</v>
+        <v>5</v>
+      </c>
+      <c r="G113" s="3" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A114" s="3">
+        <v>114</v>
+      </c>
+      <c r="C114" s="3">
+        <v>5</v>
+      </c>
+      <c r="G114" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A115" s="3">
+        <v>115</v>
+      </c>
+      <c r="C115" s="3">
+        <v>1</v>
+      </c>
+      <c r="G115" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="J115" s="3" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A116" s="3">
+        <v>116</v>
+      </c>
+      <c r="C116" s="3">
+        <v>3</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="117" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A117" s="3">
+        <v>117</v>
+      </c>
+      <c r="C117" s="3">
+        <v>1</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E117" s="7">
+        <v>43214</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="118" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A118" s="3">
+        <v>118</v>
+      </c>
+      <c r="C118" s="3">
+        <v>1</v>
+      </c>
+      <c r="D118" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E118" s="7">
+        <v>43214</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>213</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I112">
+  <autoFilter ref="A1:J118">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
-    <sortState ref="A70:I107">
-      <sortCondition ref="C1:C107"/>
+    <sortState ref="A70:J113">
+      <sortCondition ref="C1:C113"/>
     </sortState>
   </autoFilter>
-  <sortState ref="A44:I93">
+  <sortState ref="A44:J93">
     <sortCondition ref="C2:C93"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="I104" r:id="rId1"/>
-    <hyperlink ref="I96" r:id="rId2"/>
+    <hyperlink ref="J107" r:id="rId1"/>
+    <hyperlink ref="J96" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>

</xml_diff>

<commit_message>
Issue #116 Use typescript on server for ServerEmulator
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="217">
   <si>
     <t>#</t>
   </si>
@@ -681,6 +681,15 @@
   </si>
   <si>
     <t>Play/save/add track button visible when showing details of track</t>
+  </si>
+  <si>
+    <t>For ServerEmulator</t>
+  </si>
+  <si>
+    <t>For ServerCommon</t>
+  </si>
+  <si>
+    <t>Share DTOs between client and server</t>
   </si>
 </sst>
 </file>
@@ -1169,11 +1178,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J118"/>
+  <dimension ref="A1:J120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E118" sqref="E118"/>
+      <selection pane="bottomLeft" activeCell="E116" sqref="E116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3085,10 +3094,19 @@
         <v>116</v>
       </c>
       <c r="C116" s="3">
-        <v>3</v>
+        <v>1</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E116" s="7">
+        <v>43214</v>
       </c>
       <c r="G116" s="3" t="s">
         <v>210</v>
+      </c>
+      <c r="J116" s="3" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="117" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
@@ -3108,7 +3126,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" s="3">
         <v>118</v>
       </c>
@@ -3123,6 +3141,31 @@
       </c>
       <c r="G118" s="3" t="s">
         <v>213</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A119" s="3">
+        <v>119</v>
+      </c>
+      <c r="C119" s="3">
+        <v>1</v>
+      </c>
+      <c r="G119" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="J119" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A120" s="3">
+        <v>120</v>
+      </c>
+      <c r="C120" s="3">
+        <v>1</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>216</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #122 Extract Playlist class
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -16,7 +16,7 @@
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$J$118</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$J$122</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="223">
   <si>
     <t>#</t>
   </si>
@@ -585,9 +585,6 @@
     <t>On play playlist screen should only show the elements that are enabled</t>
   </si>
   <si>
-    <t>rotate and scale images</t>
-  </si>
-  <si>
     <t>see 25</t>
   </si>
   <si>
@@ -690,6 +687,27 @@
   </si>
   <si>
     <t>Share DTOs between client and server</t>
+  </si>
+  <si>
+    <t>tslint</t>
+  </si>
+  <si>
+    <t>Extract Playlist class</t>
+  </si>
+  <si>
+    <t>do after 122</t>
+  </si>
+  <si>
+    <t>do after 119</t>
+  </si>
+  <si>
+    <t>scale images</t>
+  </si>
+  <si>
+    <t>rotate</t>
+  </si>
+  <si>
+    <t>Would do this pre prod in PhotoShop</t>
   </si>
 </sst>
 </file>
@@ -1178,11 +1196,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J120"/>
+  <dimension ref="A1:J123"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E116" sqref="E116"/>
+      <selection pane="bottomLeft" activeCell="D123" sqref="D123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1211,7 +1229,7 @@
         <v>7</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F1" s="4" t="s">
         <v>4</v>
@@ -2442,16 +2460,16 @@
         <v>24</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="I72" s="3" t="s">
         <v>6</v>
       </c>
       <c r="J72" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
@@ -2533,16 +2551,16 @@
         <v>101</v>
       </c>
       <c r="C77" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G77" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="H77" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="H77" s="3" t="s">
-        <v>183</v>
-      </c>
       <c r="J77" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2584,41 +2602,41 @@
         <v>43214</v>
       </c>
       <c r="G80" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="J80" s="3" t="s">
         <v>204</v>
       </c>
-      <c r="J80" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
-        <v>73</v>
+        <v>115</v>
       </c>
       <c r="C81" s="3">
         <v>2</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I81" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+        <v>207</v>
+      </c>
+      <c r="J81" s="3" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
-        <v>14</v>
+        <v>119</v>
       </c>
       <c r="C82" s="3">
-        <v>2</v>
+        <v>1.2</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="I82" s="3" t="s">
-        <v>6</v>
+        <v>209</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>218</v>
       </c>
       <c r="J82" s="3" t="s">
-        <v>95</v>
+        <v>214</v>
       </c>
     </row>
     <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
@@ -2716,35 +2734,38 @@
     </row>
     <row r="89" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A89" s="3">
-        <v>75</v>
+        <v>120</v>
       </c>
       <c r="C89" s="3">
-        <v>2</v>
+        <v>1.3</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>143</v>
+        <v>215</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="3">
-        <v>109</v>
+        <v>122</v>
       </c>
       <c r="C90" s="3">
-        <v>2</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>195</v>
+        <v>217</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="3">
-        <v>112</v>
+        <v>123</v>
       </c>
       <c r="C91" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
     </row>
     <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
@@ -2817,55 +2838,52 @@
         <v>24</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="J96" s="6" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="97" spans="1:10" x14ac:dyDescent="0.35">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="97" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A97" s="3">
-        <v>31</v>
+        <v>73</v>
       </c>
       <c r="C97" s="3">
-        <v>3</v>
-      </c>
-      <c r="F97" s="3" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="98" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+      <c r="I97" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A98" s="3">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C98" s="3">
         <v>3</v>
       </c>
-      <c r="F98" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="G98" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="I98" s="3" t="s">
-        <v>99</v>
+        <v>6</v>
       </c>
       <c r="J98" s="3" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A99" s="3">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="C99" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>176</v>
+        <v>143</v>
       </c>
     </row>
     <row r="100" spans="1:10" ht="58" hidden="1" x14ac:dyDescent="0.35">
@@ -2882,99 +2900,105 @@
         <v>181</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="3">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="C101" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="J101" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="3">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="C102" s="3">
-        <v>3</v>
+        <v>2</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E102" s="7">
+        <v>43214</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>189</v>
+        <v>202</v>
+      </c>
+      <c r="J102" s="3" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="3">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="C103" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F103" s="3" t="s">
-        <v>85</v>
+        <v>68</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="J103" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A104" s="3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C104" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>31</v>
+        <v>68</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>62</v>
+        <v>135</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="J104" s="3" t="s">
-        <v>61</v>
+        <v>156</v>
       </c>
     </row>
     <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="3">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C105" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A106" s="3">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="C106" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>177</v>
+        <v>186</v>
+      </c>
+      <c r="J106" s="3" t="s">
+        <v>187</v>
       </c>
     </row>
     <row r="107" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A107" s="3">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="C107" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="J107" s="5" t="s">
-        <v>178</v>
+        <v>188</v>
       </c>
     </row>
     <row r="108" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2988,18 +3012,18 @@
         <v>24</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" s="3">
-        <v>99</v>
+        <v>121</v>
       </c>
       <c r="C109" s="3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>180</v>
+        <v>216</v>
       </c>
     </row>
     <row r="110" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -3013,16 +3037,16 @@
         <v>24</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="H110" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="I110" s="3" t="s">
         <v>6</v>
       </c>
       <c r="J110" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="111" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -3036,60 +3060,69 @@
         <v>24</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="J111" s="3" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="112" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A112" s="3">
-        <v>106</v>
+        <v>40</v>
       </c>
       <c r="C112" s="3">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+      <c r="J112" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" s="3">
-        <v>107</v>
+        <v>25</v>
       </c>
       <c r="C113" s="3">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="F113" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>193</v>
+        <v>62</v>
+      </c>
+      <c r="J113" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" s="3">
-        <v>114</v>
+        <v>102</v>
       </c>
       <c r="C114" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>207</v>
+        <v>190</v>
       </c>
     </row>
     <row r="115" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A115" s="3">
-        <v>115</v>
+        <v>97</v>
       </c>
       <c r="C115" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="J115" s="3" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="116" spans="1:10" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" s="3">
         <v>116</v>
       </c>
@@ -3103,10 +3136,10 @@
         <v>43214</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J116" s="3" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="117" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
@@ -3123,7 +3156,7 @@
         <v>43214</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="118" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
@@ -3140,48 +3173,81 @@
         <v>43214</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="119" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A119" s="3">
-        <v>119</v>
+        <v>98</v>
       </c>
       <c r="C119" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>210</v>
-      </c>
-      <c r="J119" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>179</v>
+      </c>
+      <c r="J119" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" s="3">
-        <v>120</v>
+        <v>99</v>
       </c>
       <c r="C120" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>216</v>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A121" s="3">
+        <v>106</v>
+      </c>
+      <c r="C121" s="3">
+        <v>5</v>
+      </c>
+      <c r="G121" s="3" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A122" s="3">
+        <v>107</v>
+      </c>
+      <c r="C122" s="3">
+        <v>5</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A123" s="3">
+        <v>114</v>
+      </c>
+      <c r="C123" s="3">
+        <v>5</v>
+      </c>
+      <c r="G123" s="3" t="s">
+        <v>206</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J118">
+  <autoFilter ref="A1:J122">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
-    <sortState ref="A70:J113">
-      <sortCondition ref="C1:C113"/>
+    <sortState ref="A77:J123">
+      <sortCondition ref="C1:C122"/>
     </sortState>
   </autoFilter>
   <sortState ref="A44:J93">
     <sortCondition ref="C2:C93"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="J107" r:id="rId1"/>
+    <hyperlink ref="J119" r:id="rId1"/>
     <hyperlink ref="J96" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Issue #119 use typescript on server
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="16050" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView minimized="1" xWindow="16050" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="223">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="224">
   <si>
     <t>#</t>
   </si>
@@ -704,10 +704,13 @@
     <t>scale images</t>
   </si>
   <si>
-    <t>rotate</t>
-  </si>
-  <si>
     <t>Would do this pre prod in PhotoShop</t>
+  </si>
+  <si>
+    <t>rotate images</t>
+  </si>
+  <si>
+    <t>Use pure virtual functions</t>
   </si>
 </sst>
 </file>
@@ -1196,11 +1199,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J123"/>
+  <dimension ref="A1:J124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D123" sqref="D123"/>
+      <selection pane="bottomLeft" activeCell="G81" sqref="G81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2548,19 +2551,13 @@
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="C77" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>221</v>
-      </c>
-      <c r="H77" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="J77" s="3" t="s">
-        <v>205</v>
+        <v>220</v>
       </c>
     </row>
     <row r="78" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -2610,16 +2607,19 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="C81" s="3">
-        <v>2</v>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E81" s="7">
+        <v>43215</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="J81" s="3" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
     </row>
     <row r="82" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -2748,24 +2748,33 @@
     </row>
     <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="3">
-        <v>122</v>
+        <v>101</v>
       </c>
       <c r="C90" s="3">
-        <v>1.1000000000000001</v>
+        <v>2</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>217</v>
+        <v>222</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="J90" s="3" t="s">
+        <v>205</v>
       </c>
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="3">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C91" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>220</v>
+        <v>207</v>
+      </c>
+      <c r="J91" s="3" t="s">
+        <v>208</v>
       </c>
     </row>
     <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
@@ -2858,32 +2867,26 @@
         <v>6</v>
       </c>
     </row>
-    <row r="98" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A98" s="3">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="C98" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="I98" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J98" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="99" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A99" s="3">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="C99" s="3">
         <v>2</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>143</v>
+        <v>194</v>
       </c>
     </row>
     <row r="100" spans="1:10" ht="58" hidden="1" x14ac:dyDescent="0.35">
@@ -2902,33 +2905,39 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="3">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="C101" s="3">
         <v>2</v>
       </c>
+      <c r="D101" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E101" s="7">
+        <v>43214</v>
+      </c>
       <c r="G101" s="3" t="s">
-        <v>194</v>
+        <v>202</v>
+      </c>
+      <c r="J101" s="3" t="s">
+        <v>221</v>
       </c>
     </row>
     <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="3">
-        <v>112</v>
+        <v>14</v>
       </c>
       <c r="C102" s="3">
-        <v>2</v>
-      </c>
-      <c r="D102" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E102" s="7">
-        <v>43214</v>
+        <v>3</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>202</v>
+        <v>130</v>
+      </c>
+      <c r="I102" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="J102" s="3" t="s">
-        <v>222</v>
+        <v>95</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.35">
@@ -3232,6 +3241,17 @@
       </c>
       <c r="G123" s="3" t="s">
         <v>206</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A124" s="3">
+        <v>124</v>
+      </c>
+      <c r="C124" s="3">
+        <v>1</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>223</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #125 Extract Player from Playlist
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="16050" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="17120" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="225">
   <si>
     <t>#</t>
   </si>
@@ -711,6 +711,9 @@
   </si>
   <si>
     <t>Use pure virtual functions</t>
+  </si>
+  <si>
+    <t>Extract Player from Playlist</t>
   </si>
 </sst>
 </file>
@@ -1199,11 +1202,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J124"/>
+  <dimension ref="A1:J125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G81" sqref="G81"/>
+      <selection pane="bottomLeft" activeCell="G125" sqref="G125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2629,6 +2632,12 @@
       <c r="C82" s="3">
         <v>1.2</v>
       </c>
+      <c r="D82" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E82" s="7">
+        <v>43215</v>
+      </c>
       <c r="G82" s="3" t="s">
         <v>209</v>
       </c>
@@ -3252,6 +3261,23 @@
       </c>
       <c r="G124" s="3" t="s">
         <v>223</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A125" s="3">
+        <v>125</v>
+      </c>
+      <c r="C125" s="3">
+        <v>1</v>
+      </c>
+      <c r="D125" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E125" s="7">
+        <v>43216</v>
+      </c>
+      <c r="G125" s="3" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #126 playlistDTOToPlaylist mapper
* black background to image

* savpoint

* Done
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="17120" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="18190" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$J$126</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$J$129</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="382" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="232">
   <si>
     <t>#</t>
   </si>
@@ -716,9 +716,6 @@
     <t>Should have a PlaylistDTOToPlaylist mapper that takes NUMLEDS and brigtness</t>
   </si>
   <si>
-    <t>This will remove a lot of stuff in the final Playlist that does not need to be there (config, newPlaylist)</t>
-  </si>
-  <si>
     <t>node debugger</t>
   </si>
   <si>
@@ -726,6 +723,18 @@
   </si>
   <si>
     <t>On UI just have a one of 4 arrows showing, absorbed into 123</t>
+  </si>
+  <si>
+    <t>default {} parameters</t>
+  </si>
+  <si>
+    <t>This will remove a lot of stuff in the final Playlist that does not need to be there (config, newPlaylist) this version uses config see 129 also</t>
+  </si>
+  <si>
+    <t>this is done on a copy and paste basis</t>
+  </si>
+  <si>
+    <t>see 128</t>
   </si>
 </sst>
 </file>
@@ -1214,11 +1223,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J127"/>
+  <dimension ref="A1:J129"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F130" sqref="F130"/>
+      <selection pane="bottomLeft" activeCell="H125" sqref="H125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2637,7 +2646,7 @@
         <v>219</v>
       </c>
       <c r="J81" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.35">
@@ -2744,18 +2753,24 @@
         <v>168</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="3">
         <v>126</v>
       </c>
       <c r="C89" s="3">
         <v>1</v>
       </c>
+      <c r="D89" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E89" s="7">
+        <v>43219</v>
+      </c>
       <c r="G89" s="3" t="s">
         <v>224</v>
       </c>
       <c r="J89" s="3" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
     </row>
     <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
@@ -2874,18 +2889,27 @@
         <v>184</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="3">
         <v>120</v>
       </c>
       <c r="C97" s="3">
         <v>1.3</v>
       </c>
+      <c r="D97" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E97" s="7">
+        <v>43219</v>
+      </c>
       <c r="G97" s="3" t="s">
         <v>214</v>
       </c>
       <c r="H97" s="3" t="s">
         <v>218</v>
+      </c>
+      <c r="J97" s="3" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
@@ -2908,7 +2932,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="99" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="3">
         <v>101</v>
       </c>
@@ -2928,7 +2952,7 @@
         <v>182</v>
       </c>
       <c r="J99" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="100" spans="1:10" ht="58" hidden="1" x14ac:dyDescent="0.35">
@@ -3315,7 +3339,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="127" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" s="3">
         <v>127</v>
       </c>
@@ -3332,11 +3356,36 @@
         <v>68</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
+      </c>
+    </row>
+    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A128" s="3">
+        <v>128</v>
+      </c>
+      <c r="C128" s="3">
+        <v>5</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="129" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+      <c r="A129" s="3">
+        <v>129</v>
+      </c>
+      <c r="C129" s="3">
+        <v>5</v>
+      </c>
+      <c r="G129" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="H129" s="3" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J126">
+  <autoFilter ref="A1:J129">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Issue #123 scale and rotate images
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="18190" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="19260" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="233">
   <si>
     <t>#</t>
   </si>
@@ -735,6 +735,9 @@
   </si>
   <si>
     <t>see 128</t>
+  </si>
+  <si>
+    <t>Ability to sheer picture</t>
   </si>
 </sst>
 </file>
@@ -1223,11 +1226,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J129"/>
+  <dimension ref="A1:J130"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H125" sqref="H125"/>
+      <selection pane="bottomLeft" activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2642,6 +2645,12 @@
       <c r="C81" s="3">
         <v>1</v>
       </c>
+      <c r="D81" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E81" s="7">
+        <v>43219</v>
+      </c>
       <c r="G81" s="3" t="s">
         <v>219</v>
       </c>
@@ -3382,6 +3391,17 @@
       </c>
       <c r="H129" s="3" t="s">
         <v>231</v>
+      </c>
+    </row>
+    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A130" s="3">
+        <v>130</v>
+      </c>
+      <c r="C130" s="3">
+        <v>1</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>232</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #131 part of
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="19260" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="20330" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$J$129</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$J$130</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="241">
   <si>
     <t>#</t>
   </si>
@@ -734,10 +734,36 @@
     <t>this is done on a copy and paste basis</t>
   </si>
   <si>
-    <t>see 128</t>
-  </si>
-  <si>
     <t>Ability to sheer picture</t>
+  </si>
+  <si>
+    <t>see 124, and 128</t>
+  </si>
+  <si>
+    <t>Build release using typescript</t>
+  </si>
+  <si>
+    <t>Should merge serverEmulator into serverCommon to make the build/dev cycle easier</t>
+  </si>
+  <si>
+    <t>be consistent with the import/export of modules</t>
+  </si>
+  <si>
+    <t>use export class …</t>
+  </si>
+  <si>
+    <t>Rejig config service to be better</t>
+  </si>
+  <si>
+    <t>currently it is not really a service … should be a singleton.</t>
+  </si>
+  <si>
+    <t>don’t forget to update the README.md file with the build instructions when you do
+I don’t really want the emulator code in the real version
+I do want the emulator code to call the server in the same way that Rpi will</t>
+  </si>
+  <si>
+    <t>revist after 134</t>
   </si>
 </sst>
 </file>
@@ -1226,11 +1252,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J130"/>
+  <dimension ref="A1:J134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E81" sqref="E81"/>
+      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H131" sqref="H131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2638,7 +2664,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>123</v>
       </c>
@@ -2658,15 +2684,15 @@
         <v>226</v>
       </c>
     </row>
-    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="C82" s="3">
         <v>1</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>222</v>
+        <v>233</v>
       </c>
     </row>
     <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
@@ -2980,103 +3006,91 @@
     </row>
     <row r="101" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A101" s="3">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C101" s="3">
         <v>2</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="J101" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A102" s="3">
-        <v>73</v>
+        <v>130</v>
       </c>
       <c r="C102" s="3">
         <v>2</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I102" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="3">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="C103" s="3">
         <v>2</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+        <v>206</v>
+      </c>
+      <c r="J103" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A104" s="3">
-        <v>109</v>
+        <v>73</v>
       </c>
       <c r="C104" s="3">
         <v>2</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+        <v>139</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A105" s="3">
-        <v>14</v>
+        <v>75</v>
       </c>
       <c r="C105" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="I105" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="J105" s="3" t="s">
-        <v>95</v>
+        <v>143</v>
       </c>
     </row>
     <row r="106" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A106" s="3">
-        <v>31</v>
+        <v>109</v>
       </c>
       <c r="C106" s="3">
-        <v>3</v>
-      </c>
-      <c r="F106" s="3" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A107" s="3">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C107" s="3">
         <v>3</v>
       </c>
-      <c r="F107" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="G107" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="I107" s="3" t="s">
-        <v>99</v>
+        <v>6</v>
       </c>
       <c r="J107" s="3" t="s">
-        <v>156</v>
+        <v>95</v>
       </c>
     </row>
     <row r="108" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -3095,13 +3109,16 @@
     </row>
     <row r="109" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A109" s="3">
-        <v>96</v>
+        <v>31</v>
       </c>
       <c r="C109" s="3">
         <v>3</v>
       </c>
+      <c r="F109" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="G109" s="3" t="s">
-        <v>176</v>
+        <v>70</v>
       </c>
     </row>
     <row r="110" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -3144,57 +3161,60 @@
         <v>197</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A112" s="3">
-        <v>104</v>
+        <v>26</v>
       </c>
       <c r="C112" s="3">
         <v>3</v>
       </c>
+      <c r="F112" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="G112" s="3" t="s">
-        <v>186</v>
+        <v>135</v>
+      </c>
+      <c r="I112" s="3" t="s">
+        <v>99</v>
       </c>
       <c r="J112" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="113" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" s="3">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C113" s="3">
         <v>3</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A114" s="3">
-        <v>121</v>
+        <v>104</v>
       </c>
       <c r="C114" s="3">
         <v>3</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" x14ac:dyDescent="0.35">
+        <v>186</v>
+      </c>
+      <c r="J114" s="3" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A115" s="3">
-        <v>40</v>
+        <v>105</v>
       </c>
       <c r="C115" s="3">
-        <v>4</v>
-      </c>
-      <c r="F115" s="3" t="s">
-        <v>85</v>
+        <v>3</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>189</v>
-      </c>
-      <c r="J115" s="3" t="s">
-        <v>84</v>
+        <v>188</v>
       </c>
     </row>
     <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
@@ -3253,99 +3273,105 @@
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A119" s="3">
-        <v>25</v>
+        <v>121</v>
       </c>
       <c r="C119" s="3">
-        <v>4</v>
-      </c>
-      <c r="F119" s="3" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="J119" s="3" t="s">
-        <v>61</v>
+        <v>215</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" s="3">
-        <v>102</v>
+        <v>40</v>
       </c>
       <c r="C120" s="3">
         <v>4</v>
       </c>
+      <c r="F120" s="3" t="s">
+        <v>85</v>
+      </c>
       <c r="G120" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
+      </c>
+      <c r="J120" s="3" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A121" s="3">
-        <v>97</v>
+        <v>25</v>
       </c>
       <c r="C121" s="3">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="F121" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="122" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+      <c r="J121" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A122" s="3">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="C122" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="J122" s="5" t="s">
-        <v>178</v>
+        <v>190</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" s="3">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C123" s="3">
         <v>5</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A124" s="3">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C124" s="3">
         <v>5</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+        <v>179</v>
+      </c>
+      <c r="J124" s="5" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A125" s="3">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C125" s="3">
         <v>5</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" s="3">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C126" s="3">
         <v>5</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
@@ -3368,56 +3394,115 @@
         <v>225</v>
       </c>
     </row>
-    <row r="128" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A128" s="3">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="C128" s="3">
         <v>5</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>228</v>
-      </c>
-    </row>
-    <row r="129" spans="1:8" ht="58" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" s="3">
-        <v>129</v>
+        <v>114</v>
       </c>
       <c r="C129" s="3">
         <v>5</v>
       </c>
       <c r="G129" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A130" s="3">
+        <v>128</v>
+      </c>
+      <c r="C130" s="3">
+        <v>5</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A131" s="3">
+        <v>129</v>
+      </c>
+      <c r="C131" s="3">
+        <v>5</v>
+      </c>
+      <c r="G131" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="H129" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A130" s="3">
-        <v>130</v>
-      </c>
-      <c r="C130" s="3">
-        <v>1</v>
-      </c>
-      <c r="G130" s="3" t="s">
+      <c r="H131" s="3" t="s">
         <v>232</v>
       </c>
     </row>
+    <row r="132" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A132" s="3">
+        <v>132</v>
+      </c>
+      <c r="C132" s="3">
+        <v>1</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="H132" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="J132" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="133" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A133" s="3">
+        <v>133</v>
+      </c>
+      <c r="C133" s="3">
+        <v>2</v>
+      </c>
+      <c r="G133" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="J133" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="134" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A134" s="3">
+        <v>134</v>
+      </c>
+      <c r="C134" s="3">
+        <v>2</v>
+      </c>
+      <c r="G134" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="H134" s="3">
+        <v>132</v>
+      </c>
+      <c r="J134" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J129">
+  <autoFilter ref="A1:J130">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
-    <sortState ref="A77:J126">
-      <sortCondition ref="C1:C122"/>
+    <sortState ref="A82:J131">
+      <sortCondition ref="C1:C130"/>
     </sortState>
   </autoFilter>
   <sortState ref="A44:J93">
     <sortCondition ref="C2:C93"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="J122" r:id="rId1"/>
+    <hyperlink ref="J124" r:id="rId1"/>
     <hyperlink ref="J96" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Issue #133 consistent import/export usage
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="20330" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="21400" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="241">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="241">
   <si>
     <t>#</t>
   </si>
@@ -1255,8 +1255,8 @@
   <dimension ref="A1:J134"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A82" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H131" sqref="H131"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E133" sqref="E133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3464,6 +3464,12 @@
       </c>
       <c r="C133" s="3">
         <v>2</v>
+      </c>
+      <c r="D133" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E133" s="7">
+        <v>43221</v>
       </c>
       <c r="G133" s="3" t="s">
         <v>235</v>

</xml_diff>

<commit_message>
Issue #109 better rounding funciton for slider
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="22470" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="24610" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="247">
   <si>
     <t>#</t>
   </si>
@@ -755,9 +755,6 @@
     <t>Rejig config service to be better</t>
   </si>
   <si>
-    <t>currently it is not really a service … should be a singleton.</t>
-  </si>
-  <si>
     <t>don’t forget to update the README.md file with the build instructions when you do
 I don’t really want the emulator code in the real version
 I do want the emulator code to call the server in the same way that Rpi will</t>
@@ -767,6 +764,26 @@
   </si>
   <si>
     <t>QUESTIONABLE</t>
+  </si>
+  <si>
+    <t>currently it is not really a service … should be a singleton.
+probably want to have clientConfig, commonConfig and other config (from Emulator or Rpi) passed in as parameters</t>
+  </si>
+  <si>
+    <t>Poss look at using git log being called from a rest service</t>
+  </si>
+  <si>
+    <t>Have better alternative for font awesome</t>
+  </si>
+  <si>
+    <t>using https://stackoverflow.com/questions/19401633/how-to-fire-an-event-on-class-change-using-jquery see notes on 5/5/2018</t>
+  </si>
+  <si>
+    <t>https://stackoverflow.com/questions/5186441/javascript-drag-and-drop-for-touch-devices
+https://medium.com/@asm/animated-slide-panel-with-angular-e985ad646f9</t>
+  </si>
+  <si>
+    <t>Have gone some way to this with the round … probably just need to add parameters to this … number.toFixed(2) looks promising. NOTE this will not be done using a pipe</t>
   </si>
 </sst>
 </file>
@@ -1255,11 +1272,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J134"/>
+  <dimension ref="A1:J135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A102" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G104" sqref="G104"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J112" sqref="J112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3068,15 +3085,24 @@
         <v>143</v>
       </c>
     </row>
-    <row r="106" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A106" s="3">
         <v>109</v>
       </c>
       <c r="C106" s="3">
         <v>2</v>
       </c>
+      <c r="D106" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E106" s="7">
+        <v>43229</v>
+      </c>
       <c r="G106" s="3" t="s">
         <v>194</v>
+      </c>
+      <c r="J106" s="3" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="107" spans="1:10" x14ac:dyDescent="0.35">
@@ -3194,6 +3220,9 @@
       <c r="G113" s="3" t="s">
         <v>176</v>
       </c>
+      <c r="J113" s="3" t="s">
+        <v>242</v>
+      </c>
     </row>
     <row r="114" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A114" s="3">
@@ -3319,7 +3348,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="122" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A122" s="3">
         <v>102</v>
       </c>
@@ -3328,6 +3357,9 @@
       </c>
       <c r="G122" s="3" t="s">
         <v>190</v>
+      </c>
+      <c r="J122" s="6" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.35">
@@ -3419,7 +3451,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A130" s="3">
         <v>128</v>
       </c>
@@ -3428,6 +3460,9 @@
       </c>
       <c r="G130" s="3" t="s">
         <v>228</v>
+      </c>
+      <c r="H130" s="3" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="131" spans="1:10" ht="58" x14ac:dyDescent="0.35">
@@ -3452,16 +3487,16 @@
         <v>1</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="G132" s="3" t="s">
         <v>234</v>
       </c>
       <c r="H132" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="J132" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="133" spans="1:10" ht="29" x14ac:dyDescent="0.35">
@@ -3498,7 +3533,21 @@
         <v>132</v>
       </c>
       <c r="J134" s="3" t="s">
-        <v>238</v>
+        <v>241</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A135" s="3">
+        <v>135</v>
+      </c>
+      <c r="C135" s="3">
+        <v>5</v>
+      </c>
+      <c r="G135" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="J135" s="3" t="s">
+        <v>244</v>
       </c>
     </row>
   </sheetData>
@@ -3516,8 +3565,9 @@
   <hyperlinks>
     <hyperlink ref="J124" r:id="rId1"/>
     <hyperlink ref="J96" r:id="rId2"/>
+    <hyperlink ref="J122" r:id="rId3" display="https://stackoverflow.com/questions/5186441/javascript-drag-and-drop-for-touch-devices"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Issue #121 add tslint
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="24610" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="25680" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="247">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="248">
   <si>
     <t>#</t>
   </si>
@@ -784,6 +784,9 @@
   </si>
   <si>
     <t>Have gone some way to this with the round … probably just need to add parameters to this … number.toFixed(2) looks promising. NOTE this will not be done using a pipe</t>
+  </si>
+  <si>
+    <t>Initial implementation and pass through of code</t>
   </si>
 </sst>
 </file>
@@ -1276,7 +1279,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J112" sqref="J112"/>
+      <selection pane="bottomLeft" activeCell="E119" sqref="E119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3310,8 +3313,17 @@
       <c r="C119" s="3">
         <v>3</v>
       </c>
+      <c r="D119" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E119" s="7">
+        <v>43229</v>
+      </c>
       <c r="G119" s="3" t="s">
         <v>215</v>
+      </c>
+      <c r="J119" s="3" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.35">
@@ -3471,6 +3483,12 @@
       </c>
       <c r="C131" s="3">
         <v>5</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E131" s="7">
+        <v>43229</v>
       </c>
       <c r="G131" s="3" t="s">
         <v>224</v>

</xml_diff>

<commit_message>
Issue #131 build type script release
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="25680" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="27820" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="250">
   <si>
     <t>#</t>
   </si>
@@ -787,6 +787,12 @@
   </si>
   <si>
     <t>Initial implementation and pass through of code</t>
+  </si>
+  <si>
+    <t>remove imports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Alignment option on detail edit of image missing from pi version </t>
   </si>
 </sst>
 </file>
@@ -1275,11 +1281,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J135"/>
+  <dimension ref="A1:J137"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E119" sqref="E119"/>
+      <selection pane="bottomLeft" activeCell="E82" sqref="E82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2714,6 +2720,12 @@
       <c r="C82" s="3">
         <v>1</v>
       </c>
+      <c r="D82" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E82" s="7">
+        <v>43231</v>
+      </c>
       <c r="G82" s="3" t="s">
         <v>233</v>
       </c>
@@ -3566,6 +3578,28 @@
       </c>
       <c r="J135" s="3" t="s">
         <v>244</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A136" s="3">
+        <v>136</v>
+      </c>
+      <c r="C136" s="3">
+        <v>5</v>
+      </c>
+      <c r="G136" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A137" s="3">
+        <v>137</v>
+      </c>
+      <c r="C137" s="3">
+        <v>1</v>
+      </c>
+      <c r="G137" s="3" t="s">
+        <v>249</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #139 copy index.html to correct place during build
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="27820" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="29960" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$J$130</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$J$138</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="413" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="252">
   <si>
     <t>#</t>
   </si>
@@ -793,6 +793,12 @@
   </si>
   <si>
     <t xml:space="preserve">Alignment option on detail edit of image missing from pi version </t>
+  </si>
+  <si>
+    <t>What to do with server common … delete it or reinstate it</t>
+  </si>
+  <si>
+    <t>copy index.html to correct place during build</t>
   </si>
 </sst>
 </file>
@@ -1281,11 +1287,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J137"/>
+  <dimension ref="A1:J139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E82" sqref="E82"/>
+      <selection pane="bottomLeft" activeCell="J102" sqref="J102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2713,7 +2719,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>131</v>
       </c>
@@ -3039,68 +3045,65 @@
         <v>181</v>
       </c>
     </row>
-    <row r="101" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A101" s="3">
-        <v>124</v>
+        <v>137</v>
       </c>
       <c r="C101" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A102" s="3">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="C102" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>231</v>
+        <v>250</v>
       </c>
     </row>
     <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="3">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C103" s="3">
         <v>2</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="J103" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="104" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" s="3">
-        <v>73</v>
+        <v>130</v>
       </c>
       <c r="C104" s="3">
         <v>2</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="I104" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="105" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="3">
-        <v>75</v>
+        <v>115</v>
       </c>
       <c r="C105" s="3">
         <v>2</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="106" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>206</v>
+      </c>
+      <c r="J105" s="3" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="106" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" s="3">
         <v>109</v>
       </c>
@@ -3120,21 +3123,18 @@
         <v>246</v>
       </c>
     </row>
-    <row r="107" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A107" s="3">
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="C107" s="3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
       <c r="I107" s="3" t="s">
         <v>6</v>
-      </c>
-      <c r="J107" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="108" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -3151,18 +3151,15 @@
         <v>193</v>
       </c>
     </row>
-    <row r="109" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A109" s="3">
-        <v>31</v>
+        <v>75</v>
       </c>
       <c r="C109" s="3">
-        <v>3</v>
-      </c>
-      <c r="F109" s="3" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>70</v>
+        <v>143</v>
       </c>
     </row>
     <row r="110" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
@@ -3205,63 +3202,72 @@
         <v>197</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A112" s="3">
-        <v>26</v>
+        <v>134</v>
       </c>
       <c r="C112" s="3">
-        <v>3</v>
-      </c>
-      <c r="F112" s="3" t="s">
-        <v>68</v>
+        <v>2</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="I112" s="3" t="s">
-        <v>99</v>
+        <v>237</v>
+      </c>
+      <c r="H112" s="3">
+        <v>132</v>
       </c>
       <c r="J112" s="3" t="s">
-        <v>156</v>
+        <v>241</v>
       </c>
     </row>
     <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" s="3">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C113" s="3">
         <v>3</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>176</v>
+        <v>130</v>
+      </c>
+      <c r="I113" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="J113" s="3" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="114" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" s="3">
-        <v>104</v>
+        <v>31</v>
       </c>
       <c r="C114" s="3">
         <v>3</v>
       </c>
+      <c r="F114" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="G114" s="3" t="s">
-        <v>186</v>
-      </c>
-      <c r="J114" s="3" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="115" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="115" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A115" s="3">
-        <v>105</v>
+        <v>26</v>
       </c>
       <c r="C115" s="3">
         <v>3</v>
       </c>
+      <c r="F115" s="3" t="s">
+        <v>68</v>
+      </c>
       <c r="G115" s="3" t="s">
-        <v>188</v>
+        <v>135</v>
+      </c>
+      <c r="I115" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="J115" s="3" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
@@ -3318,7 +3324,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="119" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" s="3">
         <v>121</v>
       </c>
@@ -3340,97 +3346,100 @@
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" s="3">
-        <v>40</v>
+        <v>96</v>
       </c>
       <c r="C120" s="3">
-        <v>4</v>
-      </c>
-      <c r="F120" s="3" t="s">
-        <v>85</v>
+        <v>3</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="J120" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="121" spans="1:10" x14ac:dyDescent="0.35">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="121" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A121" s="3">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="C121" s="3">
-        <v>4</v>
-      </c>
-      <c r="F121" s="3" t="s">
-        <v>31</v>
+        <v>3</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>62</v>
+        <v>186</v>
       </c>
       <c r="J121" s="3" t="s">
-        <v>61</v>
+        <v>187</v>
       </c>
     </row>
     <row r="122" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A122" s="3">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C122" s="3">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>190</v>
-      </c>
-      <c r="J122" s="6" t="s">
-        <v>245</v>
+        <v>188</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" s="3">
-        <v>97</v>
+        <v>40</v>
       </c>
       <c r="C123" s="3">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="F123" s="3" t="s">
+        <v>85</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="124" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>189</v>
+      </c>
+      <c r="J123" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" s="3">
-        <v>98</v>
+        <v>25</v>
       </c>
       <c r="C124" s="3">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="F124" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="J124" s="5" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="125" spans="1:10" x14ac:dyDescent="0.35">
+        <v>62</v>
+      </c>
+      <c r="J124" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="125" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A125" s="3">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C125" s="3">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>180</v>
+        <v>190</v>
+      </c>
+      <c r="J125" s="6" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" s="3">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C126" s="3">
         <v>5</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
     <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
@@ -3453,43 +3462,43 @@
         <v>225</v>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A128" s="3">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C128" s="3">
         <v>5</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>192</v>
+        <v>179</v>
+      </c>
+      <c r="J128" s="5" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" s="3">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="C129" s="3">
         <v>5</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="130" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" s="3">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="C130" s="3">
         <v>5</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>228</v>
-      </c>
-      <c r="H130" s="3" t="s">
-        <v>232</v>
-      </c>
-    </row>
-    <row r="131" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="131" spans="1:10" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" s="3">
         <v>129</v>
       </c>
@@ -3509,7 +3518,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="132" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:10" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" s="3">
         <v>132</v>
       </c>
@@ -3529,7 +3538,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="133" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" s="3">
         <v>133</v>
       </c>
@@ -3549,75 +3558,100 @@
         <v>236</v>
       </c>
     </row>
-    <row r="134" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A134" s="3">
-        <v>134</v>
+        <v>107</v>
       </c>
       <c r="C134" s="3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>237</v>
-      </c>
-      <c r="H134" s="3">
-        <v>132</v>
-      </c>
-      <c r="J134" s="3" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="135" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" s="3">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="C135" s="3">
         <v>5</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="J135" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="136" spans="1:10" x14ac:dyDescent="0.35">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="136" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A136" s="3">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C136" s="3">
         <v>5</v>
       </c>
       <c r="G136" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="H136" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="137" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A137" s="3">
+        <v>135</v>
+      </c>
+      <c r="C137" s="3">
+        <v>5</v>
+      </c>
+      <c r="G137" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="J137" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A138" s="3">
+        <v>136</v>
+      </c>
+      <c r="C138" s="3">
+        <v>5</v>
+      </c>
+      <c r="G138" s="3" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="137" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A137" s="3">
-        <v>137</v>
-      </c>
-      <c r="C137" s="3">
-        <v>1</v>
-      </c>
-      <c r="G137" s="3" t="s">
-        <v>249</v>
+    <row r="139" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A139" s="3">
+        <v>139</v>
+      </c>
+      <c r="C139" s="3">
+        <v>1</v>
+      </c>
+      <c r="D139" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E139" s="7">
+        <v>43231</v>
+      </c>
+      <c r="G139" s="3" t="s">
+        <v>251</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J130">
+  <autoFilter ref="A1:J138">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
-    <sortState ref="A82:J131">
-      <sortCondition ref="C1:C130"/>
+    <sortState ref="A101:J138">
+      <sortCondition ref="C1:C138"/>
     </sortState>
   </autoFilter>
   <sortState ref="A44:J93">
     <sortCondition ref="C2:C93"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="J124" r:id="rId1"/>
+    <hyperlink ref="J128" r:id="rId1"/>
     <hyperlink ref="J96" r:id="rId2"/>
-    <hyperlink ref="J122" r:id="rId3" display="https://stackoverflow.com/questions/5186441/javascript-drag-and-drop-for-touch-devices"/>
+    <hyperlink ref="J125" r:id="rId3" display="https://stackoverflow.com/questions/5186441/javascript-drag-and-drop-for-touch-devices"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>

</xml_diff>

<commit_message>
Issue #140 different alignment icons using iconmoon.
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="29960" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="32100" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="252">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="253">
   <si>
     <t>#</t>
   </si>
@@ -799,6 +799,9 @@
   </si>
   <si>
     <t>copy index.html to correct place during build</t>
+  </si>
+  <si>
+    <t>proper fix for alingnment icon</t>
   </si>
 </sst>
 </file>
@@ -1287,11 +1290,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J139"/>
+  <dimension ref="A1:J140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J102" sqref="J102"/>
+      <selection pane="bottomLeft" activeCell="E140" sqref="E140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3634,6 +3637,23 @@
       </c>
       <c r="G139" s="3" t="s">
         <v>251</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A140" s="3">
+        <v>140</v>
+      </c>
+      <c r="C140" s="3">
+        <v>1</v>
+      </c>
+      <c r="D140" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E140" s="7">
+        <v>43232</v>
+      </c>
+      <c r="G140" s="3" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #140 proper fix for alignment icon
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="32100" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="33170" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="255">
   <si>
     <t>#</t>
   </si>
@@ -802,6 +802,12 @@
   </si>
   <si>
     <t>proper fix for alingnment icon</t>
+  </si>
+  <si>
+    <t>Add right pad to image so that can then have repeat with pause.</t>
+  </si>
+  <si>
+    <t>Note this is a server and client change</t>
   </si>
 </sst>
 </file>
@@ -1290,11 +1296,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J140"/>
+  <dimension ref="A1:J141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E140" sqref="E140"/>
+      <selection pane="bottomLeft" activeCell="J141" sqref="J141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3654,6 +3660,20 @@
       </c>
       <c r="G140" s="3" t="s">
         <v>252</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A141" s="3">
+        <v>141</v>
+      </c>
+      <c r="C141" s="3">
+        <v>1</v>
+      </c>
+      <c r="G141" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="J141" s="3" t="s">
+        <v>254</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #141 add left and right padding to image client and server parts
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="33170" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="35310" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="420" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="256">
   <si>
     <t>#</t>
   </si>
@@ -808,6 +808,9 @@
   </si>
   <si>
     <t>Note this is a server and client change</t>
+  </si>
+  <si>
+    <t>TrackDTO and PlaylistDTO have different names on the server and the client app</t>
   </si>
 </sst>
 </file>
@@ -1296,11 +1299,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J141"/>
+  <dimension ref="A1:J142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J141" sqref="J141"/>
+      <selection pane="bottomLeft" activeCell="E141" sqref="E141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3669,11 +3672,28 @@
       <c r="C141" s="3">
         <v>1</v>
       </c>
+      <c r="D141" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E141" s="7">
+        <v>43234</v>
+      </c>
       <c r="G141" s="3" t="s">
         <v>253</v>
       </c>
       <c r="J141" s="3" t="s">
         <v>254</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+      <c r="A142" s="3">
+        <v>142</v>
+      </c>
+      <c r="C142" s="3">
+        <v>2</v>
+      </c>
+      <c r="G142" s="3" t="s">
+        <v>255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #142 rename DTO model files to be the same between editor and serverCommon
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\source\test\piWriterGIT2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\piWriter\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363AE025-E9FA-4CEB-A3D6-0088C1D80896}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35310" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="36480" yWindow="0" windowWidth="32745" windowHeight="14925" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$J$138</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$J$142</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="258">
   <si>
     <t>#</t>
   </si>
@@ -776,9 +777,6 @@
     <t>Have better alternative for font awesome</t>
   </si>
   <si>
-    <t>using https://stackoverflow.com/questions/19401633/how-to-fire-an-event-on-class-change-using-jquery see notes on 5/5/2018</t>
-  </si>
-  <si>
     <t>https://stackoverflow.com/questions/5186441/javascript-drag-and-drop-for-touch-devices
 https://medium.com/@asm/animated-slide-panel-with-angular-e985ad646f9</t>
   </si>
@@ -795,9 +793,6 @@
     <t xml:space="preserve">Alignment option on detail edit of image missing from pi version </t>
   </si>
   <si>
-    <t>What to do with server common … delete it or reinstate it</t>
-  </si>
-  <si>
     <t>copy index.html to correct place during build</t>
   </si>
   <si>
@@ -811,12 +806,25 @@
   </si>
   <si>
     <t>TrackDTO and PlaylistDTO have different names on the server and the client app</t>
+  </si>
+  <si>
+    <t>This was fixed with the iconmoon changes</t>
+  </si>
+  <si>
+    <t>What to do with serverEmulator … delete it or reinstate it</t>
+  </si>
+  <si>
+    <t>Delete it</t>
+  </si>
+  <si>
+    <t>using https://stackoverflow.com/questions/19401633/how-to-fire-an-event-on-class-change-using-jquery see notes on 5/5/2018
+This was done when the iconmoon change went in</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1210,22 +1218,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.08984375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.08984375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="84.6328125" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="8.7265625" style="3"/>
+    <col min="1" max="1" width="16.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="84.5703125" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1236,7 +1244,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1247,7 +1255,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1258,7 +1266,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -1269,7 +1277,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -1280,12 +1288,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -1297,28 +1305,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E141" sqref="E141"/>
+      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E142" sqref="E142"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="4" width="8.7265625" style="3"/>
-    <col min="5" max="5" width="10.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7265625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="22.81640625" style="3" customWidth="1"/>
+    <col min="1" max="4" width="8.7109375" style="3"/>
+    <col min="5" max="5" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" style="3" customWidth="1"/>
     <col min="8" max="8" width="10" style="3" customWidth="1"/>
-    <col min="9" max="9" width="15.6328125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="101.90625" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="8.7265625" style="3"/>
+    <col min="9" max="9" width="15.5703125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="101.85546875" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="8.7109375" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1350,7 +1358,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1367,7 +1375,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1390,7 +1398,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1413,7 +1421,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1430,7 +1438,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1447,7 +1455,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1467,7 +1475,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1484,7 +1492,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1504,7 +1512,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1518,7 +1526,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1538,7 +1546,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1555,7 +1563,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1572,7 +1580,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1589,7 +1597,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>44</v>
       </c>
@@ -1609,7 +1617,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1626,7 +1634,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1643,7 +1651,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1660,7 +1668,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1674,7 +1682,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1691,7 +1699,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1708,7 +1716,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1728,7 +1736,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1745,7 +1753,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>24</v>
       </c>
@@ -1765,7 +1773,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>67</v>
       </c>
@@ -1779,7 +1787,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
         <v>70</v>
       </c>
@@ -1796,7 +1804,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>27</v>
       </c>
@@ -1816,7 +1824,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>28</v>
       </c>
@@ -1833,7 +1841,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>29</v>
       </c>
@@ -1847,7 +1855,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>30</v>
       </c>
@@ -1861,7 +1869,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>31</v>
       </c>
@@ -1878,7 +1886,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>32</v>
       </c>
@@ -1895,7 +1903,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>39</v>
       </c>
@@ -1912,7 +1920,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -1929,7 +1937,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>35</v>
       </c>
@@ -1946,7 +1954,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
         <v>36</v>
       </c>
@@ -1963,7 +1971,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
         <v>37</v>
       </c>
@@ -1983,7 +1991,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>38</v>
       </c>
@@ -2000,7 +2008,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
         <v>43</v>
       </c>
@@ -2017,7 +2025,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
         <v>72</v>
       </c>
@@ -2034,7 +2042,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
         <v>41</v>
       </c>
@@ -2048,7 +2056,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
         <v>42</v>
       </c>
@@ -2065,7 +2073,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
         <v>74</v>
       </c>
@@ -2082,7 +2090,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
         <v>90</v>
       </c>
@@ -2096,7 +2104,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
         <v>45</v>
       </c>
@@ -2113,7 +2121,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
         <v>46</v>
       </c>
@@ -2130,7 +2138,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
         <v>58</v>
       </c>
@@ -2150,7 +2158,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>48</v>
       </c>
@@ -2167,7 +2175,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>91</v>
       </c>
@@ -2181,7 +2189,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>47</v>
       </c>
@@ -2201,7 +2209,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
         <v>51</v>
       </c>
@@ -2221,7 +2229,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>52</v>
       </c>
@@ -2241,7 +2249,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>53</v>
       </c>
@@ -2261,7 +2269,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>54</v>
       </c>
@@ -2284,7 +2292,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>55</v>
       </c>
@@ -2304,7 +2312,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>56</v>
       </c>
@@ -2321,7 +2329,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>57</v>
       </c>
@@ -2335,7 +2343,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>92</v>
       </c>
@@ -2349,7 +2357,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>59</v>
       </c>
@@ -2363,7 +2371,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>60</v>
       </c>
@@ -2383,7 +2391,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>49</v>
       </c>
@@ -2400,7 +2408,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
         <v>62</v>
       </c>
@@ -2414,7 +2422,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
         <v>63</v>
       </c>
@@ -2434,7 +2442,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
         <v>50</v>
       </c>
@@ -2451,7 +2459,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
         <v>65</v>
       </c>
@@ -2462,7 +2470,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
         <v>66</v>
       </c>
@@ -2473,7 +2481,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
         <v>64</v>
       </c>
@@ -2490,7 +2498,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
         <v>68</v>
       </c>
@@ -2501,7 +2509,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
         <v>93</v>
       </c>
@@ -2515,7 +2523,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
         <v>77</v>
       </c>
@@ -2535,7 +2543,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
         <v>71</v>
       </c>
@@ -2552,7 +2560,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
         <v>69</v>
       </c>
@@ -2575,7 +2583,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
         <v>80</v>
       </c>
@@ -2598,7 +2606,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
         <v>81</v>
       </c>
@@ -2618,7 +2626,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
         <v>61</v>
       </c>
@@ -2632,7 +2640,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
         <v>76</v>
       </c>
@@ -2649,7 +2657,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
         <v>125</v>
       </c>
@@ -2666,7 +2674,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
         <v>78</v>
       </c>
@@ -2680,7 +2688,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
         <v>79</v>
       </c>
@@ -2691,7 +2699,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
         <v>113</v>
       </c>
@@ -2711,7 +2719,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
         <v>123</v>
       </c>
@@ -2731,7 +2739,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
         <v>131</v>
       </c>
@@ -2748,7 +2756,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
         <v>83</v>
       </c>
@@ -2762,7 +2770,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
         <v>84</v>
       </c>
@@ -2776,7 +2784,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
         <v>85</v>
       </c>
@@ -2793,7 +2801,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
         <v>86</v>
       </c>
@@ -2807,7 +2815,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
         <v>87</v>
       </c>
@@ -2824,7 +2832,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
         <v>88</v>
       </c>
@@ -2841,7 +2849,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
         <v>126</v>
       </c>
@@ -2861,7 +2869,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
         <v>122</v>
       </c>
@@ -2878,7 +2886,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
         <v>119</v>
       </c>
@@ -2901,7 +2909,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
         <v>82</v>
       </c>
@@ -2918,7 +2926,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
         <v>89</v>
       </c>
@@ -2932,7 +2940,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
         <v>94</v>
       </c>
@@ -2946,7 +2954,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
         <v>95</v>
       </c>
@@ -2960,7 +2968,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
         <v>103</v>
       </c>
@@ -2977,7 +2985,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
         <v>120</v>
       </c>
@@ -3000,7 +3008,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
         <v>112</v>
       </c>
@@ -3020,7 +3028,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
         <v>101</v>
       </c>
@@ -3043,7 +3051,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
         <v>100</v>
       </c>
@@ -3057,29 +3065,44 @@
         <v>181</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>137</v>
       </c>
       <c r="C101" s="3">
         <v>1</v>
       </c>
+      <c r="D101" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="G101" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="102" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+        <v>248</v>
+      </c>
+      <c r="J101" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="102" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>138</v>
       </c>
       <c r="C102" s="3">
         <v>1</v>
       </c>
+      <c r="D102" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E102" s="7">
+        <v>43236</v>
+      </c>
       <c r="G102" s="3" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
+        <v>255</v>
+      </c>
+      <c r="J102" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="103" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
         <v>124</v>
       </c>
@@ -3090,7 +3113,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
         <v>130</v>
       </c>
@@ -3101,7 +3124,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
         <v>115</v>
       </c>
@@ -3115,7 +3138,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
         <v>109</v>
       </c>
@@ -3132,10 +3155,10 @@
         <v>194</v>
       </c>
       <c r="J106" s="3" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="107" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="107" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
         <v>73</v>
       </c>
@@ -3149,7 +3172,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
         <v>108</v>
       </c>
@@ -3163,7 +3186,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
         <v>75</v>
       </c>
@@ -3174,7 +3197,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
         <v>110</v>
       </c>
@@ -3197,7 +3220,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
         <v>111</v>
       </c>
@@ -3214,7 +3237,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
         <v>134</v>
       </c>
@@ -3231,7 +3254,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
         <v>14</v>
       </c>
@@ -3248,7 +3271,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
         <v>31</v>
       </c>
@@ -3262,7 +3285,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
         <v>26</v>
       </c>
@@ -3282,7 +3305,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
         <v>116</v>
       </c>
@@ -3302,7 +3325,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
         <v>117</v>
       </c>
@@ -3319,7 +3342,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
         <v>118</v>
       </c>
@@ -3336,7 +3359,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
         <v>121</v>
       </c>
@@ -3353,10 +3376,10 @@
         <v>215</v>
       </c>
       <c r="J119" s="3" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="120" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
         <v>96</v>
       </c>
@@ -3370,7 +3393,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
         <v>104</v>
       </c>
@@ -3384,7 +3407,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
         <v>105</v>
       </c>
@@ -3395,7 +3418,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
         <v>40</v>
       </c>
@@ -3412,7 +3435,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
         <v>25</v>
       </c>
@@ -3429,7 +3452,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="125" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
         <v>102</v>
       </c>
@@ -3440,10 +3463,10 @@
         <v>190</v>
       </c>
       <c r="J125" s="6" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="126" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
         <v>97</v>
       </c>
@@ -3454,7 +3477,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
         <v>127</v>
       </c>
@@ -3474,7 +3497,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
         <v>98</v>
       </c>
@@ -3488,7 +3511,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
         <v>99</v>
       </c>
@@ -3499,7 +3522,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
         <v>106</v>
       </c>
@@ -3510,7 +3533,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="131" spans="1:10" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
         <v>129</v>
       </c>
@@ -3530,7 +3553,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="132" spans="1:10" ht="58" hidden="1" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
         <v>132</v>
       </c>
@@ -3550,7 +3573,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="133" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
         <v>133</v>
       </c>
@@ -3570,7 +3593,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="134" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
         <v>107</v>
       </c>
@@ -3581,7 +3604,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
         <v>114</v>
       </c>
@@ -3592,7 +3615,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="136" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
         <v>128</v>
       </c>
@@ -3606,21 +3629,24 @@
         <v>232</v>
       </c>
     </row>
-    <row r="137" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>135</v>
       </c>
       <c r="C137" s="3">
         <v>5</v>
       </c>
+      <c r="D137" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="G137" s="3" t="s">
         <v>243</v>
       </c>
       <c r="J137" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
         <v>136</v>
       </c>
@@ -3628,10 +3654,10 @@
         <v>5</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="139" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="139" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
         <v>139</v>
       </c>
@@ -3645,10 +3671,10 @@
         <v>43231</v>
       </c>
       <c r="G139" s="3" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="140" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="140" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
         <v>140</v>
       </c>
@@ -3662,10 +3688,10 @@
         <v>43232</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="141" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="141" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
         <v>141</v>
       </c>
@@ -3679,25 +3705,31 @@
         <v>43234</v>
       </c>
       <c r="G141" s="3" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J141" s="3" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="142" spans="1:10" ht="58" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="142" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
         <v>142</v>
       </c>
       <c r="C142" s="3">
         <v>2</v>
       </c>
+      <c r="D142" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E142" s="7">
+        <v>43236</v>
+      </c>
       <c r="G142" s="3" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J138">
+  <autoFilter ref="A1:J142" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
@@ -3709,9 +3741,9 @@
     <sortCondition ref="C2:C93"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="J128" r:id="rId1"/>
-    <hyperlink ref="J96" r:id="rId2"/>
-    <hyperlink ref="J125" r:id="rId3" display="https://stackoverflow.com/questions/5186441/javascript-drag-and-drop-for-touch-devices"/>
+    <hyperlink ref="J128" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="J96" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="J125" r:id="rId3" display="https://stackoverflow.com/questions/5186441/javascript-drag-and-drop-for-touch-devices" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>

</xml_diff>

<commit_message>
Issue #143 ServerInfo server side
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\piWriter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{363AE025-E9FA-4CEB-A3D6-0088C1D80896}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324015B4-26C6-4076-8657-4779C1493BDD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="36480" yWindow="0" windowWidth="32745" windowHeight="14925" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="37650" yWindow="0" windowWidth="32745" windowHeight="14925" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="428" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="261">
   <si>
     <t>#</t>
   </si>
@@ -819,6 +819,15 @@
   <si>
     <t>using https://stackoverflow.com/questions/19401633/how-to-fire-an-event-on-class-change-using-jquery see notes on 5/5/2018
 This was done when the iconmoon change went in</t>
+  </si>
+  <si>
+    <t>With the change to the compiled ts the boot time is down to 30s which is sufficient at the moment.</t>
+  </si>
+  <si>
+    <t>ServerInfo server side</t>
+  </si>
+  <si>
+    <t>ServerInfo client side</t>
   </si>
 </sst>
 </file>
@@ -1307,11 +1316,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J142"/>
+  <dimension ref="A1:J144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E142" sqref="E142"/>
+      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D147" sqref="D147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3065,7 +3074,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
         <v>137</v>
       </c>
@@ -3082,7 +3091,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
         <v>138</v>
       </c>
@@ -3518,8 +3527,14 @@
       <c r="C129" s="3">
         <v>5</v>
       </c>
+      <c r="D129" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="G129" s="3" t="s">
         <v>180</v>
+      </c>
+      <c r="J129" s="3" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="130" spans="1:10" x14ac:dyDescent="0.25">
@@ -3629,7 +3644,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="137" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
         <v>135</v>
       </c>
@@ -3711,7 +3726,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
         <v>142</v>
       </c>
@@ -3726,6 +3741,35 @@
       </c>
       <c r="G142" s="3" t="s">
         <v>253</v>
+      </c>
+    </row>
+    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A143" s="3">
+        <v>143</v>
+      </c>
+      <c r="C143" s="3">
+        <v>1</v>
+      </c>
+      <c r="D143" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E143" s="7">
+        <v>43236</v>
+      </c>
+      <c r="G143" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A144" s="3">
+        <v>144</v>
+      </c>
+      <c r="C144" s="3">
+        <v>1</v>
+      </c>
+      <c r="E144" s="7"/>
+      <c r="G144" s="3" t="s">
+        <v>260</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #144 server side of ServerInfo
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\piWriter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{324015B4-26C6-4076-8657-4779C1493BDD}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7076DDD-481B-4E29-AB61-6DE7C5C73F6A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37650" yWindow="0" windowWidth="32745" windowHeight="14925" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="39990" yWindow="0" windowWidth="32745" windowHeight="14925" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="261">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="265">
   <si>
     <t>#</t>
   </si>
@@ -828,6 +828,18 @@
   </si>
   <si>
     <t>ServerInfo client side</t>
+  </si>
+  <si>
+    <t>ServerInfo Rpi</t>
+  </si>
+  <si>
+    <t>in editor wrapGet should be moved to the utilities package</t>
+  </si>
+  <si>
+    <t>Config in serverCommon should be moved to its own package</t>
+  </si>
+  <si>
+    <t>serverInfoDTO in editor should be reused in server</t>
   </si>
 </sst>
 </file>
@@ -1316,11 +1328,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J144"/>
+  <dimension ref="A1:J148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A120" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D147" sqref="D147"/>
+      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E155" sqref="E153:E155"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3767,9 +3779,58 @@
       <c r="C144" s="3">
         <v>1</v>
       </c>
-      <c r="E144" s="7"/>
+      <c r="D144" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E144" s="7">
+        <v>43238</v>
+      </c>
       <c r="G144" s="3" t="s">
         <v>260</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A145" s="3">
+        <v>145</v>
+      </c>
+      <c r="C145" s="3">
+        <v>1</v>
+      </c>
+      <c r="G145" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A146" s="3">
+        <v>146</v>
+      </c>
+      <c r="C146" s="3">
+        <v>2</v>
+      </c>
+      <c r="G146" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A147" s="3">
+        <v>147</v>
+      </c>
+      <c r="C147" s="3">
+        <v>2</v>
+      </c>
+      <c r="G147" s="3" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A148" s="3">
+        <v>148</v>
+      </c>
+      <c r="C148" s="3">
+        <v>2</v>
+      </c>
+      <c r="G148" s="3" t="s">
+        <v>264</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #149 move wrap post to utilities
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\piWriter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7076DDD-481B-4E29-AB61-6DE7C5C73F6A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD598C5C-3F7E-46DB-865A-861D4DD8EF76}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39990" yWindow="0" windowWidth="32745" windowHeight="14925" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="41160" yWindow="0" windowWidth="32745" windowHeight="14925" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="438" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="267">
   <si>
     <t>#</t>
   </si>
@@ -840,6 +840,12 @@
   </si>
   <si>
     <t>serverInfoDTO in editor should be reused in server</t>
+  </si>
+  <si>
+    <t>Playlistrepo should use get Wrapped methods in utility</t>
+  </si>
+  <si>
+    <t>move wrap post to utilities</t>
   </si>
 </sst>
 </file>
@@ -1328,11 +1334,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J148"/>
+  <dimension ref="A1:J150"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E155" sqref="E153:E155"/>
+      <selection pane="bottomLeft" activeCell="G149" sqref="G149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3807,6 +3813,12 @@
       <c r="C146" s="3">
         <v>2</v>
       </c>
+      <c r="D146" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E146" s="7">
+        <v>43238</v>
+      </c>
       <c r="G146" s="3" t="s">
         <v>262</v>
       </c>
@@ -3831,6 +3843,31 @@
       </c>
       <c r="G148" s="3" t="s">
         <v>264</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A149" s="3">
+        <v>149</v>
+      </c>
+      <c r="C149" s="3">
+        <v>1</v>
+      </c>
+      <c r="D149" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E149" s="7">
+        <v>43238</v>
+      </c>
+      <c r="G149" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A150" s="3">
+        <v>150</v>
+      </c>
+      <c r="G150" s="3" t="s">
+        <v>265</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #151 Jimp changes to image on angular client
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18431"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\source\piWriter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\source\test\piWriterGIT2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD598C5C-3F7E-46DB-865A-861D4DD8EF76}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="41160" yWindow="0" windowWidth="32745" windowHeight="14925" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42560" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="268">
   <si>
     <t>#</t>
   </si>
@@ -847,11 +846,14 @@
   <si>
     <t>move wrap post to utilities</t>
   </si>
+  <si>
+    <t>Better image handling on client using JIMP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1245,22 +1247,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="84.5703125" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="8.7109375" style="3"/>
+    <col min="1" max="1" width="16.1796875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="84.54296875" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1271,7 +1273,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
@@ -1282,7 +1284,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>6</v>
       </c>
@@ -1293,7 +1295,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>13</v>
       </c>
@@ -1304,7 +1306,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -1315,12 +1317,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -1332,28 +1334,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J150"/>
+  <dimension ref="A1:J151"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G149" sqref="G149"/>
+      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F154" sqref="F153:F154"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="4" width="8.7109375" style="3"/>
-    <col min="5" max="5" width="10.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="22.85546875" style="3" customWidth="1"/>
+    <col min="1" max="4" width="8.7265625" style="3"/>
+    <col min="5" max="5" width="10.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.7265625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="22.81640625" style="3" customWidth="1"/>
     <col min="8" max="8" width="10" style="3" customWidth="1"/>
-    <col min="9" max="9" width="15.5703125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="101.85546875" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="8.7109375" style="3"/>
+    <col min="9" max="9" width="15.54296875" style="3" customWidth="1"/>
+    <col min="10" max="10" width="101.81640625" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1385,7 +1387,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1402,7 +1404,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1425,7 +1427,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1448,7 +1450,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1465,7 +1467,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1482,7 +1484,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1502,7 +1504,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1519,7 +1521,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1539,7 +1541,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1553,7 +1555,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1573,7 +1575,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3">
         <v>11</v>
       </c>
@@ -1590,7 +1592,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3">
         <v>12</v>
       </c>
@@ -1607,7 +1609,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3">
         <v>13</v>
       </c>
@@ -1624,7 +1626,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3">
         <v>44</v>
       </c>
@@ -1644,7 +1646,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -1661,7 +1663,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -1678,7 +1680,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3">
         <v>17</v>
       </c>
@@ -1695,7 +1697,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3">
         <v>18</v>
       </c>
@@ -1709,7 +1711,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3">
         <v>19</v>
       </c>
@@ -1726,7 +1728,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3">
         <v>20</v>
       </c>
@@ -1743,7 +1745,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="3">
         <v>21</v>
       </c>
@@ -1763,7 +1765,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3">
         <v>22</v>
       </c>
@@ -1780,7 +1782,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="3">
         <v>24</v>
       </c>
@@ -1800,7 +1802,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="25" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3">
         <v>67</v>
       </c>
@@ -1814,7 +1816,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="3">
         <v>70</v>
       </c>
@@ -1831,7 +1833,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="3">
         <v>27</v>
       </c>
@@ -1851,7 +1853,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3">
         <v>28</v>
       </c>
@@ -1868,7 +1870,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3">
         <v>29</v>
       </c>
@@ -1882,7 +1884,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3">
         <v>30</v>
       </c>
@@ -1896,7 +1898,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="3">
         <v>31</v>
       </c>
@@ -1913,7 +1915,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="3">
         <v>32</v>
       </c>
@@ -1930,7 +1932,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="3">
         <v>39</v>
       </c>
@@ -1947,7 +1949,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="3">
         <v>33</v>
       </c>
@@ -1964,7 +1966,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="3">
         <v>35</v>
       </c>
@@ -1981,7 +1983,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="3">
         <v>36</v>
       </c>
@@ -1998,7 +2000,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3">
         <v>37</v>
       </c>
@@ -2018,7 +2020,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="38" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="3">
         <v>38</v>
       </c>
@@ -2035,7 +2037,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="39" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3">
         <v>43</v>
       </c>
@@ -2052,7 +2054,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3">
         <v>72</v>
       </c>
@@ -2069,7 +2071,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3">
         <v>41</v>
       </c>
@@ -2083,7 +2085,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3">
         <v>42</v>
       </c>
@@ -2100,7 +2102,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3">
         <v>74</v>
       </c>
@@ -2117,7 +2119,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="44" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3">
         <v>90</v>
       </c>
@@ -2131,7 +2133,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="45" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="3">
         <v>45</v>
       </c>
@@ -2148,7 +2150,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3">
         <v>46</v>
       </c>
@@ -2165,7 +2167,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="3">
         <v>58</v>
       </c>
@@ -2185,7 +2187,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="3">
         <v>48</v>
       </c>
@@ -2202,7 +2204,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3">
         <v>91</v>
       </c>
@@ -2216,7 +2218,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="50" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="3">
         <v>47</v>
       </c>
@@ -2236,7 +2238,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="51" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3">
         <v>51</v>
       </c>
@@ -2256,7 +2258,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="52" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="3">
         <v>52</v>
       </c>
@@ -2276,7 +2278,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="53" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="3">
         <v>53</v>
       </c>
@@ -2296,7 +2298,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="54" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="3">
         <v>54</v>
       </c>
@@ -2319,7 +2321,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="55" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3">
         <v>55</v>
       </c>
@@ -2339,7 +2341,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="56" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3">
         <v>56</v>
       </c>
@@ -2356,7 +2358,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="3">
         <v>57</v>
       </c>
@@ -2370,7 +2372,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3">
         <v>92</v>
       </c>
@@ -2384,7 +2386,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="59" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="3">
         <v>59</v>
       </c>
@@ -2398,7 +2400,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="60" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="3">
         <v>60</v>
       </c>
@@ -2418,7 +2420,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="3">
         <v>49</v>
       </c>
@@ -2435,7 +2437,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="3">
         <v>62</v>
       </c>
@@ -2449,7 +2451,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="63" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="3">
         <v>63</v>
       </c>
@@ -2469,7 +2471,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="3">
         <v>50</v>
       </c>
@@ -2486,7 +2488,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="65" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="3">
         <v>65</v>
       </c>
@@ -2497,7 +2499,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="66" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="3">
         <v>66</v>
       </c>
@@ -2508,7 +2510,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="3">
         <v>64</v>
       </c>
@@ -2525,7 +2527,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="68" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="3">
         <v>68</v>
       </c>
@@ -2536,7 +2538,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="69" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="3">
         <v>93</v>
       </c>
@@ -2550,7 +2552,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="70" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="3">
         <v>77</v>
       </c>
@@ -2570,7 +2572,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="3">
         <v>71</v>
       </c>
@@ -2587,7 +2589,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="72" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="3">
         <v>69</v>
       </c>
@@ -2610,7 +2612,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="3">
         <v>80</v>
       </c>
@@ -2633,7 +2635,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="3">
         <v>81</v>
       </c>
@@ -2653,7 +2655,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="75" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="3">
         <v>61</v>
       </c>
@@ -2667,7 +2669,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="76" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="3">
         <v>76</v>
       </c>
@@ -2684,7 +2686,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="77" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="3">
         <v>125</v>
       </c>
@@ -2701,7 +2703,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="78" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="3">
         <v>78</v>
       </c>
@@ -2715,7 +2717,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="79" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="3">
         <v>79</v>
       </c>
@@ -2726,7 +2728,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="80" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="3">
         <v>113</v>
       </c>
@@ -2746,7 +2748,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="3">
         <v>123</v>
       </c>
@@ -2766,7 +2768,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="82" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="3">
         <v>131</v>
       </c>
@@ -2783,7 +2785,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="3">
         <v>83</v>
       </c>
@@ -2797,7 +2799,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="84" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="3">
         <v>84</v>
       </c>
@@ -2811,7 +2813,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="85" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="3">
         <v>85</v>
       </c>
@@ -2828,7 +2830,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="86" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="3">
         <v>86</v>
       </c>
@@ -2842,7 +2844,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="87" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="3">
         <v>87</v>
       </c>
@@ -2859,7 +2861,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="88" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="3">
         <v>88</v>
       </c>
@@ -2876,7 +2878,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="89" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:10" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="3">
         <v>126</v>
       </c>
@@ -2896,7 +2898,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="3">
         <v>122</v>
       </c>
@@ -2913,7 +2915,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="91" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="3">
         <v>119</v>
       </c>
@@ -2936,7 +2938,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="3">
         <v>82</v>
       </c>
@@ -2953,7 +2955,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="93" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" s="3">
         <v>89</v>
       </c>
@@ -2967,7 +2969,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="94" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="3">
         <v>94</v>
       </c>
@@ -2981,7 +2983,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" s="3">
         <v>95</v>
       </c>
@@ -2995,7 +2997,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" s="3">
         <v>103</v>
       </c>
@@ -3012,7 +3014,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="97" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="3">
         <v>120</v>
       </c>
@@ -3035,7 +3037,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" s="3">
         <v>112</v>
       </c>
@@ -3055,7 +3057,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="3">
         <v>101</v>
       </c>
@@ -3078,7 +3080,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="100" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:10" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" s="3">
         <v>100</v>
       </c>
@@ -3092,7 +3094,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="101" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" s="3">
         <v>137</v>
       </c>
@@ -3109,7 +3111,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="102" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" s="3">
         <v>138</v>
       </c>
@@ -3129,7 +3131,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="103" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A103" s="3">
         <v>124</v>
       </c>
@@ -3140,7 +3142,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="104" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A104" s="3">
         <v>130</v>
       </c>
@@ -3151,7 +3153,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="105" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A105" s="3">
         <v>115</v>
       </c>
@@ -3165,7 +3167,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="106" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" s="3">
         <v>109</v>
       </c>
@@ -3185,7 +3187,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="107" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A107" s="3">
         <v>73</v>
       </c>
@@ -3199,7 +3201,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="108" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" s="3">
         <v>108</v>
       </c>
@@ -3213,7 +3215,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="109" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A109" s="3">
         <v>75</v>
       </c>
@@ -3224,7 +3226,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="110" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" s="3">
         <v>110</v>
       </c>
@@ -3247,7 +3249,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="111" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="3">
         <v>111</v>
       </c>
@@ -3264,7 +3266,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="112" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A112" s="3">
         <v>134</v>
       </c>
@@ -3281,7 +3283,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="113" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A113" s="3">
         <v>14</v>
       </c>
@@ -3298,7 +3300,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="114" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A114" s="3">
         <v>31</v>
       </c>
@@ -3312,7 +3314,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="115" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:10" ht="58" x14ac:dyDescent="0.35">
       <c r="A115" s="3">
         <v>26</v>
       </c>
@@ -3332,7 +3334,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116" s="3">
         <v>116</v>
       </c>
@@ -3352,7 +3354,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="117" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117" s="3">
         <v>117</v>
       </c>
@@ -3369,7 +3371,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="118" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118" s="3">
         <v>118</v>
       </c>
@@ -3386,7 +3388,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119" s="3">
         <v>121</v>
       </c>
@@ -3406,7 +3408,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="120" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A120" s="3">
         <v>96</v>
       </c>
@@ -3420,7 +3422,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="121" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A121" s="3">
         <v>104</v>
       </c>
@@ -3434,7 +3436,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="122" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A122" s="3">
         <v>105</v>
       </c>
@@ -3445,7 +3447,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="123" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A123" s="3">
         <v>40</v>
       </c>
@@ -3462,7 +3464,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="124" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A124" s="3">
         <v>25</v>
       </c>
@@ -3479,7 +3481,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="125" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A125" s="3">
         <v>102</v>
       </c>
@@ -3493,7 +3495,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="126" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A126" s="3">
         <v>97</v>
       </c>
@@ -3504,7 +3506,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127" s="3">
         <v>127</v>
       </c>
@@ -3524,7 +3526,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="128" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A128" s="3">
         <v>98</v>
       </c>
@@ -3538,7 +3540,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A129" s="3">
         <v>99</v>
       </c>
@@ -3555,7 +3557,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="130" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A130" s="3">
         <v>106</v>
       </c>
@@ -3566,7 +3568,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="131" spans="1:10" ht="60" hidden="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:10" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131" s="3">
         <v>129</v>
       </c>
@@ -3586,7 +3588,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="132" spans="1:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:10" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132" s="3">
         <v>132</v>
       </c>
@@ -3606,7 +3608,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="133" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133" s="3">
         <v>133</v>
       </c>
@@ -3626,7 +3628,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="134" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A134" s="3">
         <v>107</v>
       </c>
@@ -3637,7 +3639,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="135" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A135" s="3">
         <v>114</v>
       </c>
@@ -3648,7 +3650,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="136" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A136" s="3">
         <v>128</v>
       </c>
@@ -3662,7 +3664,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="137" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A137" s="3">
         <v>135</v>
       </c>
@@ -3679,7 +3681,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="138" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A138" s="3">
         <v>136</v>
       </c>
@@ -3690,7 +3692,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="139" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A139" s="3">
         <v>139</v>
       </c>
@@ -3707,7 +3709,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="140" spans="1:10" ht="30" hidden="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A140" s="3">
         <v>140</v>
       </c>
@@ -3724,7 +3726,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="141" spans="1:10" ht="45" hidden="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A141" s="3">
         <v>141</v>
       </c>
@@ -3744,7 +3746,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="142" spans="1:10" ht="75" hidden="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:10" ht="58" hidden="1" x14ac:dyDescent="0.35">
       <c r="A142" s="3">
         <v>142</v>
       </c>
@@ -3761,7 +3763,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A143" s="3">
         <v>143</v>
       </c>
@@ -3778,7 +3780,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A144" s="3">
         <v>144</v>
       </c>
@@ -3795,7 +3797,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A145" s="3">
         <v>145</v>
       </c>
@@ -3806,7 +3808,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A146" s="3">
         <v>146</v>
       </c>
@@ -3823,7 +3825,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A147" s="3">
         <v>147</v>
       </c>
@@ -3834,7 +3836,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A148" s="3">
         <v>148</v>
       </c>
@@ -3845,7 +3847,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" ht="29" x14ac:dyDescent="0.35">
       <c r="A149" s="3">
         <v>149</v>
       </c>
@@ -3862,16 +3864,36 @@
         <v>266</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A150" s="3">
         <v>150</v>
       </c>
+      <c r="C150" s="3">
+        <v>1</v>
+      </c>
       <c r="G150" s="3" t="s">
         <v>265</v>
       </c>
     </row>
+    <row r="151" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A151" s="3">
+        <v>151</v>
+      </c>
+      <c r="C151" s="3">
+        <v>1</v>
+      </c>
+      <c r="D151" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E151" s="7">
+        <v>43241</v>
+      </c>
+      <c r="G151" s="3" t="s">
+        <v>267</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J142" xr:uid="{00000000-0009-0000-0000-000001000000}">
+  <autoFilter ref="A1:J142">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>
@@ -3883,9 +3905,9 @@
     <sortCondition ref="C2:C93"/>
   </sortState>
   <hyperlinks>
-    <hyperlink ref="J128" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
-    <hyperlink ref="J96" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
-    <hyperlink ref="J125" r:id="rId3" display="https://stackoverflow.com/questions/5186441/javascript-drag-and-drop-for-touch-devices" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="J128" r:id="rId1"/>
+    <hyperlink ref="J96" r:id="rId2"/>
+    <hyperlink ref="J125" r:id="rId3" display="https://stackoverflow.com/questions/5186441/javascript-drag-and-drop-for-touch-devices"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId4"/>

</xml_diff>

<commit_message>
Issue #152 Client side recolor and stripes
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="42560" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="43960" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="270">
   <si>
     <t>#</t>
   </si>
@@ -848,6 +848,12 @@
   </si>
   <si>
     <t>Better image handling on client using JIMP</t>
+  </si>
+  <si>
+    <t>Client side recolor and stripes</t>
+  </si>
+  <si>
+    <t>Server side recolor and stripes</t>
   </si>
 </sst>
 </file>
@@ -1336,11 +1342,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J151"/>
+  <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A123" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F154" sqref="F153:F154"/>
+      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G157" sqref="G156:G157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3890,6 +3896,34 @@
       </c>
       <c r="G151" s="3" t="s">
         <v>267</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A152" s="3">
+        <v>152</v>
+      </c>
+      <c r="C152" s="3">
+        <v>1</v>
+      </c>
+      <c r="D152" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E152" s="7">
+        <v>43242</v>
+      </c>
+      <c r="G152" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A153" s="3">
+        <v>153</v>
+      </c>
+      <c r="C153" s="3">
+        <v>1</v>
+      </c>
+      <c r="G153" s="3" t="s">
+        <v>269</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #145 RPi serverInfo implementation
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="43960" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="45360" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="270">
   <si>
     <t>#</t>
   </si>
@@ -1345,8 +1345,8 @@
   <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A126" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G157" sqref="G156:G157"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E135" sqref="E135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3809,6 +3809,12 @@
       </c>
       <c r="C145" s="3">
         <v>1</v>
+      </c>
+      <c r="D145" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E145" s="7">
+        <v>43243</v>
       </c>
       <c r="G145" s="3" t="s">
         <v>261</v>

</xml_diff>

<commit_message>
Issue #154 ng build error
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="272">
   <si>
     <t>#</t>
   </si>
@@ -854,6 +854,12 @@
   </si>
   <si>
     <t>Server side recolor and stripes</t>
+  </si>
+  <si>
+    <t>Angular app build error</t>
+  </si>
+  <si>
+    <t>srcOut needed to be public</t>
   </si>
 </sst>
 </file>
@@ -1342,11 +1348,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J153"/>
+  <dimension ref="A1:J154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E135" sqref="E135"/>
+      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J154" sqref="J154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3803,7 +3809,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A145" s="3">
         <v>145</v>
       </c>
@@ -3820,7 +3826,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A146" s="3">
         <v>146</v>
       </c>
@@ -3837,7 +3843,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A147" s="3">
         <v>147</v>
       </c>
@@ -3848,7 +3854,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A148" s="3">
         <v>148</v>
       </c>
@@ -3859,7 +3865,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A149" s="3">
         <v>149</v>
       </c>
@@ -3876,7 +3882,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A150" s="3">
         <v>150</v>
       </c>
@@ -3887,7 +3893,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A151" s="3">
         <v>151</v>
       </c>
@@ -3904,7 +3910,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A152" s="3">
         <v>152</v>
       </c>
@@ -3921,7 +3927,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:10" ht="29" x14ac:dyDescent="0.35">
       <c r="A153" s="3">
         <v>153</v>
       </c>
@@ -3930,6 +3936,26 @@
       </c>
       <c r="G153" s="3" t="s">
         <v>269</v>
+      </c>
+    </row>
+    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A154" s="3">
+        <v>154</v>
+      </c>
+      <c r="C154" s="3">
+        <v>1</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E154" s="7">
+        <v>43243</v>
+      </c>
+      <c r="G154" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="J154" s="3" t="s">
+        <v>271</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Issue #153 Server side recolor and stripes
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="45360" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="49560" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
     <sheet name="Issues" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$J$142</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Issues!$A$1:$J$155</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="275">
   <si>
     <t>#</t>
   </si>
@@ -860,6 +860,15 @@
   </si>
   <si>
     <t>srcOut needed to be public</t>
+  </si>
+  <si>
+    <t>Better commonality for the JIMP processing for the client and server</t>
+  </si>
+  <si>
+    <t>Preview track on phone</t>
+  </si>
+  <si>
+    <t>Disk usage as part of server stats</t>
   </si>
 </sst>
 </file>
@@ -1348,11 +1357,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J154"/>
+  <dimension ref="A1:J157"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A144" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J154" sqref="J154"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G153" sqref="G153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3552,7 +3561,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="129" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129" s="3">
         <v>99</v>
       </c>
@@ -3775,7 +3784,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="143" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A143" s="3">
         <v>143</v>
       </c>
@@ -3792,7 +3801,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="144" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A144" s="3">
         <v>144</v>
       </c>
@@ -3809,7 +3818,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="145" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A145" s="3">
         <v>145</v>
       </c>
@@ -3826,7 +3835,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="146" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:10" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A146" s="3">
         <v>146</v>
       </c>
@@ -3865,7 +3874,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="149" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A149" s="3">
         <v>149</v>
       </c>
@@ -3893,7 +3902,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="151" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A151" s="3">
         <v>151</v>
       </c>
@@ -3910,7 +3919,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="152" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:10" ht="29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A152" s="3">
         <v>152</v>
       </c>
@@ -3934,11 +3943,17 @@
       <c r="C153" s="3">
         <v>1</v>
       </c>
+      <c r="D153" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E153" s="7">
+        <v>43243</v>
+      </c>
       <c r="G153" s="3" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="154" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A154" s="3">
         <v>154</v>
       </c>
@@ -3958,8 +3973,41 @@
         <v>271</v>
       </c>
     </row>
+    <row r="155" spans="1:10" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="A155" s="3">
+        <v>155</v>
+      </c>
+      <c r="C155" s="3">
+        <v>1</v>
+      </c>
+      <c r="G155" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="156" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A156" s="3">
+        <v>156</v>
+      </c>
+      <c r="C156" s="3">
+        <v>1</v>
+      </c>
+      <c r="G156" s="3" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="157" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A157" s="3">
+        <v>157</v>
+      </c>
+      <c r="C157" s="3">
+        <v>1</v>
+      </c>
+      <c r="G157" s="3" t="s">
+        <v>274</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:J142">
+  <autoFilter ref="A1:J155">
     <filterColumn colId="3">
       <filters blank="1"/>
     </filterColumn>

</xml_diff>

<commit_message>
Issue #158 large and small preview sizes configurable
</commit_message>
<xml_diff>
--- a/IssuesLog.xlsx
+++ b/IssuesLog.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="49560" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
+    <workbookView xWindow="50720" yWindow="0" windowWidth="32750" windowHeight="14930" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Story" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="276">
   <si>
     <t>#</t>
   </si>
@@ -869,6 +869,9 @@
   </si>
   <si>
     <t>Disk usage as part of server stats</t>
+  </si>
+  <si>
+    <t>Have settings for the large and small preview sizes</t>
   </si>
 </sst>
 </file>
@@ -1357,11 +1360,11 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J157"/>
+  <dimension ref="A1:J158"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G153" sqref="G153"/>
+      <selection pane="bottomLeft" activeCell="D161" sqref="D160:D161"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4004,6 +4007,23 @@
       </c>
       <c r="G157" s="3" t="s">
         <v>274</v>
+      </c>
+    </row>
+    <row r="158" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+      <c r="A158" s="3">
+        <v>158</v>
+      </c>
+      <c r="C158" s="3">
+        <v>1</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E158" s="7">
+        <v>43244</v>
+      </c>
+      <c r="G158" s="3" t="s">
+        <v>275</v>
       </c>
     </row>
   </sheetData>

</xml_diff>